<commit_message>
DOC: Minor text fixes
DOC: Minor text fixes
</commit_message>
<xml_diff>
--- a/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
+++ b/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iwan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iwan\Desktop\School\GitKraken\Asteroids\Documentatie\Persoonlijke Burndowncharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Leerling TestKees" sheetId="1" r:id="rId1"/>
+    <sheet name="Leerling Iwan" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Leerling TestKees'!$AD$1:$AK$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Leerling Iwan'!$AD$1:$AK$11</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1932,14 +1932,19 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1949,14 +1954,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1969,6 +1966,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2378,7 +2378,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$5</c:f>
+              <c:f>'Leerling Iwan'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2440,7 +2440,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$6:$G$16</c:f>
+              <c:f>'Leerling Iwan'!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2492,7 +2492,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$5</c:f>
+              <c:f>'Leerling Iwan'!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2554,7 +2554,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$6:$H$16</c:f>
+              <c:f>'Leerling Iwan'!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2913,7 +2913,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$31</c:f>
+              <c:f>'Leerling Iwan'!$G$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2975,7 +2975,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$32:$G$42</c:f>
+              <c:f>'Leerling Iwan'!$G$32:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3027,7 +3027,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$31</c:f>
+              <c:f>'Leerling Iwan'!$H$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3089,7 +3089,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$32:$H$42</c:f>
+              <c:f>'Leerling Iwan'!$H$32:$H$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3459,7 +3459,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$57</c:f>
+              <c:f>'Leerling Iwan'!$G$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3521,7 +3521,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$58:$G$68</c:f>
+              <c:f>'Leerling Iwan'!$G$58:$G$68</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3573,7 +3573,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$57</c:f>
+              <c:f>'Leerling Iwan'!$H$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3635,7 +3635,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$58:$H$68</c:f>
+              <c:f>'Leerling Iwan'!$H$58:$H$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4005,7 +4005,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$83</c:f>
+              <c:f>'Leerling Iwan'!$G$83</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4067,7 +4067,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$84:$G$94</c:f>
+              <c:f>'Leerling Iwan'!$G$84:$G$94</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4119,7 +4119,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$83</c:f>
+              <c:f>'Leerling Iwan'!$H$83</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4181,7 +4181,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$84:$H$94</c:f>
+              <c:f>'Leerling Iwan'!$H$84:$H$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4538,7 +4538,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$5</c:f>
+              <c:f>'Leerling Iwan'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4561,7 +4561,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$6:$G$16</c:f>
+              <c:f>'Leerling Iwan'!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4613,7 +4613,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$5</c:f>
+              <c:f>'Leerling Iwan'!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4636,7 +4636,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$6:$H$16</c:f>
+              <c:f>'Leerling Iwan'!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4978,7 +4978,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$5</c:f>
+              <c:f>'Leerling Iwan'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5001,7 +5001,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$6:$G$16</c:f>
+              <c:f>'Leerling Iwan'!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5053,7 +5053,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$5</c:f>
+              <c:f>'Leerling Iwan'!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5076,7 +5076,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$6:$H$16</c:f>
+              <c:f>'Leerling Iwan'!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5418,7 +5418,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$5</c:f>
+              <c:f>'Leerling Iwan'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5441,7 +5441,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$6:$G$16</c:f>
+              <c:f>'Leerling Iwan'!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5493,7 +5493,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$5</c:f>
+              <c:f>'Leerling Iwan'!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5516,7 +5516,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$6:$H$16</c:f>
+              <c:f>'Leerling Iwan'!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5858,7 +5858,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$G$5</c:f>
+              <c:f>'Leerling Iwan'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5881,7 +5881,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$G$6:$G$16</c:f>
+              <c:f>'Leerling Iwan'!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5933,7 +5933,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Leerling TestKees'!$H$5</c:f>
+              <c:f>'Leerling Iwan'!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5956,7 +5956,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Leerling TestKees'!$H$6:$H$16</c:f>
+              <c:f>'Leerling Iwan'!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6291,7 +6291,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>('Leerling TestKees'!$H$26,'Leerling TestKees'!$H$52,'Leerling TestKees'!$H$78,'Leerling TestKees'!$H$104)</c:f>
+              <c:f>('Leerling Iwan'!$H$26,'Leerling Iwan'!$H$52,'Leerling Iwan'!$H$78,'Leerling Iwan'!$H$104)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -13541,35 +13541,35 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
       <c r="M1" s="44"/>
       <c r="S1" s="44"/>
     </row>
     <row r="2" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
       <c r="M2" s="44"/>
       <c r="S2" s="44"/>
       <c r="AF2" s="82" t="s">
@@ -13583,10 +13583,10 @@
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="109"/>
+      <c r="H3" s="108"/>
       <c r="I3" s="45"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
@@ -13676,7 +13676,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="111" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -13732,7 +13732,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="34" t="s">
         <v>59</v>
       </c>
@@ -13766,7 +13766,7 @@
       <c r="AI7" s="87"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="111"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="34" t="s">
         <v>60</v>
       </c>
@@ -13827,7 +13827,7 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="34" t="s">
         <v>61</v>
       </c>
@@ -13881,7 +13881,7 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="111"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="34" t="s">
         <v>63</v>
       </c>
@@ -13935,7 +13935,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="111"/>
+      <c r="A11" s="112"/>
       <c r="B11" s="34"/>
       <c r="C11" s="65"/>
       <c r="D11" s="61" t="str">
@@ -13962,7 +13962,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
+      <c r="A12" s="112"/>
       <c r="B12" s="34"/>
       <c r="C12" s="65"/>
       <c r="D12" s="61" t="str">
@@ -13989,7 +13989,7 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
+      <c r="A13" s="112"/>
       <c r="B13" s="34"/>
       <c r="C13" s="65"/>
       <c r="D13" s="61" t="str">
@@ -14016,7 +14016,7 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="111"/>
+      <c r="A14" s="112"/>
       <c r="B14" s="34"/>
       <c r="C14" s="65"/>
       <c r="D14" s="61" t="str">
@@ -14043,7 +14043,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="112"/>
       <c r="B15" s="34"/>
       <c r="C15" s="65"/>
       <c r="D15" s="61" t="str">
@@ -14070,7 +14070,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="34"/>
       <c r="C16" s="65"/>
       <c r="D16" s="61" t="str">
@@ -14097,7 +14097,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
+      <c r="A17" s="112"/>
       <c r="B17" s="34"/>
       <c r="C17" s="65"/>
       <c r="D17" s="61" t="str">
@@ -14111,7 +14111,7 @@
       <c r="I17" s="50"/>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="111"/>
+      <c r="A18" s="112"/>
       <c r="B18" s="34"/>
       <c r="C18" s="65"/>
       <c r="D18" s="61" t="str">
@@ -14125,7 +14125,7 @@
       <c r="I18" s="50"/>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
+      <c r="A19" s="112"/>
       <c r="B19" s="34"/>
       <c r="C19" s="65"/>
       <c r="D19" s="61" t="str">
@@ -14144,47 +14144,47 @@
       </c>
     </row>
     <row r="20" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="111"/>
+      <c r="A20" s="112"/>
       <c r="B20" s="34"/>
       <c r="C20" s="65"/>
       <c r="D20" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E20" s="113" t="str">
+      <c r="E20" s="109" t="str">
         <f>IF(F16&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v># Uren afgetikt aan het eind van de sprint:</v>
       </c>
-      <c r="F20" s="114"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="114"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
       <c r="I20" s="12">
         <f>IF(F16&lt;&gt;"",SUM(F6:F16),"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="111"/>
+      <c r="A21" s="112"/>
       <c r="B21" s="64"/>
       <c r="C21" s="65"/>
       <c r="D21" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E21" s="115" t="str">
+      <c r="E21" s="114" t="str">
         <f>IF(F16&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v>Dit moesten er zijn:</v>
       </c>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
       <c r="I21" s="16">
         <f>IF(F16&lt;&gt;"",AB8,"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
+      <c r="A22" s="112"/>
       <c r="B22" s="64"/>
       <c r="C22" s="65"/>
       <c r="D22" s="61" t="str">
@@ -14201,7 +14201,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111"/>
+      <c r="A23" s="112"/>
       <c r="B23" s="64"/>
       <c r="C23" s="65"/>
       <c r="D23" s="61" t="str">
@@ -14215,7 +14215,7 @@
       <c r="I23" s="50"/>
     </row>
     <row r="24" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
+      <c r="A24" s="112"/>
       <c r="B24" s="64" t="s">
         <v>62</v>
       </c>
@@ -14231,7 +14231,7 @@
       <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="64" t="s">
         <v>57</v>
       </c>
@@ -14247,7 +14247,7 @@
       <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="66" t="s">
         <v>64</v>
       </c>
@@ -14269,20 +14269,20 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
-      <c r="B27" s="107" t="str">
+      <c r="B27" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
       <c r="M27" s="44"/>
       <c r="N27" s="44"/>
       <c r="O27" s="44"/>
@@ -14293,17 +14293,17 @@
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="117"/>
       <c r="M28" s="44"/>
       <c r="N28" s="44"/>
       <c r="O28" s="44"/>
@@ -14319,10 +14319,10 @@
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
-      <c r="G29" s="108" t="s">
+      <c r="G29" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="109"/>
+      <c r="H29" s="108"/>
       <c r="I29" s="45"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
@@ -14392,7 +14392,7 @@
       <c r="S31" s="44"/>
     </row>
     <row r="32" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="110" t="s">
+      <c r="A32" s="111" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="33"/>
@@ -14421,7 +14421,7 @@
       </c>
     </row>
     <row r="33" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="34"/>
       <c r="C33" s="104"/>
       <c r="D33" s="98"/>
@@ -14443,7 +14443,7 @@
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="111"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="64"/>
       <c r="C34" s="68"/>
       <c r="D34" s="61" t="str">
@@ -14475,7 +14475,7 @@
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
+      <c r="A35" s="112"/>
       <c r="B35" s="64"/>
       <c r="C35" s="65"/>
       <c r="D35" s="61" t="str">
@@ -14500,7 +14500,7 @@
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="111"/>
+      <c r="A36" s="112"/>
       <c r="B36" s="64"/>
       <c r="C36" s="65"/>
       <c r="D36" s="61" t="str">
@@ -14525,7 +14525,7 @@
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
+      <c r="A37" s="112"/>
       <c r="B37" s="64"/>
       <c r="C37" s="65"/>
       <c r="D37" s="61" t="str">
@@ -14550,7 +14550,7 @@
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="111"/>
+      <c r="A38" s="112"/>
       <c r="B38" s="64"/>
       <c r="C38" s="65"/>
       <c r="D38" s="61" t="str">
@@ -14575,7 +14575,7 @@
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
+      <c r="A39" s="112"/>
       <c r="B39" s="64"/>
       <c r="C39" s="65"/>
       <c r="D39" s="61" t="str">
@@ -14600,7 +14600,7 @@
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="111"/>
+      <c r="A40" s="112"/>
       <c r="B40" s="64"/>
       <c r="C40" s="65"/>
       <c r="D40" s="61" t="str">
@@ -14625,7 +14625,7 @@
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="64"/>
       <c r="C41" s="65"/>
       <c r="D41" s="61" t="str">
@@ -14650,7 +14650,7 @@
       </c>
     </row>
     <row r="42" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="111"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="64"/>
       <c r="C42" s="65"/>
       <c r="D42" s="61" t="str">
@@ -14675,7 +14675,7 @@
       </c>
     </row>
     <row r="43" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
+      <c r="A43" s="112"/>
       <c r="B43" s="64"/>
       <c r="C43" s="65"/>
       <c r="D43" s="61" t="str">
@@ -14689,7 +14689,7 @@
       <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="111"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="64"/>
       <c r="C44" s="65"/>
       <c r="D44" s="61" t="str">
@@ -14703,7 +14703,7 @@
       <c r="I44" s="50"/>
     </row>
     <row r="45" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
+      <c r="A45" s="112"/>
       <c r="B45" s="64"/>
       <c r="C45" s="65"/>
       <c r="D45" s="61" t="str">
@@ -14722,47 +14722,47 @@
       </c>
     </row>
     <row r="46" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="64"/>
       <c r="C46" s="65"/>
       <c r="D46" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E46" s="113" t="str">
+      <c r="E46" s="109" t="str">
         <f>IF(F42&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F46" s="114"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="114"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
       <c r="I46" s="12" t="str">
         <f>IF(F42&lt;&gt;"",SUM(F32:F42),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="111"/>
+      <c r="A47" s="112"/>
       <c r="B47" s="64"/>
       <c r="C47" s="65"/>
       <c r="D47" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E47" s="115" t="str">
+      <c r="E47" s="114" t="str">
         <f>IF(F42&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F47" s="116"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="116"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
       <c r="I47" s="16" t="str">
         <f>IF(F42&lt;&gt;"",AB34,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="112"/>
       <c r="B48" s="34"/>
       <c r="C48" s="69"/>
       <c r="D48" s="61" t="str">
@@ -14779,7 +14779,7 @@
       </c>
     </row>
     <row r="49" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="112"/>
       <c r="B49" s="34"/>
       <c r="C49" s="65"/>
       <c r="D49" s="61" t="str">
@@ -14793,7 +14793,7 @@
       <c r="I49" s="50"/>
     </row>
     <row r="50" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
+      <c r="A50" s="112"/>
       <c r="B50" s="34"/>
       <c r="C50" s="65"/>
       <c r="D50" s="61" t="str">
@@ -14807,7 +14807,7 @@
       <c r="I50" s="50"/>
     </row>
     <row r="51" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="111"/>
+      <c r="A51" s="112"/>
       <c r="B51" s="34"/>
       <c r="C51" s="65"/>
       <c r="D51" s="61" t="str">
@@ -14821,7 +14821,7 @@
       <c r="I51" s="50"/>
     </row>
     <row r="52" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="112"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="70"/>
       <c r="C52" s="67"/>
       <c r="D52" s="62" t="str">
@@ -14841,20 +14841,20 @@
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
-      <c r="B53" s="107" t="str">
+      <c r="B53" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C53" s="107"/>
-      <c r="D53" s="107"/>
-      <c r="E53" s="107"/>
-      <c r="F53" s="107"/>
-      <c r="G53" s="107"/>
-      <c r="H53" s="107"/>
-      <c r="I53" s="107"/>
-      <c r="J53" s="107"/>
-      <c r="K53" s="107"/>
-      <c r="L53" s="107"/>
+      <c r="C53" s="117"/>
+      <c r="D53" s="117"/>
+      <c r="E53" s="117"/>
+      <c r="F53" s="117"/>
+      <c r="G53" s="117"/>
+      <c r="H53" s="117"/>
+      <c r="I53" s="117"/>
+      <c r="J53" s="117"/>
+      <c r="K53" s="117"/>
+      <c r="L53" s="117"/>
       <c r="M53" s="44"/>
       <c r="N53" s="44"/>
       <c r="O53" s="44"/>
@@ -14865,17 +14865,17 @@
     </row>
     <row r="54" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="107"/>
-      <c r="F54" s="107"/>
-      <c r="G54" s="107"/>
-      <c r="H54" s="107"/>
-      <c r="I54" s="107"/>
-      <c r="J54" s="107"/>
-      <c r="K54" s="107"/>
-      <c r="L54" s="107"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="117"/>
+      <c r="D54" s="117"/>
+      <c r="E54" s="117"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="117"/>
+      <c r="H54" s="117"/>
+      <c r="I54" s="117"/>
+      <c r="J54" s="117"/>
+      <c r="K54" s="117"/>
+      <c r="L54" s="117"/>
       <c r="M54" s="44"/>
       <c r="N54" s="44"/>
       <c r="O54" s="44"/>
@@ -14891,10 +14891,10 @@
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
       <c r="F55" s="44"/>
-      <c r="G55" s="108" t="s">
+      <c r="G55" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H55" s="109"/>
+      <c r="H55" s="108"/>
       <c r="I55" s="45"/>
       <c r="J55" s="44"/>
       <c r="K55" s="44"/>
@@ -14964,7 +14964,7 @@
       <c r="S57" s="44"/>
     </row>
     <row r="58" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="110" t="s">
+      <c r="A58" s="111" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="33"/>
@@ -14994,7 +14994,7 @@
       <c r="J58" s="106"/>
     </row>
     <row r="59" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="111"/>
+      <c r="A59" s="112"/>
       <c r="B59" s="34"/>
       <c r="C59" s="104"/>
       <c r="D59" s="98"/>
@@ -15017,7 +15017,7 @@
       <c r="J59" s="106"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A60" s="111"/>
+      <c r="A60" s="112"/>
       <c r="B60" s="64"/>
       <c r="C60" s="68"/>
       <c r="D60" s="61" t="str">
@@ -15050,7 +15050,7 @@
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A61" s="111"/>
+      <c r="A61" s="112"/>
       <c r="B61" s="64"/>
       <c r="C61" s="65"/>
       <c r="D61" s="61" t="str">
@@ -15076,7 +15076,7 @@
       <c r="J61" s="106"/>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A62" s="111"/>
+      <c r="A62" s="112"/>
       <c r="B62" s="64"/>
       <c r="C62" s="65"/>
       <c r="D62" s="61" t="str">
@@ -15102,7 +15102,7 @@
       <c r="J62" s="106"/>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A63" s="111"/>
+      <c r="A63" s="112"/>
       <c r="B63" s="64"/>
       <c r="C63" s="65"/>
       <c r="D63" s="61" t="str">
@@ -15128,7 +15128,7 @@
       <c r="J63" s="106"/>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A64" s="111"/>
+      <c r="A64" s="112"/>
       <c r="B64" s="64"/>
       <c r="C64" s="65"/>
       <c r="D64" s="61" t="str">
@@ -15154,7 +15154,7 @@
       <c r="J64" s="106"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="111"/>
+      <c r="A65" s="112"/>
       <c r="B65" s="64"/>
       <c r="C65" s="65"/>
       <c r="D65" s="61" t="str">
@@ -15180,7 +15180,7 @@
       <c r="J65" s="106"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="111"/>
+      <c r="A66" s="112"/>
       <c r="B66" s="64"/>
       <c r="C66" s="65"/>
       <c r="D66" s="61" t="str">
@@ -15206,7 +15206,7 @@
       <c r="J66" s="106"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="111"/>
+      <c r="A67" s="112"/>
       <c r="B67" s="64"/>
       <c r="C67" s="65"/>
       <c r="D67" s="61" t="str">
@@ -15232,7 +15232,7 @@
       <c r="J67" s="106"/>
     </row>
     <row r="68" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="111"/>
+      <c r="A68" s="112"/>
       <c r="B68" s="64"/>
       <c r="C68" s="65"/>
       <c r="D68" s="61" t="str">
@@ -15258,7 +15258,7 @@
       <c r="J68" s="106"/>
     </row>
     <row r="69" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="111"/>
+      <c r="A69" s="112"/>
       <c r="B69" s="64"/>
       <c r="C69" s="65"/>
       <c r="D69" s="61" t="str">
@@ -15272,7 +15272,7 @@
       <c r="I69" s="50"/>
     </row>
     <row r="70" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="111"/>
+      <c r="A70" s="112"/>
       <c r="B70" s="64"/>
       <c r="C70" s="65"/>
       <c r="D70" s="61" t="str">
@@ -15286,7 +15286,7 @@
       <c r="I70" s="50"/>
     </row>
     <row r="71" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="111"/>
+      <c r="A71" s="112"/>
       <c r="B71" s="64"/>
       <c r="C71" s="65"/>
       <c r="D71" s="61" t="str">
@@ -15305,47 +15305,47 @@
       </c>
     </row>
     <row r="72" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="111"/>
+      <c r="A72" s="112"/>
       <c r="B72" s="64"/>
       <c r="C72" s="65"/>
       <c r="D72" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E72" s="113" t="str">
+      <c r="E72" s="109" t="str">
         <f>IF(F68&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F72" s="114"/>
-      <c r="G72" s="114"/>
-      <c r="H72" s="114"/>
+      <c r="F72" s="110"/>
+      <c r="G72" s="110"/>
+      <c r="H72" s="110"/>
       <c r="I72" s="12" t="str">
         <f>IF(F68&lt;&gt;"",SUM(F58:F68),"")</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="111"/>
+      <c r="A73" s="112"/>
       <c r="B73" s="64"/>
       <c r="C73" s="65"/>
       <c r="D73" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E73" s="115" t="str">
+      <c r="E73" s="114" t="str">
         <f>IF(F68&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F73" s="116"/>
-      <c r="G73" s="116"/>
-      <c r="H73" s="116"/>
+      <c r="F73" s="115"/>
+      <c r="G73" s="115"/>
+      <c r="H73" s="115"/>
       <c r="I73" s="16" t="str">
         <f>IF(F68&lt;&gt;"",AB60,"")</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
+      <c r="A74" s="112"/>
       <c r="B74" s="64"/>
       <c r="C74" s="65"/>
       <c r="D74" s="61" t="str">
@@ -15362,7 +15362,7 @@
       </c>
     </row>
     <row r="75" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
+      <c r="A75" s="112"/>
       <c r="B75" s="64"/>
       <c r="C75" s="65"/>
       <c r="D75" s="61" t="str">
@@ -15376,7 +15376,7 @@
       <c r="I75" s="50"/>
     </row>
     <row r="76" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="111"/>
+      <c r="A76" s="112"/>
       <c r="B76" s="64"/>
       <c r="C76" s="65"/>
       <c r="D76" s="61" t="str">
@@ -15390,7 +15390,7 @@
       <c r="I76" s="50"/>
     </row>
     <row r="77" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="111"/>
+      <c r="A77" s="112"/>
       <c r="B77" s="64"/>
       <c r="C77" s="65"/>
       <c r="D77" s="61" t="str">
@@ -15404,7 +15404,7 @@
       <c r="I77" s="50"/>
     </row>
     <row r="78" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="112"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="66"/>
       <c r="C78" s="67"/>
       <c r="D78" s="62" t="str">
@@ -15424,20 +15424,20 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
-      <c r="B79" s="107" t="str">
+      <c r="B79" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C79" s="107"/>
-      <c r="D79" s="107"/>
-      <c r="E79" s="107"/>
-      <c r="F79" s="107"/>
-      <c r="G79" s="107"/>
-      <c r="H79" s="107"/>
-      <c r="I79" s="107"/>
-      <c r="J79" s="107"/>
-      <c r="K79" s="107"/>
-      <c r="L79" s="107"/>
+      <c r="C79" s="117"/>
+      <c r="D79" s="117"/>
+      <c r="E79" s="117"/>
+      <c r="F79" s="117"/>
+      <c r="G79" s="117"/>
+      <c r="H79" s="117"/>
+      <c r="I79" s="117"/>
+      <c r="J79" s="117"/>
+      <c r="K79" s="117"/>
+      <c r="L79" s="117"/>
       <c r="M79" s="44"/>
       <c r="N79" s="44"/>
       <c r="O79" s="44"/>
@@ -15448,17 +15448,17 @@
     </row>
     <row r="80" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="43"/>
-      <c r="B80" s="107"/>
-      <c r="C80" s="107"/>
-      <c r="D80" s="107"/>
-      <c r="E80" s="107"/>
-      <c r="F80" s="107"/>
-      <c r="G80" s="107"/>
-      <c r="H80" s="107"/>
-      <c r="I80" s="107"/>
-      <c r="J80" s="107"/>
-      <c r="K80" s="107"/>
-      <c r="L80" s="107"/>
+      <c r="B80" s="117"/>
+      <c r="C80" s="117"/>
+      <c r="D80" s="117"/>
+      <c r="E80" s="117"/>
+      <c r="F80" s="117"/>
+      <c r="G80" s="117"/>
+      <c r="H80" s="117"/>
+      <c r="I80" s="117"/>
+      <c r="J80" s="117"/>
+      <c r="K80" s="117"/>
+      <c r="L80" s="117"/>
       <c r="M80" s="44"/>
       <c r="N80" s="44"/>
       <c r="O80" s="44"/>
@@ -15474,10 +15474,10 @@
       <c r="D81" s="44"/>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
-      <c r="G81" s="108" t="s">
+      <c r="G81" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H81" s="109"/>
+      <c r="H81" s="108"/>
       <c r="I81" s="45"/>
       <c r="J81" s="44"/>
       <c r="K81" s="44"/>
@@ -15547,7 +15547,7 @@
       <c r="S83" s="44"/>
     </row>
     <row r="84" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="110" t="s">
+      <c r="A84" s="111" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="33"/>
@@ -15576,7 +15576,7 @@
       </c>
     </row>
     <row r="85" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
+      <c r="A85" s="112"/>
       <c r="B85" s="34"/>
       <c r="C85" s="69"/>
       <c r="D85" s="98"/>
@@ -15598,7 +15598,7 @@
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A86" s="111"/>
+      <c r="A86" s="112"/>
       <c r="B86" s="64"/>
       <c r="C86" s="65"/>
       <c r="D86" s="61" t="str">
@@ -15630,7 +15630,7 @@
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A87" s="111"/>
+      <c r="A87" s="112"/>
       <c r="B87" s="64"/>
       <c r="C87" s="65"/>
       <c r="D87" s="61" t="str">
@@ -15655,7 +15655,7 @@
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A88" s="111"/>
+      <c r="A88" s="112"/>
       <c r="B88" s="64"/>
       <c r="C88" s="65"/>
       <c r="D88" s="61" t="str">
@@ -15680,7 +15680,7 @@
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A89" s="111"/>
+      <c r="A89" s="112"/>
       <c r="B89" s="64"/>
       <c r="C89" s="65"/>
       <c r="D89" s="61" t="str">
@@ -15705,7 +15705,7 @@
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A90" s="111"/>
+      <c r="A90" s="112"/>
       <c r="B90" s="64"/>
       <c r="C90" s="65"/>
       <c r="D90" s="61" t="str">
@@ -15730,7 +15730,7 @@
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="111"/>
+      <c r="A91" s="112"/>
       <c r="B91" s="64"/>
       <c r="C91" s="65"/>
       <c r="D91" s="61" t="str">
@@ -15755,7 +15755,7 @@
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A92" s="111"/>
+      <c r="A92" s="112"/>
       <c r="B92" s="64"/>
       <c r="C92" s="65"/>
       <c r="D92" s="61" t="str">
@@ -15780,7 +15780,7 @@
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A93" s="111"/>
+      <c r="A93" s="112"/>
       <c r="B93" s="64"/>
       <c r="C93" s="65"/>
       <c r="D93" s="61" t="str">
@@ -15805,7 +15805,7 @@
       </c>
     </row>
     <row r="94" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="111"/>
+      <c r="A94" s="112"/>
       <c r="B94" s="64"/>
       <c r="C94" s="65"/>
       <c r="D94" s="61" t="str">
@@ -15830,7 +15830,7 @@
       </c>
     </row>
     <row r="95" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="111"/>
+      <c r="A95" s="112"/>
       <c r="B95" s="64"/>
       <c r="C95" s="65"/>
       <c r="D95" s="61" t="str">
@@ -15844,7 +15844,7 @@
       <c r="I95" s="50"/>
     </row>
     <row r="96" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="111"/>
+      <c r="A96" s="112"/>
       <c r="B96" s="64"/>
       <c r="C96" s="65"/>
       <c r="D96" s="61" t="str">
@@ -15858,7 +15858,7 @@
       <c r="I96" s="50"/>
     </row>
     <row r="97" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="111"/>
+      <c r="A97" s="112"/>
       <c r="B97" s="64"/>
       <c r="C97" s="65"/>
       <c r="D97" s="61" t="str">
@@ -15877,47 +15877,47 @@
       </c>
     </row>
     <row r="98" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="111"/>
+      <c r="A98" s="112"/>
       <c r="B98" s="64"/>
       <c r="C98" s="65"/>
       <c r="D98" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E98" s="113" t="str">
+      <c r="E98" s="109" t="str">
         <f>IF(F94&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F98" s="114"/>
-      <c r="G98" s="114"/>
-      <c r="H98" s="114"/>
+      <c r="F98" s="110"/>
+      <c r="G98" s="110"/>
+      <c r="H98" s="110"/>
       <c r="I98" s="12" t="str">
         <f>IF(F94&lt;&gt;"",SUM(F84:F94),"")</f>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="111"/>
+      <c r="A99" s="112"/>
       <c r="B99" s="64"/>
       <c r="C99" s="65"/>
       <c r="D99" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E99" s="115" t="str">
+      <c r="E99" s="114" t="str">
         <f>IF(F94&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116"/>
+      <c r="F99" s="115"/>
+      <c r="G99" s="115"/>
+      <c r="H99" s="115"/>
       <c r="I99" s="16" t="str">
         <f>IF(F94&lt;&gt;"",AB86,"")</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="111"/>
+      <c r="A100" s="112"/>
       <c r="B100" s="64"/>
       <c r="C100" s="65"/>
       <c r="D100" s="61" t="str">
@@ -15934,7 +15934,7 @@
       </c>
     </row>
     <row r="101" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="111"/>
+      <c r="A101" s="112"/>
       <c r="B101" s="64"/>
       <c r="C101" s="65"/>
       <c r="D101" s="61" t="str">
@@ -15948,7 +15948,7 @@
       <c r="I101" s="50"/>
     </row>
     <row r="102" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="111"/>
+      <c r="A102" s="112"/>
       <c r="B102" s="64"/>
       <c r="C102" s="65"/>
       <c r="D102" s="61" t="str">
@@ -15962,7 +15962,7 @@
       <c r="I102" s="50"/>
     </row>
     <row r="103" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="111"/>
+      <c r="A103" s="112"/>
       <c r="B103" s="64"/>
       <c r="C103" s="65"/>
       <c r="D103" s="61" t="str">
@@ -15976,7 +15976,7 @@
       <c r="I103" s="50"/>
     </row>
     <row r="104" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="112"/>
+      <c r="A104" s="113"/>
       <c r="B104" s="66"/>
       <c r="C104" s="67"/>
       <c r="D104" s="62" t="str">
@@ -15996,19 +15996,19 @@
     </row>
     <row r="105" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="43"/>
-      <c r="B105" s="107" t="s">
+      <c r="B105" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="107"/>
-      <c r="D105" s="107"/>
-      <c r="E105" s="107"/>
-      <c r="F105" s="107"/>
-      <c r="G105" s="107"/>
-      <c r="H105" s="107"/>
-      <c r="I105" s="107"/>
-      <c r="J105" s="107"/>
-      <c r="K105" s="107"/>
-      <c r="L105" s="107"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
       <c r="M105" s="44"/>
       <c r="N105" s="44"/>
       <c r="O105" s="44"/>
@@ -16019,17 +16019,17 @@
     </row>
     <row r="106" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="43"/>
-      <c r="B106" s="107"/>
-      <c r="C106" s="107"/>
-      <c r="D106" s="107"/>
-      <c r="E106" s="107"/>
-      <c r="F106" s="107"/>
-      <c r="G106" s="107"/>
-      <c r="H106" s="107"/>
-      <c r="I106" s="107"/>
-      <c r="J106" s="107"/>
-      <c r="K106" s="107"/>
-      <c r="L106" s="107"/>
+      <c r="B106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
       <c r="M106" s="44"/>
       <c r="N106" s="44"/>
       <c r="O106" s="44"/>
@@ -16045,10 +16045,10 @@
       <c r="D107" s="44"/>
       <c r="E107" s="44"/>
       <c r="F107" s="44"/>
-      <c r="G107" s="108" t="s">
+      <c r="G107" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H107" s="109"/>
+      <c r="H107" s="108"/>
       <c r="I107" s="45"/>
       <c r="J107" s="44"/>
       <c r="K107" s="44"/>
@@ -16118,7 +16118,7 @@
       <c r="S109" s="44"/>
     </row>
     <row r="110" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="110" t="s">
+      <c r="A110" s="111" t="s">
         <v>26</v>
       </c>
       <c r="B110" s="56"/>
@@ -16148,7 +16148,7 @@
       </c>
     </row>
     <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="111"/>
+      <c r="A111" s="112"/>
       <c r="B111" s="56"/>
       <c r="C111" s="32"/>
       <c r="D111" s="10" t="str">
@@ -16180,7 +16180,7 @@
       </c>
     </row>
     <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="111"/>
+      <c r="A112" s="112"/>
       <c r="B112" s="56"/>
       <c r="C112" s="32"/>
       <c r="D112" s="10" t="str">
@@ -16202,7 +16202,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="111"/>
+      <c r="A113" s="112"/>
       <c r="B113" s="56"/>
       <c r="C113" s="32"/>
       <c r="D113" s="10" t="str">
@@ -16224,7 +16224,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="111"/>
+      <c r="A114" s="112"/>
       <c r="B114" s="56"/>
       <c r="C114" s="32"/>
       <c r="D114" s="10" t="str">
@@ -16246,7 +16246,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="111"/>
+      <c r="A115" s="112"/>
       <c r="B115" s="56"/>
       <c r="C115" s="32"/>
       <c r="D115" s="10" t="str">
@@ -16268,7 +16268,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="111"/>
+      <c r="A116" s="112"/>
       <c r="B116" s="56"/>
       <c r="C116" s="32"/>
       <c r="D116" s="10" t="str">
@@ -16290,7 +16290,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="111"/>
+      <c r="A117" s="112"/>
       <c r="B117" s="56"/>
       <c r="C117" s="32"/>
       <c r="D117" s="10" t="str">
@@ -16312,7 +16312,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="111"/>
+      <c r="A118" s="112"/>
       <c r="B118" s="56"/>
       <c r="C118" s="32"/>
       <c r="D118" s="10" t="str">
@@ -16334,7 +16334,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="111"/>
+      <c r="A119" s="112"/>
       <c r="B119" s="56"/>
       <c r="C119" s="32"/>
       <c r="D119" s="10" t="str">
@@ -16354,7 +16354,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="111"/>
+      <c r="A120" s="112"/>
       <c r="B120" s="56"/>
       <c r="C120" s="32"/>
       <c r="D120" s="10" t="str">
@@ -16368,7 +16368,7 @@
       <c r="I120" s="49"/>
     </row>
     <row r="121" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="111"/>
+      <c r="A121" s="112"/>
       <c r="B121" s="56"/>
       <c r="C121" s="32"/>
       <c r="D121" s="10" t="str">
@@ -16382,7 +16382,7 @@
       <c r="I121" s="50"/>
     </row>
     <row r="122" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="111"/>
+      <c r="A122" s="112"/>
       <c r="B122" s="56"/>
       <c r="C122" s="32"/>
       <c r="D122" s="10" t="str">
@@ -16401,47 +16401,47 @@
       </c>
     </row>
     <row r="123" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="111"/>
+      <c r="A123" s="112"/>
       <c r="B123" s="56"/>
       <c r="C123" s="32"/>
       <c r="D123" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E123" s="113" t="str">
+      <c r="E123" s="109" t="str">
         <f>IF(F119&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F123" s="114"/>
-      <c r="G123" s="114"/>
-      <c r="H123" s="114"/>
+      <c r="F123" s="110"/>
+      <c r="G123" s="110"/>
+      <c r="H123" s="110"/>
       <c r="I123" s="12" t="str">
         <f>IF(F119&lt;&gt;"",SUM(F110:F119),"")</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="111"/>
+      <c r="A124" s="112"/>
       <c r="B124" s="56"/>
       <c r="C124" s="32"/>
       <c r="D124" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E124" s="115" t="str">
+      <c r="E124" s="114" t="str">
         <f>IF(F119&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F124" s="116"/>
-      <c r="G124" s="116"/>
-      <c r="H124" s="116"/>
+      <c r="F124" s="115"/>
+      <c r="G124" s="115"/>
+      <c r="H124" s="115"/>
       <c r="I124" s="16" t="str">
         <f>IF(F119&lt;&gt;"",AB111,"")</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="111"/>
+      <c r="A125" s="112"/>
       <c r="B125" s="34"/>
       <c r="C125" s="58"/>
       <c r="D125" s="10" t="str">
@@ -16458,7 +16458,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="111"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="34"/>
       <c r="C126" s="32"/>
       <c r="D126" s="10" t="str">
@@ -16472,7 +16472,7 @@
       <c r="I126" s="50"/>
     </row>
     <row r="127" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="111"/>
+      <c r="A127" s="112"/>
       <c r="B127" s="34"/>
       <c r="C127" s="32"/>
       <c r="D127" s="10" t="str">
@@ -16486,7 +16486,7 @@
       <c r="I127" s="50"/>
     </row>
     <row r="128" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="111"/>
+      <c r="A128" s="112"/>
       <c r="B128" s="34"/>
       <c r="C128" s="32"/>
       <c r="D128" s="10" t="str">
@@ -16500,7 +16500,7 @@
       <c r="I128" s="50"/>
     </row>
     <row r="129" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="112"/>
+      <c r="A129" s="113"/>
       <c r="B129" s="34"/>
       <c r="C129" s="32"/>
       <c r="D129" s="11" t="str">
@@ -16520,19 +16520,19 @@
     </row>
     <row r="130" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="43"/>
-      <c r="B130" s="107" t="s">
+      <c r="B130" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C130" s="107"/>
-      <c r="D130" s="107"/>
-      <c r="E130" s="107"/>
-      <c r="F130" s="107"/>
-      <c r="G130" s="107"/>
-      <c r="H130" s="107"/>
-      <c r="I130" s="107"/>
-      <c r="J130" s="107"/>
-      <c r="K130" s="107"/>
-      <c r="L130" s="107"/>
+      <c r="C130" s="117"/>
+      <c r="D130" s="117"/>
+      <c r="E130" s="117"/>
+      <c r="F130" s="117"/>
+      <c r="G130" s="117"/>
+      <c r="H130" s="117"/>
+      <c r="I130" s="117"/>
+      <c r="J130" s="117"/>
+      <c r="K130" s="117"/>
+      <c r="L130" s="117"/>
       <c r="M130" s="44"/>
       <c r="N130" s="44"/>
       <c r="O130" s="44"/>
@@ -16543,17 +16543,17 @@
     </row>
     <row r="131" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="43"/>
-      <c r="B131" s="107"/>
-      <c r="C131" s="107"/>
-      <c r="D131" s="107"/>
-      <c r="E131" s="107"/>
-      <c r="F131" s="107"/>
-      <c r="G131" s="107"/>
-      <c r="H131" s="107"/>
-      <c r="I131" s="107"/>
-      <c r="J131" s="107"/>
-      <c r="K131" s="107"/>
-      <c r="L131" s="107"/>
+      <c r="B131" s="117"/>
+      <c r="C131" s="117"/>
+      <c r="D131" s="117"/>
+      <c r="E131" s="117"/>
+      <c r="F131" s="117"/>
+      <c r="G131" s="117"/>
+      <c r="H131" s="117"/>
+      <c r="I131" s="117"/>
+      <c r="J131" s="117"/>
+      <c r="K131" s="117"/>
+      <c r="L131" s="117"/>
       <c r="M131" s="44"/>
       <c r="N131" s="44"/>
       <c r="O131" s="44"/>
@@ -16569,10 +16569,10 @@
       <c r="D132" s="44"/>
       <c r="E132" s="44"/>
       <c r="F132" s="44"/>
-      <c r="G132" s="108" t="s">
+      <c r="G132" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H132" s="109"/>
+      <c r="H132" s="108"/>
       <c r="I132" s="45"/>
       <c r="J132" s="44"/>
       <c r="K132" s="44"/>
@@ -16642,7 +16642,7 @@
       <c r="S134" s="44"/>
     </row>
     <row r="135" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="110" t="s">
+      <c r="A135" s="111" t="s">
         <v>27</v>
       </c>
       <c r="B135" s="57"/>
@@ -16672,7 +16672,7 @@
       </c>
     </row>
     <row r="136" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="111"/>
+      <c r="A136" s="112"/>
       <c r="B136" s="56"/>
       <c r="C136" s="32"/>
       <c r="D136" s="10" t="str">
@@ -16704,7 +16704,7 @@
       </c>
     </row>
     <row r="137" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="111"/>
+      <c r="A137" s="112"/>
       <c r="B137" s="56"/>
       <c r="C137" s="32"/>
       <c r="D137" s="10" t="str">
@@ -16726,7 +16726,7 @@
       </c>
     </row>
     <row r="138" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="111"/>
+      <c r="A138" s="112"/>
       <c r="B138" s="56"/>
       <c r="C138" s="32"/>
       <c r="D138" s="10" t="str">
@@ -16748,7 +16748,7 @@
       </c>
     </row>
     <row r="139" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="111"/>
+      <c r="A139" s="112"/>
       <c r="B139" s="56"/>
       <c r="C139" s="32"/>
       <c r="D139" s="10" t="str">
@@ -16770,7 +16770,7 @@
       </c>
     </row>
     <row r="140" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="111"/>
+      <c r="A140" s="112"/>
       <c r="B140" s="56"/>
       <c r="C140" s="32"/>
       <c r="D140" s="10" t="str">
@@ -16792,7 +16792,7 @@
       </c>
     </row>
     <row r="141" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="111"/>
+      <c r="A141" s="112"/>
       <c r="B141" s="56"/>
       <c r="C141" s="32"/>
       <c r="D141" s="10" t="str">
@@ -16814,7 +16814,7 @@
       </c>
     </row>
     <row r="142" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="111"/>
+      <c r="A142" s="112"/>
       <c r="B142" s="56"/>
       <c r="C142" s="32"/>
       <c r="D142" s="10" t="str">
@@ -16836,7 +16836,7 @@
       </c>
     </row>
     <row r="143" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="111"/>
+      <c r="A143" s="112"/>
       <c r="B143" s="56"/>
       <c r="C143" s="32"/>
       <c r="D143" s="10" t="str">
@@ -16858,7 +16858,7 @@
       </c>
     </row>
     <row r="144" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="111"/>
+      <c r="A144" s="112"/>
       <c r="B144" s="56"/>
       <c r="C144" s="32"/>
       <c r="D144" s="10" t="str">
@@ -16878,7 +16878,7 @@
       </c>
     </row>
     <row r="145" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="111"/>
+      <c r="A145" s="112"/>
       <c r="B145" s="56"/>
       <c r="C145" s="32"/>
       <c r="D145" s="10" t="str">
@@ -16892,7 +16892,7 @@
       <c r="I145" s="49"/>
     </row>
     <row r="146" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="111"/>
+      <c r="A146" s="112"/>
       <c r="B146" s="56"/>
       <c r="C146" s="32"/>
       <c r="D146" s="10" t="str">
@@ -16906,7 +16906,7 @@
       <c r="I146" s="50"/>
     </row>
     <row r="147" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="111"/>
+      <c r="A147" s="112"/>
       <c r="B147" s="56"/>
       <c r="C147" s="32"/>
       <c r="D147" s="10" t="str">
@@ -16925,47 +16925,47 @@
       </c>
     </row>
     <row r="148" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="111"/>
+      <c r="A148" s="112"/>
       <c r="B148" s="56"/>
       <c r="C148" s="32"/>
       <c r="D148" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E148" s="113" t="str">
+      <c r="E148" s="109" t="str">
         <f>IF(F144&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F148" s="114"/>
-      <c r="G148" s="114"/>
-      <c r="H148" s="114"/>
+      <c r="F148" s="110"/>
+      <c r="G148" s="110"/>
+      <c r="H148" s="110"/>
       <c r="I148" s="12" t="str">
         <f>IF(F144&lt;&gt;"",SUM(F135:F144),"")</f>
         <v/>
       </c>
     </row>
     <row r="149" spans="1:27" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="111"/>
+      <c r="A149" s="112"/>
       <c r="B149" s="56"/>
       <c r="C149" s="32"/>
       <c r="D149" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E149" s="115" t="str">
+      <c r="E149" s="114" t="str">
         <f>IF(F144&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F149" s="116"/>
-      <c r="G149" s="116"/>
-      <c r="H149" s="116"/>
+      <c r="F149" s="115"/>
+      <c r="G149" s="115"/>
+      <c r="H149" s="115"/>
       <c r="I149" s="16" t="str">
         <f>IF(F144&lt;&gt;"",AB136,"")</f>
         <v/>
       </c>
     </row>
     <row r="150" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="111"/>
+      <c r="A150" s="112"/>
       <c r="B150" s="56"/>
       <c r="C150" s="32"/>
       <c r="D150" s="10" t="str">
@@ -16982,7 +16982,7 @@
       </c>
     </row>
     <row r="151" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="111"/>
+      <c r="A151" s="112"/>
       <c r="B151" s="34"/>
       <c r="C151" s="32"/>
       <c r="D151" s="10" t="str">
@@ -16996,7 +16996,7 @@
       <c r="I151" s="50"/>
     </row>
     <row r="152" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="111"/>
+      <c r="A152" s="112"/>
       <c r="B152" s="34"/>
       <c r="C152" s="32"/>
       <c r="D152" s="10" t="str">
@@ -17010,7 +17010,7 @@
       <c r="I152" s="50"/>
     </row>
     <row r="153" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="111"/>
+      <c r="A153" s="112"/>
       <c r="B153" s="34"/>
       <c r="C153" s="32"/>
       <c r="D153" s="10" t="str">
@@ -17024,7 +17024,7 @@
       <c r="I153" s="50"/>
     </row>
     <row r="154" spans="1:27" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="112"/>
+      <c r="A154" s="113"/>
       <c r="B154" s="34"/>
       <c r="C154" s="32"/>
       <c r="D154" s="11" t="str">
@@ -17044,19 +17044,19 @@
     </row>
     <row r="155" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="43"/>
-      <c r="B155" s="107" t="s">
+      <c r="B155" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C155" s="107"/>
-      <c r="D155" s="107"/>
-      <c r="E155" s="107"/>
-      <c r="F155" s="107"/>
-      <c r="G155" s="107"/>
-      <c r="H155" s="107"/>
-      <c r="I155" s="107"/>
-      <c r="J155" s="107"/>
-      <c r="K155" s="107"/>
-      <c r="L155" s="107"/>
+      <c r="C155" s="117"/>
+      <c r="D155" s="117"/>
+      <c r="E155" s="117"/>
+      <c r="F155" s="117"/>
+      <c r="G155" s="117"/>
+      <c r="H155" s="117"/>
+      <c r="I155" s="117"/>
+      <c r="J155" s="117"/>
+      <c r="K155" s="117"/>
+      <c r="L155" s="117"/>
       <c r="M155" s="44"/>
       <c r="N155" s="44"/>
       <c r="O155" s="44"/>
@@ -17067,17 +17067,17 @@
     </row>
     <row r="156" spans="1:27" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="43"/>
-      <c r="B156" s="107"/>
-      <c r="C156" s="107"/>
-      <c r="D156" s="107"/>
-      <c r="E156" s="107"/>
-      <c r="F156" s="107"/>
-      <c r="G156" s="107"/>
-      <c r="H156" s="107"/>
-      <c r="I156" s="107"/>
-      <c r="J156" s="107"/>
-      <c r="K156" s="107"/>
-      <c r="L156" s="107"/>
+      <c r="B156" s="117"/>
+      <c r="C156" s="117"/>
+      <c r="D156" s="117"/>
+      <c r="E156" s="117"/>
+      <c r="F156" s="117"/>
+      <c r="G156" s="117"/>
+      <c r="H156" s="117"/>
+      <c r="I156" s="117"/>
+      <c r="J156" s="117"/>
+      <c r="K156" s="117"/>
+      <c r="L156" s="117"/>
       <c r="M156" s="44"/>
       <c r="N156" s="44"/>
       <c r="O156" s="44"/>
@@ -17093,10 +17093,10 @@
       <c r="D157" s="44"/>
       <c r="E157" s="44"/>
       <c r="F157" s="44"/>
-      <c r="G157" s="108" t="s">
+      <c r="G157" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H157" s="109"/>
+      <c r="H157" s="108"/>
       <c r="I157" s="45"/>
       <c r="J157" s="44"/>
       <c r="K157" s="44"/>
@@ -17166,7 +17166,7 @@
       <c r="S159" s="44"/>
     </row>
     <row r="160" spans="1:27" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="110" t="s">
+      <c r="A160" s="111" t="s">
         <v>28</v>
       </c>
       <c r="B160" s="56"/>
@@ -17196,7 +17196,7 @@
       </c>
     </row>
     <row r="161" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="111"/>
+      <c r="A161" s="112"/>
       <c r="B161" s="56"/>
       <c r="C161" s="32"/>
       <c r="D161" s="10" t="str">
@@ -17228,7 +17228,7 @@
       </c>
     </row>
     <row r="162" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="111"/>
+      <c r="A162" s="112"/>
       <c r="B162" s="56"/>
       <c r="C162" s="32"/>
       <c r="D162" s="10" t="str">
@@ -17250,7 +17250,7 @@
       </c>
     </row>
     <row r="163" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="111"/>
+      <c r="A163" s="112"/>
       <c r="B163" s="56"/>
       <c r="C163" s="32"/>
       <c r="D163" s="10" t="str">
@@ -17272,7 +17272,7 @@
       </c>
     </row>
     <row r="164" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="111"/>
+      <c r="A164" s="112"/>
       <c r="B164" s="56"/>
       <c r="C164" s="32"/>
       <c r="D164" s="10" t="str">
@@ -17294,7 +17294,7 @@
       </c>
     </row>
     <row r="165" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="111"/>
+      <c r="A165" s="112"/>
       <c r="B165" s="56"/>
       <c r="C165" s="32"/>
       <c r="D165" s="10" t="str">
@@ -17316,7 +17316,7 @@
       </c>
     </row>
     <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="111"/>
+      <c r="A166" s="112"/>
       <c r="B166" s="56"/>
       <c r="C166" s="32"/>
       <c r="D166" s="10" t="str">
@@ -17338,7 +17338,7 @@
       </c>
     </row>
     <row r="167" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="111"/>
+      <c r="A167" s="112"/>
       <c r="B167" s="56"/>
       <c r="C167" s="32"/>
       <c r="D167" s="10" t="str">
@@ -17360,7 +17360,7 @@
       </c>
     </row>
     <row r="168" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="111"/>
+      <c r="A168" s="112"/>
       <c r="B168" s="56"/>
       <c r="C168" s="32"/>
       <c r="D168" s="10" t="str">
@@ -17382,7 +17382,7 @@
       </c>
     </row>
     <row r="169" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="111"/>
+      <c r="A169" s="112"/>
       <c r="B169" s="56"/>
       <c r="C169" s="32"/>
       <c r="D169" s="10" t="str">
@@ -17402,7 +17402,7 @@
       </c>
     </row>
     <row r="170" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="111"/>
+      <c r="A170" s="112"/>
       <c r="B170" s="56"/>
       <c r="C170" s="32"/>
       <c r="D170" s="10" t="str">
@@ -17416,7 +17416,7 @@
       <c r="I170" s="49"/>
     </row>
     <row r="171" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="111"/>
+      <c r="A171" s="112"/>
       <c r="B171" s="56"/>
       <c r="C171" s="32"/>
       <c r="D171" s="10" t="str">
@@ -17430,7 +17430,7 @@
       <c r="I171" s="50"/>
     </row>
     <row r="172" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="111"/>
+      <c r="A172" s="112"/>
       <c r="B172" s="56"/>
       <c r="C172" s="32"/>
       <c r="D172" s="10" t="str">
@@ -17449,47 +17449,47 @@
       </c>
     </row>
     <row r="173" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="111"/>
+      <c r="A173" s="112"/>
       <c r="B173" s="56"/>
       <c r="C173" s="32"/>
       <c r="D173" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E173" s="113" t="str">
+      <c r="E173" s="109" t="str">
         <f>IF(F169&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F173" s="114"/>
-      <c r="G173" s="114"/>
-      <c r="H173" s="114"/>
+      <c r="F173" s="110"/>
+      <c r="G173" s="110"/>
+      <c r="H173" s="110"/>
       <c r="I173" s="12" t="str">
         <f>IF(F169&lt;&gt;"",SUM(F160:F169),"")</f>
         <v/>
       </c>
     </row>
     <row r="174" spans="1:28" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="111"/>
+      <c r="A174" s="112"/>
       <c r="B174" s="56"/>
       <c r="C174" s="32"/>
       <c r="D174" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E174" s="115" t="str">
+      <c r="E174" s="114" t="str">
         <f>IF(F169&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F174" s="116"/>
-      <c r="G174" s="116"/>
-      <c r="H174" s="116"/>
+      <c r="F174" s="115"/>
+      <c r="G174" s="115"/>
+      <c r="H174" s="115"/>
       <c r="I174" s="16" t="str">
         <f>IF(F169&lt;&gt;"",AB161,"")</f>
         <v/>
       </c>
     </row>
     <row r="175" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="111"/>
+      <c r="A175" s="112"/>
       <c r="B175" s="34"/>
       <c r="C175" s="58"/>
       <c r="D175" s="10" t="str">
@@ -17506,7 +17506,7 @@
       </c>
     </row>
     <row r="176" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="111"/>
+      <c r="A176" s="112"/>
       <c r="B176" s="34"/>
       <c r="C176" s="32"/>
       <c r="D176" s="10" t="str">
@@ -17520,7 +17520,7 @@
       <c r="I176" s="50"/>
     </row>
     <row r="177" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="111"/>
+      <c r="A177" s="112"/>
       <c r="B177" s="34"/>
       <c r="C177" s="32"/>
       <c r="D177" s="10" t="str">
@@ -17534,7 +17534,7 @@
       <c r="I177" s="50"/>
     </row>
     <row r="178" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="111"/>
+      <c r="A178" s="112"/>
       <c r="B178" s="34"/>
       <c r="C178" s="32"/>
       <c r="D178" s="10" t="str">
@@ -17548,7 +17548,7 @@
       <c r="I178" s="50"/>
     </row>
     <row r="179" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="112"/>
+      <c r="A179" s="113"/>
       <c r="B179" s="34"/>
       <c r="C179" s="32"/>
       <c r="D179" s="11" t="str">
@@ -17568,19 +17568,19 @@
     </row>
     <row r="180" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="43"/>
-      <c r="B180" s="107" t="s">
+      <c r="B180" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C180" s="107"/>
-      <c r="D180" s="107"/>
-      <c r="E180" s="107"/>
-      <c r="F180" s="107"/>
-      <c r="G180" s="107"/>
-      <c r="H180" s="107"/>
-      <c r="I180" s="107"/>
-      <c r="J180" s="107"/>
-      <c r="K180" s="107"/>
-      <c r="L180" s="107"/>
+      <c r="C180" s="117"/>
+      <c r="D180" s="117"/>
+      <c r="E180" s="117"/>
+      <c r="F180" s="117"/>
+      <c r="G180" s="117"/>
+      <c r="H180" s="117"/>
+      <c r="I180" s="117"/>
+      <c r="J180" s="117"/>
+      <c r="K180" s="117"/>
+      <c r="L180" s="117"/>
       <c r="M180" s="44"/>
       <c r="N180" s="44"/>
       <c r="O180" s="44"/>
@@ -17591,17 +17591,17 @@
     </row>
     <row r="181" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="43"/>
-      <c r="B181" s="107"/>
-      <c r="C181" s="107"/>
-      <c r="D181" s="107"/>
-      <c r="E181" s="107"/>
-      <c r="F181" s="107"/>
-      <c r="G181" s="107"/>
-      <c r="H181" s="107"/>
-      <c r="I181" s="107"/>
-      <c r="J181" s="107"/>
-      <c r="K181" s="107"/>
-      <c r="L181" s="107"/>
+      <c r="B181" s="117"/>
+      <c r="C181" s="117"/>
+      <c r="D181" s="117"/>
+      <c r="E181" s="117"/>
+      <c r="F181" s="117"/>
+      <c r="G181" s="117"/>
+      <c r="H181" s="117"/>
+      <c r="I181" s="117"/>
+      <c r="J181" s="117"/>
+      <c r="K181" s="117"/>
+      <c r="L181" s="117"/>
       <c r="M181" s="44"/>
       <c r="N181" s="44"/>
       <c r="O181" s="44"/>
@@ -17617,10 +17617,10 @@
       <c r="D182" s="44"/>
       <c r="E182" s="44"/>
       <c r="F182" s="44"/>
-      <c r="G182" s="108" t="s">
+      <c r="G182" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H182" s="109"/>
+      <c r="H182" s="108"/>
       <c r="I182" s="45"/>
       <c r="J182" s="44"/>
       <c r="K182" s="44"/>
@@ -17690,7 +17690,7 @@
       <c r="S184" s="44"/>
     </row>
     <row r="185" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="110" t="s">
+      <c r="A185" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B185" s="56"/>
@@ -17720,7 +17720,7 @@
       </c>
     </row>
     <row r="186" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="111"/>
+      <c r="A186" s="112"/>
       <c r="B186" s="56"/>
       <c r="C186" s="32"/>
       <c r="D186" s="10" t="str">
@@ -17752,7 +17752,7 @@
       </c>
     </row>
     <row r="187" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="111"/>
+      <c r="A187" s="112"/>
       <c r="B187" s="56"/>
       <c r="C187" s="32"/>
       <c r="D187" s="10" t="str">
@@ -17774,7 +17774,7 @@
       </c>
     </row>
     <row r="188" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="111"/>
+      <c r="A188" s="112"/>
       <c r="B188" s="56"/>
       <c r="C188" s="32"/>
       <c r="D188" s="10" t="str">
@@ -17796,7 +17796,7 @@
       </c>
     </row>
     <row r="189" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="111"/>
+      <c r="A189" s="112"/>
       <c r="B189" s="56"/>
       <c r="C189" s="32"/>
       <c r="D189" s="10" t="str">
@@ -17818,7 +17818,7 @@
       </c>
     </row>
     <row r="190" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="111"/>
+      <c r="A190" s="112"/>
       <c r="B190" s="56"/>
       <c r="C190" s="32"/>
       <c r="D190" s="10" t="str">
@@ -17840,7 +17840,7 @@
       </c>
     </row>
     <row r="191" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="111"/>
+      <c r="A191" s="112"/>
       <c r="B191" s="56"/>
       <c r="C191" s="32"/>
       <c r="D191" s="10" t="str">
@@ -17862,7 +17862,7 @@
       </c>
     </row>
     <row r="192" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="111"/>
+      <c r="A192" s="112"/>
       <c r="B192" s="56"/>
       <c r="C192" s="32"/>
       <c r="D192" s="10" t="str">
@@ -17884,7 +17884,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="111"/>
+      <c r="A193" s="112"/>
       <c r="B193" s="56"/>
       <c r="C193" s="32"/>
       <c r="D193" s="10" t="str">
@@ -17906,7 +17906,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="111"/>
+      <c r="A194" s="112"/>
       <c r="B194" s="56"/>
       <c r="C194" s="32"/>
       <c r="D194" s="10" t="str">
@@ -17926,7 +17926,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="111"/>
+      <c r="A195" s="112"/>
       <c r="B195" s="56"/>
       <c r="C195" s="32"/>
       <c r="D195" s="10" t="str">
@@ -17940,7 +17940,7 @@
       <c r="I195" s="49"/>
     </row>
     <row r="196" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="111"/>
+      <c r="A196" s="112"/>
       <c r="B196" s="56"/>
       <c r="C196" s="32"/>
       <c r="D196" s="10" t="str">
@@ -17954,7 +17954,7 @@
       <c r="I196" s="50"/>
     </row>
     <row r="197" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="111"/>
+      <c r="A197" s="112"/>
       <c r="B197" s="56"/>
       <c r="C197" s="32"/>
       <c r="D197" s="10" t="str">
@@ -17973,47 +17973,47 @@
       </c>
     </row>
     <row r="198" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="111"/>
+      <c r="A198" s="112"/>
       <c r="B198" s="56"/>
       <c r="C198" s="32"/>
       <c r="D198" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E198" s="113" t="str">
+      <c r="E198" s="109" t="str">
         <f>IF(F194&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F198" s="114"/>
-      <c r="G198" s="114"/>
-      <c r="H198" s="114"/>
+      <c r="F198" s="110"/>
+      <c r="G198" s="110"/>
+      <c r="H198" s="110"/>
       <c r="I198" s="12" t="str">
         <f>IF(F194&lt;&gt;"",SUM(F185:F194),"")</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="111"/>
+      <c r="A199" s="112"/>
       <c r="B199" s="56"/>
       <c r="C199" s="32"/>
       <c r="D199" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E199" s="115" t="str">
+      <c r="E199" s="114" t="str">
         <f>IF(F194&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F199" s="116"/>
-      <c r="G199" s="116"/>
-      <c r="H199" s="116"/>
+      <c r="F199" s="115"/>
+      <c r="G199" s="115"/>
+      <c r="H199" s="115"/>
       <c r="I199" s="16" t="str">
         <f>IF(F194&lt;&gt;"",AB186,"")</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="111"/>
+      <c r="A200" s="112"/>
       <c r="B200" s="56"/>
       <c r="C200" s="32"/>
       <c r="D200" s="10" t="str">
@@ -18030,7 +18030,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="111"/>
+      <c r="A201" s="112"/>
       <c r="B201" s="34"/>
       <c r="C201" s="32"/>
       <c r="D201" s="10" t="str">
@@ -18044,7 +18044,7 @@
       <c r="I201" s="50"/>
     </row>
     <row r="202" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="111"/>
+      <c r="A202" s="112"/>
       <c r="B202" s="34"/>
       <c r="C202" s="32"/>
       <c r="D202" s="10" t="str">
@@ -18058,7 +18058,7 @@
       <c r="I202" s="50"/>
     </row>
     <row r="203" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="111"/>
+      <c r="A203" s="112"/>
       <c r="B203" s="34"/>
       <c r="C203" s="32"/>
       <c r="D203" s="10" t="str">
@@ -18072,7 +18072,7 @@
       <c r="I203" s="50"/>
     </row>
     <row r="204" spans="1:9" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="112"/>
+      <c r="A204" s="113"/>
       <c r="B204" s="34"/>
       <c r="C204" s="32"/>
       <c r="D204" s="11" t="str">
@@ -18093,46 +18093,46 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xvw55rBl+8QauwDbqXfPTEJvlFDUCVQW9eBF4D1fCPDMzZnBE0eg23U/adjRGpGtDkno/gEp3o8WBaDX9CrDpg==" saltValue="kVJ3wM2y/GPu2SWvmMPnkg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="40">
+    <mergeCell ref="B180:L181"/>
+    <mergeCell ref="G182:H182"/>
+    <mergeCell ref="A185:A204"/>
+    <mergeCell ref="E198:H198"/>
+    <mergeCell ref="E199:H199"/>
+    <mergeCell ref="B155:L156"/>
+    <mergeCell ref="G157:H157"/>
+    <mergeCell ref="A160:A179"/>
+    <mergeCell ref="E173:H173"/>
+    <mergeCell ref="E174:H174"/>
+    <mergeCell ref="B130:L131"/>
+    <mergeCell ref="G132:H132"/>
+    <mergeCell ref="A135:A154"/>
+    <mergeCell ref="E148:H148"/>
+    <mergeCell ref="E149:H149"/>
+    <mergeCell ref="B105:L106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="A110:A129"/>
+    <mergeCell ref="E123:H123"/>
+    <mergeCell ref="E124:H124"/>
+    <mergeCell ref="B79:L80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="A84:A104"/>
+    <mergeCell ref="E98:H98"/>
+    <mergeCell ref="E99:H99"/>
+    <mergeCell ref="B53:L54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A58:A78"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="B27:L28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A32:A52"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="A6:A26"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="B1:L2"/>
-    <mergeCell ref="B27:L28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A32:A52"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="B53:L54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A58:A78"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="B79:L80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="A84:A104"/>
-    <mergeCell ref="E98:H98"/>
-    <mergeCell ref="E99:H99"/>
-    <mergeCell ref="B105:L106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="A110:A129"/>
-    <mergeCell ref="E123:H123"/>
-    <mergeCell ref="E124:H124"/>
-    <mergeCell ref="B130:L131"/>
-    <mergeCell ref="G132:H132"/>
-    <mergeCell ref="A135:A154"/>
-    <mergeCell ref="E148:H148"/>
-    <mergeCell ref="E149:H149"/>
-    <mergeCell ref="B155:L156"/>
-    <mergeCell ref="G157:H157"/>
-    <mergeCell ref="A160:A179"/>
-    <mergeCell ref="E173:H173"/>
-    <mergeCell ref="E174:H174"/>
-    <mergeCell ref="B180:L181"/>
-    <mergeCell ref="G182:H182"/>
-    <mergeCell ref="A185:A204"/>
-    <mergeCell ref="E198:H198"/>
-    <mergeCell ref="E199:H199"/>
   </mergeCells>
   <conditionalFormatting sqref="I205:I1048576 I3:I6 I8:I16">
     <cfRule type="cellIs" dxfId="35" priority="57" operator="lessThan">
@@ -18322,21 +18322,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -18385,16 +18370,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18408,16 +18409,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOC: Updated DoD for Sprint 4
DOC: Updated DoD for Sprint 4, and personal Burndown Chart Iwan vd B
</commit_message>
<xml_diff>
--- a/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
+++ b/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leerling Iwan" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="71">
   <si>
     <t>Omschrijving taak</t>
   </si>
@@ -833,6 +833,24 @@
   </si>
   <si>
     <t>Team Leader</t>
+  </si>
+  <si>
+    <t>Bord opnmaken</t>
+  </si>
+  <si>
+    <t>User stories en taken prioriseren</t>
+  </si>
+  <si>
+    <t>Code conventions maken</t>
+  </si>
+  <si>
+    <t>Formule level progression</t>
+  </si>
+  <si>
+    <t>Controleren van taken volgens de DoD</t>
+  </si>
+  <si>
+    <t>Persoonlijke burndown charts maken</t>
   </si>
 </sst>
 </file>
@@ -1932,19 +1950,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1954,6 +1967,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1966,9 +1987,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3526,37 +3544,37 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>14.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>12.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.9999999999999964</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7.1999999999999966</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5.3999999999999968</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3.599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.7999999999999969</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-3.1086244689504383E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3640,37 +3658,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6302,7 +6320,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -13510,8 +13528,8 @@
   </sheetPr>
   <dimension ref="A1:AI204"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13541,35 +13559,35 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
       <c r="M1" s="44"/>
       <c r="S1" s="44"/>
     </row>
     <row r="2" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
       <c r="M2" s="44"/>
       <c r="S2" s="44"/>
       <c r="AF2" s="82" t="s">
@@ -13583,10 +13601,10 @@
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
-      <c r="G3" s="107" t="s">
+      <c r="G3" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="108"/>
+      <c r="H3" s="109"/>
       <c r="I3" s="45"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
@@ -13621,7 +13639,7 @@
       </c>
       <c r="AG4" s="80">
         <f ca="1">TODAY()</f>
-        <v>43063</v>
+        <v>43108</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13676,7 +13694,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="110" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -13732,7 +13750,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="34" t="s">
         <v>59</v>
       </c>
@@ -13766,7 +13784,7 @@
       <c r="AI7" s="87"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
+      <c r="A8" s="111"/>
       <c r="B8" s="34" t="s">
         <v>60</v>
       </c>
@@ -13827,7 +13845,7 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
+      <c r="A9" s="111"/>
       <c r="B9" s="34" t="s">
         <v>61</v>
       </c>
@@ -13861,27 +13879,27 @@
       </c>
       <c r="AE9" s="78">
         <f>I71</f>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="78" t="str">
+        <v>1.8</v>
+      </c>
+      <c r="AF9" s="78">
         <f>I72</f>
-        <v/>
-      </c>
-      <c r="AG9" s="78" t="str">
+        <v>18</v>
+      </c>
+      <c r="AG9" s="78">
         <f>I73</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AH9" s="79" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AI9" s="87" t="str">
+        <v>Keurig</v>
+      </c>
+      <c r="AI9" s="87">
         <f>H78</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
+      <c r="A10" s="111"/>
       <c r="B10" s="34" t="s">
         <v>63</v>
       </c>
@@ -13935,7 +13953,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="34"/>
       <c r="C11" s="65"/>
       <c r="D11" s="61" t="str">
@@ -13962,7 +13980,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="34"/>
       <c r="C12" s="65"/>
       <c r="D12" s="61" t="str">
@@ -13989,7 +14007,7 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="34"/>
       <c r="C13" s="65"/>
       <c r="D13" s="61" t="str">
@@ -14016,7 +14034,7 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="34"/>
       <c r="C14" s="65"/>
       <c r="D14" s="61" t="str">
@@ -14043,7 +14061,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="34"/>
       <c r="C15" s="65"/>
       <c r="D15" s="61" t="str">
@@ -14070,7 +14088,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="112"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="34"/>
       <c r="C16" s="65"/>
       <c r="D16" s="61" t="str">
@@ -14097,7 +14115,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="34"/>
       <c r="C17" s="65"/>
       <c r="D17" s="61" t="str">
@@ -14111,7 +14129,7 @@
       <c r="I17" s="50"/>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="34"/>
       <c r="C18" s="65"/>
       <c r="D18" s="61" t="str">
@@ -14125,7 +14143,7 @@
       <c r="I18" s="50"/>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="34"/>
       <c r="C19" s="65"/>
       <c r="D19" s="61" t="str">
@@ -14144,47 +14162,47 @@
       </c>
     </row>
     <row r="20" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="34"/>
       <c r="C20" s="65"/>
       <c r="D20" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E20" s="109" t="str">
+      <c r="E20" s="113" t="str">
         <f>IF(F16&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v># Uren afgetikt aan het eind van de sprint:</v>
       </c>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
+      <c r="F20" s="114"/>
+      <c r="G20" s="114"/>
+      <c r="H20" s="114"/>
       <c r="I20" s="12">
         <f>IF(F16&lt;&gt;"",SUM(F6:F16),"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="64"/>
       <c r="C21" s="65"/>
       <c r="D21" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E21" s="114" t="str">
+      <c r="E21" s="115" t="str">
         <f>IF(F16&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v>Dit moesten er zijn:</v>
       </c>
-      <c r="F21" s="115"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="115"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="116"/>
+      <c r="H21" s="116"/>
       <c r="I21" s="16">
         <f>IF(F16&lt;&gt;"",AB8,"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="64"/>
       <c r="C22" s="65"/>
       <c r="D22" s="61" t="str">
@@ -14201,7 +14219,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="64"/>
       <c r="C23" s="65"/>
       <c r="D23" s="61" t="str">
@@ -14215,7 +14233,7 @@
       <c r="I23" s="50"/>
     </row>
     <row r="24" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112"/>
+      <c r="A24" s="111"/>
       <c r="B24" s="64" t="s">
         <v>62</v>
       </c>
@@ -14231,7 +14249,7 @@
       <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112"/>
+      <c r="A25" s="111"/>
       <c r="B25" s="64" t="s">
         <v>57</v>
       </c>
@@ -14247,7 +14265,7 @@
       <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="113"/>
+      <c r="A26" s="112"/>
       <c r="B26" s="66" t="s">
         <v>64</v>
       </c>
@@ -14269,20 +14287,20 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
-      <c r="B27" s="117" t="str">
+      <c r="B27" s="107" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
-      <c r="G27" s="117"/>
-      <c r="H27" s="117"/>
-      <c r="I27" s="117"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="117"/>
-      <c r="L27" s="117"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
       <c r="M27" s="44"/>
       <c r="N27" s="44"/>
       <c r="O27" s="44"/>
@@ -14293,17 +14311,17 @@
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
-      <c r="B28" s="117"/>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="117"/>
-      <c r="I28" s="117"/>
-      <c r="J28" s="117"/>
-      <c r="K28" s="117"/>
-      <c r="L28" s="117"/>
+      <c r="B28" s="107"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="107"/>
+      <c r="L28" s="107"/>
       <c r="M28" s="44"/>
       <c r="N28" s="44"/>
       <c r="O28" s="44"/>
@@ -14319,10 +14337,10 @@
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
-      <c r="G29" s="107" t="s">
+      <c r="G29" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="108"/>
+      <c r="H29" s="109"/>
       <c r="I29" s="45"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
@@ -14392,7 +14410,7 @@
       <c r="S31" s="44"/>
     </row>
     <row r="32" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="111" t="s">
+      <c r="A32" s="110" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="33"/>
@@ -14421,7 +14439,7 @@
       </c>
     </row>
     <row r="33" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="112"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="34"/>
       <c r="C33" s="104"/>
       <c r="D33" s="98"/>
@@ -14443,7 +14461,7 @@
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="64"/>
       <c r="C34" s="68"/>
       <c r="D34" s="61" t="str">
@@ -14475,7 +14493,7 @@
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="64"/>
       <c r="C35" s="65"/>
       <c r="D35" s="61" t="str">
@@ -14500,7 +14518,7 @@
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="112"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="64"/>
       <c r="C36" s="65"/>
       <c r="D36" s="61" t="str">
@@ -14525,7 +14543,7 @@
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="64"/>
       <c r="C37" s="65"/>
       <c r="D37" s="61" t="str">
@@ -14550,7 +14568,7 @@
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="112"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="64"/>
       <c r="C38" s="65"/>
       <c r="D38" s="61" t="str">
@@ -14575,7 +14593,7 @@
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
+      <c r="A39" s="111"/>
       <c r="B39" s="64"/>
       <c r="C39" s="65"/>
       <c r="D39" s="61" t="str">
@@ -14600,7 +14618,7 @@
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="112"/>
+      <c r="A40" s="111"/>
       <c r="B40" s="64"/>
       <c r="C40" s="65"/>
       <c r="D40" s="61" t="str">
@@ -14625,7 +14643,7 @@
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="112"/>
+      <c r="A41" s="111"/>
       <c r="B41" s="64"/>
       <c r="C41" s="65"/>
       <c r="D41" s="61" t="str">
@@ -14650,7 +14668,7 @@
       </c>
     </row>
     <row r="42" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="112"/>
+      <c r="A42" s="111"/>
       <c r="B42" s="64"/>
       <c r="C42" s="65"/>
       <c r="D42" s="61" t="str">
@@ -14675,7 +14693,7 @@
       </c>
     </row>
     <row r="43" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="112"/>
+      <c r="A43" s="111"/>
       <c r="B43" s="64"/>
       <c r="C43" s="65"/>
       <c r="D43" s="61" t="str">
@@ -14689,7 +14707,7 @@
       <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="112"/>
+      <c r="A44" s="111"/>
       <c r="B44" s="64"/>
       <c r="C44" s="65"/>
       <c r="D44" s="61" t="str">
@@ -14703,7 +14721,7 @@
       <c r="I44" s="50"/>
     </row>
     <row r="45" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="112"/>
+      <c r="A45" s="111"/>
       <c r="B45" s="64"/>
       <c r="C45" s="65"/>
       <c r="D45" s="61" t="str">
@@ -14722,47 +14740,47 @@
       </c>
     </row>
     <row r="46" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="112"/>
+      <c r="A46" s="111"/>
       <c r="B46" s="64"/>
       <c r="C46" s="65"/>
       <c r="D46" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E46" s="109" t="str">
+      <c r="E46" s="113" t="str">
         <f>IF(F42&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F46" s="110"/>
-      <c r="G46" s="110"/>
-      <c r="H46" s="110"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="114"/>
+      <c r="H46" s="114"/>
       <c r="I46" s="12" t="str">
         <f>IF(F42&lt;&gt;"",SUM(F32:F42),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="112"/>
+      <c r="A47" s="111"/>
       <c r="B47" s="64"/>
       <c r="C47" s="65"/>
       <c r="D47" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E47" s="114" t="str">
+      <c r="E47" s="115" t="str">
         <f>IF(F42&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F47" s="115"/>
-      <c r="G47" s="115"/>
-      <c r="H47" s="115"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="116"/>
+      <c r="H47" s="116"/>
       <c r="I47" s="16" t="str">
         <f>IF(F42&lt;&gt;"",AB34,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="112"/>
+      <c r="A48" s="111"/>
       <c r="B48" s="34"/>
       <c r="C48" s="69"/>
       <c r="D48" s="61" t="str">
@@ -14779,7 +14797,7 @@
       </c>
     </row>
     <row r="49" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="112"/>
+      <c r="A49" s="111"/>
       <c r="B49" s="34"/>
       <c r="C49" s="65"/>
       <c r="D49" s="61" t="str">
@@ -14793,7 +14811,7 @@
       <c r="I49" s="50"/>
     </row>
     <row r="50" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="112"/>
+      <c r="A50" s="111"/>
       <c r="B50" s="34"/>
       <c r="C50" s="65"/>
       <c r="D50" s="61" t="str">
@@ -14807,7 +14825,7 @@
       <c r="I50" s="50"/>
     </row>
     <row r="51" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="112"/>
+      <c r="A51" s="111"/>
       <c r="B51" s="34"/>
       <c r="C51" s="65"/>
       <c r="D51" s="61" t="str">
@@ -14821,7 +14839,7 @@
       <c r="I51" s="50"/>
     </row>
     <row r="52" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="113"/>
+      <c r="A52" s="112"/>
       <c r="B52" s="70"/>
       <c r="C52" s="67"/>
       <c r="D52" s="62" t="str">
@@ -14841,20 +14859,20 @@
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
-      <c r="B53" s="117" t="str">
+      <c r="B53" s="107" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C53" s="117"/>
-      <c r="D53" s="117"/>
-      <c r="E53" s="117"/>
-      <c r="F53" s="117"/>
-      <c r="G53" s="117"/>
-      <c r="H53" s="117"/>
-      <c r="I53" s="117"/>
-      <c r="J53" s="117"/>
-      <c r="K53" s="117"/>
-      <c r="L53" s="117"/>
+      <c r="C53" s="107"/>
+      <c r="D53" s="107"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="107"/>
+      <c r="G53" s="107"/>
+      <c r="H53" s="107"/>
+      <c r="I53" s="107"/>
+      <c r="J53" s="107"/>
+      <c r="K53" s="107"/>
+      <c r="L53" s="107"/>
       <c r="M53" s="44"/>
       <c r="N53" s="44"/>
       <c r="O53" s="44"/>
@@ -14865,17 +14883,17 @@
     </row>
     <row r="54" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
-      <c r="B54" s="117"/>
-      <c r="C54" s="117"/>
-      <c r="D54" s="117"/>
-      <c r="E54" s="117"/>
-      <c r="F54" s="117"/>
-      <c r="G54" s="117"/>
-      <c r="H54" s="117"/>
-      <c r="I54" s="117"/>
-      <c r="J54" s="117"/>
-      <c r="K54" s="117"/>
-      <c r="L54" s="117"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="107"/>
+      <c r="D54" s="107"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="107"/>
+      <c r="G54" s="107"/>
+      <c r="H54" s="107"/>
+      <c r="I54" s="107"/>
+      <c r="J54" s="107"/>
+      <c r="K54" s="107"/>
+      <c r="L54" s="107"/>
       <c r="M54" s="44"/>
       <c r="N54" s="44"/>
       <c r="O54" s="44"/>
@@ -14891,10 +14909,10 @@
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
       <c r="F55" s="44"/>
-      <c r="G55" s="107" t="s">
+      <c r="G55" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H55" s="108"/>
+      <c r="H55" s="109"/>
       <c r="I55" s="45"/>
       <c r="J55" s="44"/>
       <c r="K55" s="44"/>
@@ -14964,11 +14982,15 @@
       <c r="S57" s="44"/>
     </row>
     <row r="58" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="111" t="s">
+      <c r="A58" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="63"/>
+      <c r="B58" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="63">
+        <v>5</v>
+      </c>
       <c r="D58" s="60" t="str">
         <f>IF(C58&lt;&gt;"",IF(AND(C58&lt;&gt;1,C58&lt;&gt;2,C58&lt;&gt;3,C58&lt;&gt;5,C58&lt;&gt;8,C58&lt;&gt;13,C58&lt;&gt;20,C58&lt;&gt;40,C58&lt;&gt;100),"Fout",""),"")</f>
         <v/>
@@ -14981,11 +15003,11 @@
       </c>
       <c r="G58" s="17">
         <f>AB60</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H58" s="20">
         <f>AB60-F58</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I58" s="21">
         <f>G58-H58</f>
@@ -14994,32 +15016,42 @@
       <c r="J58" s="106"/>
     </row>
     <row r="59" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="112"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="104"/>
+      <c r="A59" s="111"/>
+      <c r="B59" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="104">
+        <v>10</v>
+      </c>
       <c r="D59" s="98"/>
       <c r="E59" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="F59" s="100"/>
+      <c r="F59" s="100">
+        <v>0</v>
+      </c>
       <c r="G59" s="101">
         <f t="shared" ref="G59:G68" si="11">(G58-(AB$60/10))</f>
-        <v>0</v>
-      </c>
-      <c r="H59" s="96" t="e">
+        <v>16.2</v>
+      </c>
+      <c r="H59" s="96">
         <f>IF(F59="",NA(),H58-F59)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I59" s="22" t="str">
+        <v>18</v>
+      </c>
+      <c r="I59" s="22">
         <f t="shared" ref="I59:I62" si="12">IF(F59="","",G59-H59)</f>
-        <v/>
+        <v>-1.8000000000000007</v>
       </c>
       <c r="J59" s="106"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A60" s="112"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="68"/>
+      <c r="A60" s="111"/>
+      <c r="B60" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="68">
+        <v>3</v>
+      </c>
       <c r="D60" s="61" t="str">
         <f t="shared" ref="D60:D78" si="13">IF(C60&lt;&gt;"",IF(AND(C60&lt;&gt;1,C60&lt;&gt;2,C60&lt;&gt;3,C60&lt;&gt;5,C60&lt;&gt;8,C60&lt;&gt;13,C60&lt;&gt;20,C60&lt;&gt;40,C60&lt;&gt;100),"Fout",""),"")</f>
         <v/>
@@ -15027,18 +15059,20 @@
       <c r="E60" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="F60" s="75"/>
+      <c r="F60" s="75">
+        <v>0</v>
+      </c>
       <c r="G60" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H60" s="96" t="e">
+        <v>14.399999999999999</v>
+      </c>
+      <c r="H60" s="96">
         <f>IF(F60="",NA(),H59-F60)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I60" s="22" t="str">
+        <v>18</v>
+      </c>
+      <c r="I60" s="22">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-3.6000000000000014</v>
       </c>
       <c r="J60" s="106"/>
       <c r="AA60" t="s">
@@ -15046,11 +15080,11 @@
       </c>
       <c r="AB60">
         <f>SUM(C58:C78)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A61" s="112"/>
+      <c r="A61" s="111"/>
       <c r="B61" s="64"/>
       <c r="C61" s="65"/>
       <c r="D61" s="61" t="str">
@@ -15060,23 +15094,25 @@
       <c r="E61" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="75"/>
+      <c r="F61" s="75">
+        <v>0</v>
+      </c>
       <c r="G61" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H61" s="96" t="e">
+        <v>12.599999999999998</v>
+      </c>
+      <c r="H61" s="96">
         <f t="shared" ref="H61:H68" si="14">IF(F61="",NA(),H60-F61)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I61" s="22" t="str">
+        <v>18</v>
+      </c>
+      <c r="I61" s="22">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-5.4000000000000021</v>
       </c>
       <c r="J61" s="106"/>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A62" s="112"/>
+      <c r="A62" s="111"/>
       <c r="B62" s="64"/>
       <c r="C62" s="65"/>
       <c r="D62" s="61" t="str">
@@ -15086,23 +15122,25 @@
       <c r="E62" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="F62" s="75"/>
+      <c r="F62" s="75">
+        <v>5</v>
+      </c>
       <c r="G62" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H62" s="96" t="e">
+        <v>10.799999999999997</v>
+      </c>
+      <c r="H62" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I62" s="22" t="str">
+        <v>13</v>
+      </c>
+      <c r="I62" s="22">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-2.2000000000000028</v>
       </c>
       <c r="J62" s="106"/>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A63" s="112"/>
+      <c r="A63" s="111"/>
       <c r="B63" s="64"/>
       <c r="C63" s="65"/>
       <c r="D63" s="61" t="str">
@@ -15112,23 +15150,25 @@
       <c r="E63" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F63" s="75"/>
+      <c r="F63" s="75">
+        <v>0</v>
+      </c>
       <c r="G63" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H63" s="96" t="e">
+        <v>8.9999999999999964</v>
+      </c>
+      <c r="H63" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I63" s="22" t="str">
+        <v>13</v>
+      </c>
+      <c r="I63" s="22">
         <f>IF(F63="","",G63-H63)</f>
-        <v/>
+        <v>-4.0000000000000036</v>
       </c>
       <c r="J63" s="106"/>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A64" s="112"/>
+      <c r="A64" s="111"/>
       <c r="B64" s="64"/>
       <c r="C64" s="65"/>
       <c r="D64" s="61" t="str">
@@ -15138,23 +15178,25 @@
       <c r="E64" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="F64" s="75"/>
+      <c r="F64" s="75">
+        <v>0</v>
+      </c>
       <c r="G64" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H64" s="96" t="e">
+        <v>7.1999999999999966</v>
+      </c>
+      <c r="H64" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I64" s="22" t="str">
+        <v>13</v>
+      </c>
+      <c r="I64" s="22">
         <f t="shared" ref="I64:I68" si="15">IF(F64="","",G64-H64)</f>
-        <v/>
+        <v>-5.8000000000000034</v>
       </c>
       <c r="J64" s="106"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="112"/>
+      <c r="A65" s="111"/>
       <c r="B65" s="64"/>
       <c r="C65" s="65"/>
       <c r="D65" s="61" t="str">
@@ -15164,23 +15206,25 @@
       <c r="E65" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="75"/>
+      <c r="F65" s="75">
+        <v>0</v>
+      </c>
       <c r="G65" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H65" s="96" t="e">
+        <v>5.3999999999999968</v>
+      </c>
+      <c r="H65" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I65" s="22" t="str">
+        <v>13</v>
+      </c>
+      <c r="I65" s="22">
         <f t="shared" si="15"/>
-        <v/>
+        <v>-7.6000000000000032</v>
       </c>
       <c r="J65" s="106"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="112"/>
+      <c r="A66" s="111"/>
       <c r="B66" s="64"/>
       <c r="C66" s="65"/>
       <c r="D66" s="61" t="str">
@@ -15190,23 +15234,25 @@
       <c r="E66" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="F66" s="75"/>
+      <c r="F66" s="75">
+        <v>10</v>
+      </c>
       <c r="G66" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H66" s="96" t="e">
+        <v>3.599999999999997</v>
+      </c>
+      <c r="H66" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I66" s="22" t="str">
+        <v>3</v>
+      </c>
+      <c r="I66" s="22">
         <f t="shared" si="15"/>
-        <v/>
+        <v>0.59999999999999698</v>
       </c>
       <c r="J66" s="106"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="112"/>
+      <c r="A67" s="111"/>
       <c r="B67" s="64"/>
       <c r="C67" s="65"/>
       <c r="D67" s="61" t="str">
@@ -15216,23 +15262,25 @@
       <c r="E67" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="75"/>
+      <c r="F67" s="75">
+        <v>0</v>
+      </c>
       <c r="G67" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H67" s="96" t="e">
+        <v>1.7999999999999969</v>
+      </c>
+      <c r="H67" s="96">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I67" s="22" t="str">
+        <v>3</v>
+      </c>
+      <c r="I67" s="22">
         <f t="shared" si="15"/>
-        <v/>
+        <v>-1.2000000000000031</v>
       </c>
       <c r="J67" s="106"/>
     </row>
     <row r="68" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="112"/>
+      <c r="A68" s="111"/>
       <c r="B68" s="64"/>
       <c r="C68" s="65"/>
       <c r="D68" s="61" t="str">
@@ -15242,23 +15290,25 @@
       <c r="E68" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="F68" s="76"/>
+      <c r="F68" s="76">
+        <v>3</v>
+      </c>
       <c r="G68" s="19">
         <f t="shared" si="11"/>
+        <v>-3.1086244689504383E-15</v>
+      </c>
+      <c r="H68" s="97">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H68" s="97" t="e">
-        <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I68" s="77" t="str">
+      <c r="I68" s="77">
         <f t="shared" si="15"/>
-        <v/>
+        <v>-3.1086244689504383E-15</v>
       </c>
       <c r="J68" s="106"/>
     </row>
     <row r="69" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="112"/>
+      <c r="A69" s="111"/>
       <c r="B69" s="64"/>
       <c r="C69" s="65"/>
       <c r="D69" s="61" t="str">
@@ -15272,7 +15322,7 @@
       <c r="I69" s="50"/>
     </row>
     <row r="70" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="112"/>
+      <c r="A70" s="111"/>
       <c r="B70" s="64"/>
       <c r="C70" s="65"/>
       <c r="D70" s="61" t="str">
@@ -15286,7 +15336,7 @@
       <c r="I70" s="50"/>
     </row>
     <row r="71" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="112"/>
+      <c r="A71" s="111"/>
       <c r="B71" s="64"/>
       <c r="C71" s="65"/>
       <c r="D71" s="61" t="str">
@@ -15301,51 +15351,51 @@
       </c>
       <c r="I71" s="28">
         <f>AB60/10</f>
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="72" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="112"/>
+      <c r="A72" s="111"/>
       <c r="B72" s="64"/>
       <c r="C72" s="65"/>
       <c r="D72" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E72" s="109" t="str">
+      <c r="E72" s="113" t="str">
         <f>IF(F68&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
-        <v/>
-      </c>
-      <c r="F72" s="110"/>
-      <c r="G72" s="110"/>
-      <c r="H72" s="110"/>
-      <c r="I72" s="12" t="str">
+        <v># Uren afgetikt aan het eind van de sprint:</v>
+      </c>
+      <c r="F72" s="114"/>
+      <c r="G72" s="114"/>
+      <c r="H72" s="114"/>
+      <c r="I72" s="12">
         <f>IF(F68&lt;&gt;"",SUM(F58:F68),"")</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="112"/>
+      <c r="A73" s="111"/>
       <c r="B73" s="64"/>
       <c r="C73" s="65"/>
       <c r="D73" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E73" s="114" t="str">
+      <c r="E73" s="115" t="str">
         <f>IF(F68&lt;&gt;"","Dit moesten er zijn:","")</f>
-        <v/>
-      </c>
-      <c r="F73" s="115"/>
-      <c r="G73" s="115"/>
-      <c r="H73" s="115"/>
-      <c r="I73" s="16" t="str">
+        <v>Dit moesten er zijn:</v>
+      </c>
+      <c r="F73" s="116"/>
+      <c r="G73" s="116"/>
+      <c r="H73" s="116"/>
+      <c r="I73" s="16">
         <f>IF(F68&lt;&gt;"",AB60,"")</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="112"/>
+      <c r="A74" s="111"/>
       <c r="B74" s="64"/>
       <c r="C74" s="65"/>
       <c r="D74" s="61" t="str">
@@ -15358,12 +15408,14 @@
       <c r="H74" s="47"/>
       <c r="I74" s="51" t="str">
         <f>IF(F68="","",IF(I72&lt;I73,"Dus te weinig.","Keurig"))</f>
-        <v/>
+        <v>Keurig</v>
       </c>
     </row>
     <row r="75" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="112"/>
-      <c r="B75" s="64"/>
+      <c r="A75" s="111"/>
+      <c r="B75" s="64" t="s">
+        <v>69</v>
+      </c>
       <c r="C75" s="65"/>
       <c r="D75" s="61" t="str">
         <f t="shared" si="13"/>
@@ -15376,8 +15428,10 @@
       <c r="I75" s="50"/>
     </row>
     <row r="76" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="112"/>
-      <c r="B76" s="64"/>
+      <c r="A76" s="111"/>
+      <c r="B76" s="64" t="s">
+        <v>57</v>
+      </c>
       <c r="C76" s="65"/>
       <c r="D76" s="61" t="str">
         <f t="shared" si="13"/>
@@ -15390,8 +15444,10 @@
       <c r="I76" s="50"/>
     </row>
     <row r="77" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="112"/>
-      <c r="B77" s="64"/>
+      <c r="A77" s="111"/>
+      <c r="B77" s="64" t="s">
+        <v>66</v>
+      </c>
       <c r="C77" s="65"/>
       <c r="D77" s="61" t="str">
         <f t="shared" si="13"/>
@@ -15404,8 +15460,10 @@
       <c r="I77" s="50"/>
     </row>
     <row r="78" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="113"/>
-      <c r="B78" s="66"/>
+      <c r="A78" s="112"/>
+      <c r="B78" s="66" t="s">
+        <v>65</v>
+      </c>
       <c r="C78" s="67"/>
       <c r="D78" s="62" t="str">
         <f t="shared" si="13"/>
@@ -15416,28 +15474,28 @@
       </c>
       <c r="F78" s="25"/>
       <c r="G78" s="25"/>
-      <c r="H78" s="26" t="str">
+      <c r="H78" s="26">
         <f>I72</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I78" s="27"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
-      <c r="B79" s="117" t="str">
+      <c r="B79" s="107" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C79" s="117"/>
-      <c r="D79" s="117"/>
-      <c r="E79" s="117"/>
-      <c r="F79" s="117"/>
-      <c r="G79" s="117"/>
-      <c r="H79" s="117"/>
-      <c r="I79" s="117"/>
-      <c r="J79" s="117"/>
-      <c r="K79" s="117"/>
-      <c r="L79" s="117"/>
+      <c r="C79" s="107"/>
+      <c r="D79" s="107"/>
+      <c r="E79" s="107"/>
+      <c r="F79" s="107"/>
+      <c r="G79" s="107"/>
+      <c r="H79" s="107"/>
+      <c r="I79" s="107"/>
+      <c r="J79" s="107"/>
+      <c r="K79" s="107"/>
+      <c r="L79" s="107"/>
       <c r="M79" s="44"/>
       <c r="N79" s="44"/>
       <c r="O79" s="44"/>
@@ -15448,17 +15506,17 @@
     </row>
     <row r="80" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="43"/>
-      <c r="B80" s="117"/>
-      <c r="C80" s="117"/>
-      <c r="D80" s="117"/>
-      <c r="E80" s="117"/>
-      <c r="F80" s="117"/>
-      <c r="G80" s="117"/>
-      <c r="H80" s="117"/>
-      <c r="I80" s="117"/>
-      <c r="J80" s="117"/>
-      <c r="K80" s="117"/>
-      <c r="L80" s="117"/>
+      <c r="B80" s="107"/>
+      <c r="C80" s="107"/>
+      <c r="D80" s="107"/>
+      <c r="E80" s="107"/>
+      <c r="F80" s="107"/>
+      <c r="G80" s="107"/>
+      <c r="H80" s="107"/>
+      <c r="I80" s="107"/>
+      <c r="J80" s="107"/>
+      <c r="K80" s="107"/>
+      <c r="L80" s="107"/>
       <c r="M80" s="44"/>
       <c r="N80" s="44"/>
       <c r="O80" s="44"/>
@@ -15474,10 +15532,10 @@
       <c r="D81" s="44"/>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
-      <c r="G81" s="107" t="s">
+      <c r="G81" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H81" s="108"/>
+      <c r="H81" s="109"/>
       <c r="I81" s="45"/>
       <c r="J81" s="44"/>
       <c r="K81" s="44"/>
@@ -15547,7 +15605,7 @@
       <c r="S83" s="44"/>
     </row>
     <row r="84" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="111" t="s">
+      <c r="A84" s="110" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="33"/>
@@ -15576,7 +15634,7 @@
       </c>
     </row>
     <row r="85" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="112"/>
+      <c r="A85" s="111"/>
       <c r="B85" s="34"/>
       <c r="C85" s="69"/>
       <c r="D85" s="98"/>
@@ -15598,7 +15656,7 @@
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A86" s="112"/>
+      <c r="A86" s="111"/>
       <c r="B86" s="64"/>
       <c r="C86" s="65"/>
       <c r="D86" s="61" t="str">
@@ -15630,7 +15688,7 @@
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A87" s="112"/>
+      <c r="A87" s="111"/>
       <c r="B87" s="64"/>
       <c r="C87" s="65"/>
       <c r="D87" s="61" t="str">
@@ -15655,7 +15713,7 @@
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A88" s="112"/>
+      <c r="A88" s="111"/>
       <c r="B88" s="64"/>
       <c r="C88" s="65"/>
       <c r="D88" s="61" t="str">
@@ -15680,7 +15738,7 @@
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A89" s="112"/>
+      <c r="A89" s="111"/>
       <c r="B89" s="64"/>
       <c r="C89" s="65"/>
       <c r="D89" s="61" t="str">
@@ -15705,7 +15763,7 @@
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A90" s="112"/>
+      <c r="A90" s="111"/>
       <c r="B90" s="64"/>
       <c r="C90" s="65"/>
       <c r="D90" s="61" t="str">
@@ -15730,7 +15788,7 @@
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="112"/>
+      <c r="A91" s="111"/>
       <c r="B91" s="64"/>
       <c r="C91" s="65"/>
       <c r="D91" s="61" t="str">
@@ -15755,7 +15813,7 @@
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A92" s="112"/>
+      <c r="A92" s="111"/>
       <c r="B92" s="64"/>
       <c r="C92" s="65"/>
       <c r="D92" s="61" t="str">
@@ -15780,7 +15838,7 @@
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A93" s="112"/>
+      <c r="A93" s="111"/>
       <c r="B93" s="64"/>
       <c r="C93" s="65"/>
       <c r="D93" s="61" t="str">
@@ -15805,7 +15863,7 @@
       </c>
     </row>
     <row r="94" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="112"/>
+      <c r="A94" s="111"/>
       <c r="B94" s="64"/>
       <c r="C94" s="65"/>
       <c r="D94" s="61" t="str">
@@ -15830,7 +15888,7 @@
       </c>
     </row>
     <row r="95" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="112"/>
+      <c r="A95" s="111"/>
       <c r="B95" s="64"/>
       <c r="C95" s="65"/>
       <c r="D95" s="61" t="str">
@@ -15844,7 +15902,7 @@
       <c r="I95" s="50"/>
     </row>
     <row r="96" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="112"/>
+      <c r="A96" s="111"/>
       <c r="B96" s="64"/>
       <c r="C96" s="65"/>
       <c r="D96" s="61" t="str">
@@ -15858,7 +15916,7 @@
       <c r="I96" s="50"/>
     </row>
     <row r="97" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="112"/>
+      <c r="A97" s="111"/>
       <c r="B97" s="64"/>
       <c r="C97" s="65"/>
       <c r="D97" s="61" t="str">
@@ -15877,47 +15935,47 @@
       </c>
     </row>
     <row r="98" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="112"/>
+      <c r="A98" s="111"/>
       <c r="B98" s="64"/>
       <c r="C98" s="65"/>
       <c r="D98" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E98" s="109" t="str">
+      <c r="E98" s="113" t="str">
         <f>IF(F94&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F98" s="110"/>
-      <c r="G98" s="110"/>
-      <c r="H98" s="110"/>
+      <c r="F98" s="114"/>
+      <c r="G98" s="114"/>
+      <c r="H98" s="114"/>
       <c r="I98" s="12" t="str">
         <f>IF(F94&lt;&gt;"",SUM(F84:F94),"")</f>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="112"/>
+      <c r="A99" s="111"/>
       <c r="B99" s="64"/>
       <c r="C99" s="65"/>
       <c r="D99" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E99" s="114" t="str">
+      <c r="E99" s="115" t="str">
         <f>IF(F94&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F99" s="115"/>
-      <c r="G99" s="115"/>
-      <c r="H99" s="115"/>
+      <c r="F99" s="116"/>
+      <c r="G99" s="116"/>
+      <c r="H99" s="116"/>
       <c r="I99" s="16" t="str">
         <f>IF(F94&lt;&gt;"",AB86,"")</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="112"/>
+      <c r="A100" s="111"/>
       <c r="B100" s="64"/>
       <c r="C100" s="65"/>
       <c r="D100" s="61" t="str">
@@ -15934,7 +15992,7 @@
       </c>
     </row>
     <row r="101" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="112"/>
+      <c r="A101" s="111"/>
       <c r="B101" s="64"/>
       <c r="C101" s="65"/>
       <c r="D101" s="61" t="str">
@@ -15948,7 +16006,7 @@
       <c r="I101" s="50"/>
     </row>
     <row r="102" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="112"/>
+      <c r="A102" s="111"/>
       <c r="B102" s="64"/>
       <c r="C102" s="65"/>
       <c r="D102" s="61" t="str">
@@ -15962,7 +16020,7 @@
       <c r="I102" s="50"/>
     </row>
     <row r="103" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="112"/>
+      <c r="A103" s="111"/>
       <c r="B103" s="64"/>
       <c r="C103" s="65"/>
       <c r="D103" s="61" t="str">
@@ -15976,7 +16034,7 @@
       <c r="I103" s="50"/>
     </row>
     <row r="104" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="113"/>
+      <c r="A104" s="112"/>
       <c r="B104" s="66"/>
       <c r="C104" s="67"/>
       <c r="D104" s="62" t="str">
@@ -15996,19 +16054,19 @@
     </row>
     <row r="105" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="43"/>
-      <c r="B105" s="117" t="s">
+      <c r="B105" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="117"/>
-      <c r="D105" s="117"/>
-      <c r="E105" s="117"/>
-      <c r="F105" s="117"/>
-      <c r="G105" s="117"/>
-      <c r="H105" s="117"/>
-      <c r="I105" s="117"/>
-      <c r="J105" s="117"/>
-      <c r="K105" s="117"/>
-      <c r="L105" s="117"/>
+      <c r="C105" s="107"/>
+      <c r="D105" s="107"/>
+      <c r="E105" s="107"/>
+      <c r="F105" s="107"/>
+      <c r="G105" s="107"/>
+      <c r="H105" s="107"/>
+      <c r="I105" s="107"/>
+      <c r="J105" s="107"/>
+      <c r="K105" s="107"/>
+      <c r="L105" s="107"/>
       <c r="M105" s="44"/>
       <c r="N105" s="44"/>
       <c r="O105" s="44"/>
@@ -16019,17 +16077,17 @@
     </row>
     <row r="106" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="43"/>
-      <c r="B106" s="117"/>
-      <c r="C106" s="117"/>
-      <c r="D106" s="117"/>
-      <c r="E106" s="117"/>
-      <c r="F106" s="117"/>
-      <c r="G106" s="117"/>
-      <c r="H106" s="117"/>
-      <c r="I106" s="117"/>
-      <c r="J106" s="117"/>
-      <c r="K106" s="117"/>
-      <c r="L106" s="117"/>
+      <c r="B106" s="107"/>
+      <c r="C106" s="107"/>
+      <c r="D106" s="107"/>
+      <c r="E106" s="107"/>
+      <c r="F106" s="107"/>
+      <c r="G106" s="107"/>
+      <c r="H106" s="107"/>
+      <c r="I106" s="107"/>
+      <c r="J106" s="107"/>
+      <c r="K106" s="107"/>
+      <c r="L106" s="107"/>
       <c r="M106" s="44"/>
       <c r="N106" s="44"/>
       <c r="O106" s="44"/>
@@ -16045,10 +16103,10 @@
       <c r="D107" s="44"/>
       <c r="E107" s="44"/>
       <c r="F107" s="44"/>
-      <c r="G107" s="107" t="s">
+      <c r="G107" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H107" s="108"/>
+      <c r="H107" s="109"/>
       <c r="I107" s="45"/>
       <c r="J107" s="44"/>
       <c r="K107" s="44"/>
@@ -16118,7 +16176,7 @@
       <c r="S109" s="44"/>
     </row>
     <row r="110" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="111" t="s">
+      <c r="A110" s="110" t="s">
         <v>26</v>
       </c>
       <c r="B110" s="56"/>
@@ -16148,7 +16206,7 @@
       </c>
     </row>
     <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="112"/>
+      <c r="A111" s="111"/>
       <c r="B111" s="56"/>
       <c r="C111" s="32"/>
       <c r="D111" s="10" t="str">
@@ -16180,7 +16238,7 @@
       </c>
     </row>
     <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="112"/>
+      <c r="A112" s="111"/>
       <c r="B112" s="56"/>
       <c r="C112" s="32"/>
       <c r="D112" s="10" t="str">
@@ -16202,7 +16260,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="112"/>
+      <c r="A113" s="111"/>
       <c r="B113" s="56"/>
       <c r="C113" s="32"/>
       <c r="D113" s="10" t="str">
@@ -16224,7 +16282,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="112"/>
+      <c r="A114" s="111"/>
       <c r="B114" s="56"/>
       <c r="C114" s="32"/>
       <c r="D114" s="10" t="str">
@@ -16246,7 +16304,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="112"/>
+      <c r="A115" s="111"/>
       <c r="B115" s="56"/>
       <c r="C115" s="32"/>
       <c r="D115" s="10" t="str">
@@ -16268,7 +16326,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="112"/>
+      <c r="A116" s="111"/>
       <c r="B116" s="56"/>
       <c r="C116" s="32"/>
       <c r="D116" s="10" t="str">
@@ -16290,7 +16348,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="112"/>
+      <c r="A117" s="111"/>
       <c r="B117" s="56"/>
       <c r="C117" s="32"/>
       <c r="D117" s="10" t="str">
@@ -16312,7 +16370,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="112"/>
+      <c r="A118" s="111"/>
       <c r="B118" s="56"/>
       <c r="C118" s="32"/>
       <c r="D118" s="10" t="str">
@@ -16334,7 +16392,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="112"/>
+      <c r="A119" s="111"/>
       <c r="B119" s="56"/>
       <c r="C119" s="32"/>
       <c r="D119" s="10" t="str">
@@ -16354,7 +16412,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="112"/>
+      <c r="A120" s="111"/>
       <c r="B120" s="56"/>
       <c r="C120" s="32"/>
       <c r="D120" s="10" t="str">
@@ -16368,7 +16426,7 @@
       <c r="I120" s="49"/>
     </row>
     <row r="121" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="112"/>
+      <c r="A121" s="111"/>
       <c r="B121" s="56"/>
       <c r="C121" s="32"/>
       <c r="D121" s="10" t="str">
@@ -16382,7 +16440,7 @@
       <c r="I121" s="50"/>
     </row>
     <row r="122" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="112"/>
+      <c r="A122" s="111"/>
       <c r="B122" s="56"/>
       <c r="C122" s="32"/>
       <c r="D122" s="10" t="str">
@@ -16401,47 +16459,47 @@
       </c>
     </row>
     <row r="123" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="112"/>
+      <c r="A123" s="111"/>
       <c r="B123" s="56"/>
       <c r="C123" s="32"/>
       <c r="D123" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E123" s="109" t="str">
+      <c r="E123" s="113" t="str">
         <f>IF(F119&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F123" s="110"/>
-      <c r="G123" s="110"/>
-      <c r="H123" s="110"/>
+      <c r="F123" s="114"/>
+      <c r="G123" s="114"/>
+      <c r="H123" s="114"/>
       <c r="I123" s="12" t="str">
         <f>IF(F119&lt;&gt;"",SUM(F110:F119),"")</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="112"/>
+      <c r="A124" s="111"/>
       <c r="B124" s="56"/>
       <c r="C124" s="32"/>
       <c r="D124" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E124" s="114" t="str">
+      <c r="E124" s="115" t="str">
         <f>IF(F119&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F124" s="115"/>
-      <c r="G124" s="115"/>
-      <c r="H124" s="115"/>
+      <c r="F124" s="116"/>
+      <c r="G124" s="116"/>
+      <c r="H124" s="116"/>
       <c r="I124" s="16" t="str">
         <f>IF(F119&lt;&gt;"",AB111,"")</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="112"/>
+      <c r="A125" s="111"/>
       <c r="B125" s="34"/>
       <c r="C125" s="58"/>
       <c r="D125" s="10" t="str">
@@ -16458,7 +16516,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="112"/>
+      <c r="A126" s="111"/>
       <c r="B126" s="34"/>
       <c r="C126" s="32"/>
       <c r="D126" s="10" t="str">
@@ -16472,7 +16530,7 @@
       <c r="I126" s="50"/>
     </row>
     <row r="127" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="112"/>
+      <c r="A127" s="111"/>
       <c r="B127" s="34"/>
       <c r="C127" s="32"/>
       <c r="D127" s="10" t="str">
@@ -16486,7 +16544,7 @@
       <c r="I127" s="50"/>
     </row>
     <row r="128" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="112"/>
+      <c r="A128" s="111"/>
       <c r="B128" s="34"/>
       <c r="C128" s="32"/>
       <c r="D128" s="10" t="str">
@@ -16500,7 +16558,7 @@
       <c r="I128" s="50"/>
     </row>
     <row r="129" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="113"/>
+      <c r="A129" s="112"/>
       <c r="B129" s="34"/>
       <c r="C129" s="32"/>
       <c r="D129" s="11" t="str">
@@ -16520,19 +16578,19 @@
     </row>
     <row r="130" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="43"/>
-      <c r="B130" s="117" t="s">
+      <c r="B130" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C130" s="117"/>
-      <c r="D130" s="117"/>
-      <c r="E130" s="117"/>
-      <c r="F130" s="117"/>
-      <c r="G130" s="117"/>
-      <c r="H130" s="117"/>
-      <c r="I130" s="117"/>
-      <c r="J130" s="117"/>
-      <c r="K130" s="117"/>
-      <c r="L130" s="117"/>
+      <c r="C130" s="107"/>
+      <c r="D130" s="107"/>
+      <c r="E130" s="107"/>
+      <c r="F130" s="107"/>
+      <c r="G130" s="107"/>
+      <c r="H130" s="107"/>
+      <c r="I130" s="107"/>
+      <c r="J130" s="107"/>
+      <c r="K130" s="107"/>
+      <c r="L130" s="107"/>
       <c r="M130" s="44"/>
       <c r="N130" s="44"/>
       <c r="O130" s="44"/>
@@ -16543,17 +16601,17 @@
     </row>
     <row r="131" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="43"/>
-      <c r="B131" s="117"/>
-      <c r="C131" s="117"/>
-      <c r="D131" s="117"/>
-      <c r="E131" s="117"/>
-      <c r="F131" s="117"/>
-      <c r="G131" s="117"/>
-      <c r="H131" s="117"/>
-      <c r="I131" s="117"/>
-      <c r="J131" s="117"/>
-      <c r="K131" s="117"/>
-      <c r="L131" s="117"/>
+      <c r="B131" s="107"/>
+      <c r="C131" s="107"/>
+      <c r="D131" s="107"/>
+      <c r="E131" s="107"/>
+      <c r="F131" s="107"/>
+      <c r="G131" s="107"/>
+      <c r="H131" s="107"/>
+      <c r="I131" s="107"/>
+      <c r="J131" s="107"/>
+      <c r="K131" s="107"/>
+      <c r="L131" s="107"/>
       <c r="M131" s="44"/>
       <c r="N131" s="44"/>
       <c r="O131" s="44"/>
@@ -16569,10 +16627,10 @@
       <c r="D132" s="44"/>
       <c r="E132" s="44"/>
       <c r="F132" s="44"/>
-      <c r="G132" s="107" t="s">
+      <c r="G132" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H132" s="108"/>
+      <c r="H132" s="109"/>
       <c r="I132" s="45"/>
       <c r="J132" s="44"/>
       <c r="K132" s="44"/>
@@ -16642,7 +16700,7 @@
       <c r="S134" s="44"/>
     </row>
     <row r="135" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="111" t="s">
+      <c r="A135" s="110" t="s">
         <v>27</v>
       </c>
       <c r="B135" s="57"/>
@@ -16672,7 +16730,7 @@
       </c>
     </row>
     <row r="136" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="112"/>
+      <c r="A136" s="111"/>
       <c r="B136" s="56"/>
       <c r="C136" s="32"/>
       <c r="D136" s="10" t="str">
@@ -16704,7 +16762,7 @@
       </c>
     </row>
     <row r="137" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="112"/>
+      <c r="A137" s="111"/>
       <c r="B137" s="56"/>
       <c r="C137" s="32"/>
       <c r="D137" s="10" t="str">
@@ -16726,7 +16784,7 @@
       </c>
     </row>
     <row r="138" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="112"/>
+      <c r="A138" s="111"/>
       <c r="B138" s="56"/>
       <c r="C138" s="32"/>
       <c r="D138" s="10" t="str">
@@ -16748,7 +16806,7 @@
       </c>
     </row>
     <row r="139" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="112"/>
+      <c r="A139" s="111"/>
       <c r="B139" s="56"/>
       <c r="C139" s="32"/>
       <c r="D139" s="10" t="str">
@@ -16770,7 +16828,7 @@
       </c>
     </row>
     <row r="140" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="112"/>
+      <c r="A140" s="111"/>
       <c r="B140" s="56"/>
       <c r="C140" s="32"/>
       <c r="D140" s="10" t="str">
@@ -16792,7 +16850,7 @@
       </c>
     </row>
     <row r="141" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="112"/>
+      <c r="A141" s="111"/>
       <c r="B141" s="56"/>
       <c r="C141" s="32"/>
       <c r="D141" s="10" t="str">
@@ -16814,7 +16872,7 @@
       </c>
     </row>
     <row r="142" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="112"/>
+      <c r="A142" s="111"/>
       <c r="B142" s="56"/>
       <c r="C142" s="32"/>
       <c r="D142" s="10" t="str">
@@ -16836,7 +16894,7 @@
       </c>
     </row>
     <row r="143" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="112"/>
+      <c r="A143" s="111"/>
       <c r="B143" s="56"/>
       <c r="C143" s="32"/>
       <c r="D143" s="10" t="str">
@@ -16858,7 +16916,7 @@
       </c>
     </row>
     <row r="144" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="112"/>
+      <c r="A144" s="111"/>
       <c r="B144" s="56"/>
       <c r="C144" s="32"/>
       <c r="D144" s="10" t="str">
@@ -16878,7 +16936,7 @@
       </c>
     </row>
     <row r="145" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="112"/>
+      <c r="A145" s="111"/>
       <c r="B145" s="56"/>
       <c r="C145" s="32"/>
       <c r="D145" s="10" t="str">
@@ -16892,7 +16950,7 @@
       <c r="I145" s="49"/>
     </row>
     <row r="146" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="112"/>
+      <c r="A146" s="111"/>
       <c r="B146" s="56"/>
       <c r="C146" s="32"/>
       <c r="D146" s="10" t="str">
@@ -16906,7 +16964,7 @@
       <c r="I146" s="50"/>
     </row>
     <row r="147" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="112"/>
+      <c r="A147" s="111"/>
       <c r="B147" s="56"/>
       <c r="C147" s="32"/>
       <c r="D147" s="10" t="str">
@@ -16925,47 +16983,47 @@
       </c>
     </row>
     <row r="148" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="112"/>
+      <c r="A148" s="111"/>
       <c r="B148" s="56"/>
       <c r="C148" s="32"/>
       <c r="D148" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E148" s="109" t="str">
+      <c r="E148" s="113" t="str">
         <f>IF(F144&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F148" s="110"/>
-      <c r="G148" s="110"/>
-      <c r="H148" s="110"/>
+      <c r="F148" s="114"/>
+      <c r="G148" s="114"/>
+      <c r="H148" s="114"/>
       <c r="I148" s="12" t="str">
         <f>IF(F144&lt;&gt;"",SUM(F135:F144),"")</f>
         <v/>
       </c>
     </row>
     <row r="149" spans="1:27" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="112"/>
+      <c r="A149" s="111"/>
       <c r="B149" s="56"/>
       <c r="C149" s="32"/>
       <c r="D149" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E149" s="114" t="str">
+      <c r="E149" s="115" t="str">
         <f>IF(F144&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F149" s="115"/>
-      <c r="G149" s="115"/>
-      <c r="H149" s="115"/>
+      <c r="F149" s="116"/>
+      <c r="G149" s="116"/>
+      <c r="H149" s="116"/>
       <c r="I149" s="16" t="str">
         <f>IF(F144&lt;&gt;"",AB136,"")</f>
         <v/>
       </c>
     </row>
     <row r="150" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="112"/>
+      <c r="A150" s="111"/>
       <c r="B150" s="56"/>
       <c r="C150" s="32"/>
       <c r="D150" s="10" t="str">
@@ -16982,7 +17040,7 @@
       </c>
     </row>
     <row r="151" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="112"/>
+      <c r="A151" s="111"/>
       <c r="B151" s="34"/>
       <c r="C151" s="32"/>
       <c r="D151" s="10" t="str">
@@ -16996,7 +17054,7 @@
       <c r="I151" s="50"/>
     </row>
     <row r="152" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="112"/>
+      <c r="A152" s="111"/>
       <c r="B152" s="34"/>
       <c r="C152" s="32"/>
       <c r="D152" s="10" t="str">
@@ -17010,7 +17068,7 @@
       <c r="I152" s="50"/>
     </row>
     <row r="153" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="112"/>
+      <c r="A153" s="111"/>
       <c r="B153" s="34"/>
       <c r="C153" s="32"/>
       <c r="D153" s="10" t="str">
@@ -17024,7 +17082,7 @@
       <c r="I153" s="50"/>
     </row>
     <row r="154" spans="1:27" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="113"/>
+      <c r="A154" s="112"/>
       <c r="B154" s="34"/>
       <c r="C154" s="32"/>
       <c r="D154" s="11" t="str">
@@ -17044,19 +17102,19 @@
     </row>
     <row r="155" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="43"/>
-      <c r="B155" s="117" t="s">
+      <c r="B155" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C155" s="117"/>
-      <c r="D155" s="117"/>
-      <c r="E155" s="117"/>
-      <c r="F155" s="117"/>
-      <c r="G155" s="117"/>
-      <c r="H155" s="117"/>
-      <c r="I155" s="117"/>
-      <c r="J155" s="117"/>
-      <c r="K155" s="117"/>
-      <c r="L155" s="117"/>
+      <c r="C155" s="107"/>
+      <c r="D155" s="107"/>
+      <c r="E155" s="107"/>
+      <c r="F155" s="107"/>
+      <c r="G155" s="107"/>
+      <c r="H155" s="107"/>
+      <c r="I155" s="107"/>
+      <c r="J155" s="107"/>
+      <c r="K155" s="107"/>
+      <c r="L155" s="107"/>
       <c r="M155" s="44"/>
       <c r="N155" s="44"/>
       <c r="O155" s="44"/>
@@ -17067,17 +17125,17 @@
     </row>
     <row r="156" spans="1:27" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="43"/>
-      <c r="B156" s="117"/>
-      <c r="C156" s="117"/>
-      <c r="D156" s="117"/>
-      <c r="E156" s="117"/>
-      <c r="F156" s="117"/>
-      <c r="G156" s="117"/>
-      <c r="H156" s="117"/>
-      <c r="I156" s="117"/>
-      <c r="J156" s="117"/>
-      <c r="K156" s="117"/>
-      <c r="L156" s="117"/>
+      <c r="B156" s="107"/>
+      <c r="C156" s="107"/>
+      <c r="D156" s="107"/>
+      <c r="E156" s="107"/>
+      <c r="F156" s="107"/>
+      <c r="G156" s="107"/>
+      <c r="H156" s="107"/>
+      <c r="I156" s="107"/>
+      <c r="J156" s="107"/>
+      <c r="K156" s="107"/>
+      <c r="L156" s="107"/>
       <c r="M156" s="44"/>
       <c r="N156" s="44"/>
       <c r="O156" s="44"/>
@@ -17093,10 +17151,10 @@
       <c r="D157" s="44"/>
       <c r="E157" s="44"/>
       <c r="F157" s="44"/>
-      <c r="G157" s="107" t="s">
+      <c r="G157" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H157" s="108"/>
+      <c r="H157" s="109"/>
       <c r="I157" s="45"/>
       <c r="J157" s="44"/>
       <c r="K157" s="44"/>
@@ -17166,7 +17224,7 @@
       <c r="S159" s="44"/>
     </row>
     <row r="160" spans="1:27" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="111" t="s">
+      <c r="A160" s="110" t="s">
         <v>28</v>
       </c>
       <c r="B160" s="56"/>
@@ -17196,7 +17254,7 @@
       </c>
     </row>
     <row r="161" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="112"/>
+      <c r="A161" s="111"/>
       <c r="B161" s="56"/>
       <c r="C161" s="32"/>
       <c r="D161" s="10" t="str">
@@ -17228,7 +17286,7 @@
       </c>
     </row>
     <row r="162" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="112"/>
+      <c r="A162" s="111"/>
       <c r="B162" s="56"/>
       <c r="C162" s="32"/>
       <c r="D162" s="10" t="str">
@@ -17250,7 +17308,7 @@
       </c>
     </row>
     <row r="163" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="112"/>
+      <c r="A163" s="111"/>
       <c r="B163" s="56"/>
       <c r="C163" s="32"/>
       <c r="D163" s="10" t="str">
@@ -17272,7 +17330,7 @@
       </c>
     </row>
     <row r="164" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="112"/>
+      <c r="A164" s="111"/>
       <c r="B164" s="56"/>
       <c r="C164" s="32"/>
       <c r="D164" s="10" t="str">
@@ -17294,7 +17352,7 @@
       </c>
     </row>
     <row r="165" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="112"/>
+      <c r="A165" s="111"/>
       <c r="B165" s="56"/>
       <c r="C165" s="32"/>
       <c r="D165" s="10" t="str">
@@ -17316,7 +17374,7 @@
       </c>
     </row>
     <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="112"/>
+      <c r="A166" s="111"/>
       <c r="B166" s="56"/>
       <c r="C166" s="32"/>
       <c r="D166" s="10" t="str">
@@ -17338,7 +17396,7 @@
       </c>
     </row>
     <row r="167" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="112"/>
+      <c r="A167" s="111"/>
       <c r="B167" s="56"/>
       <c r="C167" s="32"/>
       <c r="D167" s="10" t="str">
@@ -17360,7 +17418,7 @@
       </c>
     </row>
     <row r="168" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="112"/>
+      <c r="A168" s="111"/>
       <c r="B168" s="56"/>
       <c r="C168" s="32"/>
       <c r="D168" s="10" t="str">
@@ -17382,7 +17440,7 @@
       </c>
     </row>
     <row r="169" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="112"/>
+      <c r="A169" s="111"/>
       <c r="B169" s="56"/>
       <c r="C169" s="32"/>
       <c r="D169" s="10" t="str">
@@ -17402,7 +17460,7 @@
       </c>
     </row>
     <row r="170" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="112"/>
+      <c r="A170" s="111"/>
       <c r="B170" s="56"/>
       <c r="C170" s="32"/>
       <c r="D170" s="10" t="str">
@@ -17416,7 +17474,7 @@
       <c r="I170" s="49"/>
     </row>
     <row r="171" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="112"/>
+      <c r="A171" s="111"/>
       <c r="B171" s="56"/>
       <c r="C171" s="32"/>
       <c r="D171" s="10" t="str">
@@ -17430,7 +17488,7 @@
       <c r="I171" s="50"/>
     </row>
     <row r="172" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="112"/>
+      <c r="A172" s="111"/>
       <c r="B172" s="56"/>
       <c r="C172" s="32"/>
       <c r="D172" s="10" t="str">
@@ -17449,47 +17507,47 @@
       </c>
     </row>
     <row r="173" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="112"/>
+      <c r="A173" s="111"/>
       <c r="B173" s="56"/>
       <c r="C173" s="32"/>
       <c r="D173" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E173" s="109" t="str">
+      <c r="E173" s="113" t="str">
         <f>IF(F169&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F173" s="110"/>
-      <c r="G173" s="110"/>
-      <c r="H173" s="110"/>
+      <c r="F173" s="114"/>
+      <c r="G173" s="114"/>
+      <c r="H173" s="114"/>
       <c r="I173" s="12" t="str">
         <f>IF(F169&lt;&gt;"",SUM(F160:F169),"")</f>
         <v/>
       </c>
     </row>
     <row r="174" spans="1:28" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="112"/>
+      <c r="A174" s="111"/>
       <c r="B174" s="56"/>
       <c r="C174" s="32"/>
       <c r="D174" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E174" s="114" t="str">
+      <c r="E174" s="115" t="str">
         <f>IF(F169&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F174" s="115"/>
-      <c r="G174" s="115"/>
-      <c r="H174" s="115"/>
+      <c r="F174" s="116"/>
+      <c r="G174" s="116"/>
+      <c r="H174" s="116"/>
       <c r="I174" s="16" t="str">
         <f>IF(F169&lt;&gt;"",AB161,"")</f>
         <v/>
       </c>
     </row>
     <row r="175" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="112"/>
+      <c r="A175" s="111"/>
       <c r="B175" s="34"/>
       <c r="C175" s="58"/>
       <c r="D175" s="10" t="str">
@@ -17506,7 +17564,7 @@
       </c>
     </row>
     <row r="176" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="112"/>
+      <c r="A176" s="111"/>
       <c r="B176" s="34"/>
       <c r="C176" s="32"/>
       <c r="D176" s="10" t="str">
@@ -17520,7 +17578,7 @@
       <c r="I176" s="50"/>
     </row>
     <row r="177" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="112"/>
+      <c r="A177" s="111"/>
       <c r="B177" s="34"/>
       <c r="C177" s="32"/>
       <c r="D177" s="10" t="str">
@@ -17534,7 +17592,7 @@
       <c r="I177" s="50"/>
     </row>
     <row r="178" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="112"/>
+      <c r="A178" s="111"/>
       <c r="B178" s="34"/>
       <c r="C178" s="32"/>
       <c r="D178" s="10" t="str">
@@ -17548,7 +17606,7 @@
       <c r="I178" s="50"/>
     </row>
     <row r="179" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="113"/>
+      <c r="A179" s="112"/>
       <c r="B179" s="34"/>
       <c r="C179" s="32"/>
       <c r="D179" s="11" t="str">
@@ -17568,19 +17626,19 @@
     </row>
     <row r="180" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="43"/>
-      <c r="B180" s="117" t="s">
+      <c r="B180" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C180" s="117"/>
-      <c r="D180" s="117"/>
-      <c r="E180" s="117"/>
-      <c r="F180" s="117"/>
-      <c r="G180" s="117"/>
-      <c r="H180" s="117"/>
-      <c r="I180" s="117"/>
-      <c r="J180" s="117"/>
-      <c r="K180" s="117"/>
-      <c r="L180" s="117"/>
+      <c r="C180" s="107"/>
+      <c r="D180" s="107"/>
+      <c r="E180" s="107"/>
+      <c r="F180" s="107"/>
+      <c r="G180" s="107"/>
+      <c r="H180" s="107"/>
+      <c r="I180" s="107"/>
+      <c r="J180" s="107"/>
+      <c r="K180" s="107"/>
+      <c r="L180" s="107"/>
       <c r="M180" s="44"/>
       <c r="N180" s="44"/>
       <c r="O180" s="44"/>
@@ -17591,17 +17649,17 @@
     </row>
     <row r="181" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="43"/>
-      <c r="B181" s="117"/>
-      <c r="C181" s="117"/>
-      <c r="D181" s="117"/>
-      <c r="E181" s="117"/>
-      <c r="F181" s="117"/>
-      <c r="G181" s="117"/>
-      <c r="H181" s="117"/>
-      <c r="I181" s="117"/>
-      <c r="J181" s="117"/>
-      <c r="K181" s="117"/>
-      <c r="L181" s="117"/>
+      <c r="B181" s="107"/>
+      <c r="C181" s="107"/>
+      <c r="D181" s="107"/>
+      <c r="E181" s="107"/>
+      <c r="F181" s="107"/>
+      <c r="G181" s="107"/>
+      <c r="H181" s="107"/>
+      <c r="I181" s="107"/>
+      <c r="J181" s="107"/>
+      <c r="K181" s="107"/>
+      <c r="L181" s="107"/>
       <c r="M181" s="44"/>
       <c r="N181" s="44"/>
       <c r="O181" s="44"/>
@@ -17617,10 +17675,10 @@
       <c r="D182" s="44"/>
       <c r="E182" s="44"/>
       <c r="F182" s="44"/>
-      <c r="G182" s="107" t="s">
+      <c r="G182" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="H182" s="108"/>
+      <c r="H182" s="109"/>
       <c r="I182" s="45"/>
       <c r="J182" s="44"/>
       <c r="K182" s="44"/>
@@ -17690,7 +17748,7 @@
       <c r="S184" s="44"/>
     </row>
     <row r="185" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="111" t="s">
+      <c r="A185" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B185" s="56"/>
@@ -17720,7 +17778,7 @@
       </c>
     </row>
     <row r="186" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="112"/>
+      <c r="A186" s="111"/>
       <c r="B186" s="56"/>
       <c r="C186" s="32"/>
       <c r="D186" s="10" t="str">
@@ -17752,7 +17810,7 @@
       </c>
     </row>
     <row r="187" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="112"/>
+      <c r="A187" s="111"/>
       <c r="B187" s="56"/>
       <c r="C187" s="32"/>
       <c r="D187" s="10" t="str">
@@ -17774,7 +17832,7 @@
       </c>
     </row>
     <row r="188" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="112"/>
+      <c r="A188" s="111"/>
       <c r="B188" s="56"/>
       <c r="C188" s="32"/>
       <c r="D188" s="10" t="str">
@@ -17796,7 +17854,7 @@
       </c>
     </row>
     <row r="189" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="112"/>
+      <c r="A189" s="111"/>
       <c r="B189" s="56"/>
       <c r="C189" s="32"/>
       <c r="D189" s="10" t="str">
@@ -17818,7 +17876,7 @@
       </c>
     </row>
     <row r="190" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="112"/>
+      <c r="A190" s="111"/>
       <c r="B190" s="56"/>
       <c r="C190" s="32"/>
       <c r="D190" s="10" t="str">
@@ -17840,7 +17898,7 @@
       </c>
     </row>
     <row r="191" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="112"/>
+      <c r="A191" s="111"/>
       <c r="B191" s="56"/>
       <c r="C191" s="32"/>
       <c r="D191" s="10" t="str">
@@ -17862,7 +17920,7 @@
       </c>
     </row>
     <row r="192" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="112"/>
+      <c r="A192" s="111"/>
       <c r="B192" s="56"/>
       <c r="C192" s="32"/>
       <c r="D192" s="10" t="str">
@@ -17884,7 +17942,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="112"/>
+      <c r="A193" s="111"/>
       <c r="B193" s="56"/>
       <c r="C193" s="32"/>
       <c r="D193" s="10" t="str">
@@ -17906,7 +17964,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="112"/>
+      <c r="A194" s="111"/>
       <c r="B194" s="56"/>
       <c r="C194" s="32"/>
       <c r="D194" s="10" t="str">
@@ -17926,7 +17984,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="112"/>
+      <c r="A195" s="111"/>
       <c r="B195" s="56"/>
       <c r="C195" s="32"/>
       <c r="D195" s="10" t="str">
@@ -17940,7 +17998,7 @@
       <c r="I195" s="49"/>
     </row>
     <row r="196" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="112"/>
+      <c r="A196" s="111"/>
       <c r="B196" s="56"/>
       <c r="C196" s="32"/>
       <c r="D196" s="10" t="str">
@@ -17954,7 +18012,7 @@
       <c r="I196" s="50"/>
     </row>
     <row r="197" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="112"/>
+      <c r="A197" s="111"/>
       <c r="B197" s="56"/>
       <c r="C197" s="32"/>
       <c r="D197" s="10" t="str">
@@ -17973,47 +18031,47 @@
       </c>
     </row>
     <row r="198" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="112"/>
+      <c r="A198" s="111"/>
       <c r="B198" s="56"/>
       <c r="C198" s="32"/>
       <c r="D198" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E198" s="109" t="str">
+      <c r="E198" s="113" t="str">
         <f>IF(F194&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F198" s="110"/>
-      <c r="G198" s="110"/>
-      <c r="H198" s="110"/>
+      <c r="F198" s="114"/>
+      <c r="G198" s="114"/>
+      <c r="H198" s="114"/>
       <c r="I198" s="12" t="str">
         <f>IF(F194&lt;&gt;"",SUM(F185:F194),"")</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="112"/>
+      <c r="A199" s="111"/>
       <c r="B199" s="56"/>
       <c r="C199" s="32"/>
       <c r="D199" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E199" s="114" t="str">
+      <c r="E199" s="115" t="str">
         <f>IF(F194&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F199" s="115"/>
-      <c r="G199" s="115"/>
-      <c r="H199" s="115"/>
+      <c r="F199" s="116"/>
+      <c r="G199" s="116"/>
+      <c r="H199" s="116"/>
       <c r="I199" s="16" t="str">
         <f>IF(F194&lt;&gt;"",AB186,"")</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="112"/>
+      <c r="A200" s="111"/>
       <c r="B200" s="56"/>
       <c r="C200" s="32"/>
       <c r="D200" s="10" t="str">
@@ -18030,7 +18088,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="112"/>
+      <c r="A201" s="111"/>
       <c r="B201" s="34"/>
       <c r="C201" s="32"/>
       <c r="D201" s="10" t="str">
@@ -18044,7 +18102,7 @@
       <c r="I201" s="50"/>
     </row>
     <row r="202" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="112"/>
+      <c r="A202" s="111"/>
       <c r="B202" s="34"/>
       <c r="C202" s="32"/>
       <c r="D202" s="10" t="str">
@@ -18058,7 +18116,7 @@
       <c r="I202" s="50"/>
     </row>
     <row r="203" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="112"/>
+      <c r="A203" s="111"/>
       <c r="B203" s="34"/>
       <c r="C203" s="32"/>
       <c r="D203" s="10" t="str">
@@ -18072,7 +18130,7 @@
       <c r="I203" s="50"/>
     </row>
     <row r="204" spans="1:9" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="113"/>
+      <c r="A204" s="112"/>
       <c r="B204" s="34"/>
       <c r="C204" s="32"/>
       <c r="D204" s="11" t="str">
@@ -18093,46 +18151,46 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xvw55rBl+8QauwDbqXfPTEJvlFDUCVQW9eBF4D1fCPDMzZnBE0eg23U/adjRGpGtDkno/gEp3o8WBaDX9CrDpg==" saltValue="kVJ3wM2y/GPu2SWvmMPnkg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="40">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="A6:A26"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="B27:L28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A32:A52"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="B53:L54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A58:A78"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="B79:L80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="A84:A104"/>
+    <mergeCell ref="E98:H98"/>
+    <mergeCell ref="E99:H99"/>
+    <mergeCell ref="B105:L106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="A110:A129"/>
+    <mergeCell ref="E123:H123"/>
+    <mergeCell ref="E124:H124"/>
+    <mergeCell ref="B130:L131"/>
+    <mergeCell ref="G132:H132"/>
+    <mergeCell ref="A135:A154"/>
+    <mergeCell ref="E148:H148"/>
+    <mergeCell ref="E149:H149"/>
+    <mergeCell ref="B155:L156"/>
+    <mergeCell ref="G157:H157"/>
+    <mergeCell ref="A160:A179"/>
+    <mergeCell ref="E173:H173"/>
+    <mergeCell ref="E174:H174"/>
     <mergeCell ref="B180:L181"/>
     <mergeCell ref="G182:H182"/>
     <mergeCell ref="A185:A204"/>
     <mergeCell ref="E198:H198"/>
     <mergeCell ref="E199:H199"/>
-    <mergeCell ref="B155:L156"/>
-    <mergeCell ref="G157:H157"/>
-    <mergeCell ref="A160:A179"/>
-    <mergeCell ref="E173:H173"/>
-    <mergeCell ref="E174:H174"/>
-    <mergeCell ref="B130:L131"/>
-    <mergeCell ref="G132:H132"/>
-    <mergeCell ref="A135:A154"/>
-    <mergeCell ref="E148:H148"/>
-    <mergeCell ref="E149:H149"/>
-    <mergeCell ref="B105:L106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="A110:A129"/>
-    <mergeCell ref="E123:H123"/>
-    <mergeCell ref="E124:H124"/>
-    <mergeCell ref="B79:L80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="A84:A104"/>
-    <mergeCell ref="E98:H98"/>
-    <mergeCell ref="E99:H99"/>
-    <mergeCell ref="B53:L54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A58:A78"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="B27:L28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A32:A52"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="A6:A26"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="B1:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="I205:I1048576 I3:I6 I8:I16">
     <cfRule type="cellIs" dxfId="35" priority="57" operator="lessThan">
@@ -18322,6 +18380,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -18370,32 +18443,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18409,15 +18466,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc: Personal Burndownchart Iwan
Doc: Personal Burndownchart Iwan
</commit_message>
<xml_diff>
--- a/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
+++ b/Documentatie/Persoonlijke Burndowncharts/Iwan van der Bruggen - Burndownchart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leerling Iwan" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t>Omschrijving taak</t>
   </si>
@@ -835,9 +835,6 @@
     <t>Team Leader</t>
   </si>
   <si>
-    <t>Bord opnmaken</t>
-  </si>
-  <si>
     <t>User stories en taken prioriseren</t>
   </si>
   <si>
@@ -851,6 +848,39 @@
   </si>
   <si>
     <t>Persoonlijke burndown charts maken</t>
+  </si>
+  <si>
+    <t>Handleiding</t>
+  </si>
+  <si>
+    <t>Handleiding Open dag</t>
+  </si>
+  <si>
+    <t>Klassendiagram maken</t>
+  </si>
+  <si>
+    <t>Bord opmaken</t>
+  </si>
+  <si>
+    <t>Tasks maken</t>
+  </si>
+  <si>
+    <t>Teamleden ondersteunen</t>
+  </si>
+  <si>
+    <t>Controleren van taken volgens DoD</t>
+  </si>
+  <si>
+    <t>Game Design Document</t>
+  </si>
+  <si>
+    <t>Andere geholpen met documentatie</t>
+  </si>
+  <si>
+    <t>Andere ondersteunt</t>
+  </si>
+  <si>
+    <t>Tasks gecontroleerd volgens de DoD</t>
   </si>
 </sst>
 </file>
@@ -1950,14 +1980,19 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1967,14 +2002,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1987,6 +2014,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2998,34 +3028,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3112,37 +3142,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,37 +4120,37 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>19.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>17.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>13.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8.8000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.6000000000000041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4.4000000000000039</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.2000000000000037</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3.5527136788005009E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4204,37 +4234,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6317,13 +6347,13 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13528,8 +13558,8 @@
   </sheetPr>
   <dimension ref="A1:AI204"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13559,35 +13589,35 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
       <c r="M1" s="44"/>
       <c r="S1" s="44"/>
     </row>
     <row r="2" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
       <c r="M2" s="44"/>
       <c r="S2" s="44"/>
       <c r="AF2" s="82" t="s">
@@ -13601,10 +13631,10 @@
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="109"/>
+      <c r="H3" s="108"/>
       <c r="I3" s="45"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
@@ -13639,7 +13669,7 @@
       </c>
       <c r="AG4" s="80">
         <f ca="1">TODAY()</f>
-        <v>43108</v>
+        <v>43119</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13694,7 +13724,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="111" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -13750,7 +13780,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="34" t="s">
         <v>59</v>
       </c>
@@ -13784,7 +13814,7 @@
       <c r="AI7" s="87"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="111"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="34" t="s">
         <v>60</v>
       </c>
@@ -13825,27 +13855,27 @@
       </c>
       <c r="AE8" s="78">
         <f>I45</f>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="78" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="78">
         <f>I46</f>
-        <v/>
-      </c>
-      <c r="AG8" s="78" t="str">
+        <v>20</v>
+      </c>
+      <c r="AG8" s="78">
         <f>I47</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="AH8" s="79" t="str">
         <f t="shared" ref="AH8:AH10" si="2">IF(AF8="","",IF(AF8&lt;AG8,"Te weinig","Keurig"))</f>
-        <v/>
-      </c>
-      <c r="AI8" s="87" t="str">
+        <v>Keurig</v>
+      </c>
+      <c r="AI8" s="87">
         <f>H52</f>
-        <v/>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="34" t="s">
         <v>61</v>
       </c>
@@ -13899,7 +13929,7 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="111"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="34" t="s">
         <v>63</v>
       </c>
@@ -13933,27 +13963,27 @@
       </c>
       <c r="AE10" s="89">
         <f>I97</f>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="89" t="str">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AF10" s="89">
         <f>I98</f>
-        <v/>
-      </c>
-      <c r="AG10" s="89" t="str">
+        <v>22</v>
+      </c>
+      <c r="AG10" s="89">
         <f>I99</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="AH10" s="90" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AI10" s="91" t="str">
+        <v>Keurig</v>
+      </c>
+      <c r="AI10" s="91">
         <f>H104</f>
-        <v/>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="111"/>
+      <c r="A11" s="112"/>
       <c r="B11" s="34"/>
       <c r="C11" s="65"/>
       <c r="D11" s="61" t="str">
@@ -13980,7 +14010,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
+      <c r="A12" s="112"/>
       <c r="B12" s="34"/>
       <c r="C12" s="65"/>
       <c r="D12" s="61" t="str">
@@ -14007,7 +14037,7 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
+      <c r="A13" s="112"/>
       <c r="B13" s="34"/>
       <c r="C13" s="65"/>
       <c r="D13" s="61" t="str">
@@ -14034,7 +14064,7 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="111"/>
+      <c r="A14" s="112"/>
       <c r="B14" s="34"/>
       <c r="C14" s="65"/>
       <c r="D14" s="61" t="str">
@@ -14061,7 +14091,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="112"/>
       <c r="B15" s="34"/>
       <c r="C15" s="65"/>
       <c r="D15" s="61" t="str">
@@ -14088,7 +14118,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="34"/>
       <c r="C16" s="65"/>
       <c r="D16" s="61" t="str">
@@ -14115,7 +14145,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
+      <c r="A17" s="112"/>
       <c r="B17" s="34"/>
       <c r="C17" s="65"/>
       <c r="D17" s="61" t="str">
@@ -14129,7 +14159,7 @@
       <c r="I17" s="50"/>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="111"/>
+      <c r="A18" s="112"/>
       <c r="B18" s="34"/>
       <c r="C18" s="65"/>
       <c r="D18" s="61" t="str">
@@ -14143,7 +14173,7 @@
       <c r="I18" s="50"/>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
+      <c r="A19" s="112"/>
       <c r="B19" s="34"/>
       <c r="C19" s="65"/>
       <c r="D19" s="61" t="str">
@@ -14162,47 +14192,47 @@
       </c>
     </row>
     <row r="20" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="111"/>
+      <c r="A20" s="112"/>
       <c r="B20" s="34"/>
       <c r="C20" s="65"/>
       <c r="D20" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E20" s="113" t="str">
+      <c r="E20" s="109" t="str">
         <f>IF(F16&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v># Uren afgetikt aan het eind van de sprint:</v>
       </c>
-      <c r="F20" s="114"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="114"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
       <c r="I20" s="12">
         <f>IF(F16&lt;&gt;"",SUM(F6:F16),"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="111"/>
+      <c r="A21" s="112"/>
       <c r="B21" s="64"/>
       <c r="C21" s="65"/>
       <c r="D21" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E21" s="115" t="str">
+      <c r="E21" s="114" t="str">
         <f>IF(F16&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v>Dit moesten er zijn:</v>
       </c>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
       <c r="I21" s="16">
         <f>IF(F16&lt;&gt;"",AB8,"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
+      <c r="A22" s="112"/>
       <c r="B22" s="64"/>
       <c r="C22" s="65"/>
       <c r="D22" s="61" t="str">
@@ -14219,7 +14249,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111"/>
+      <c r="A23" s="112"/>
       <c r="B23" s="64"/>
       <c r="C23" s="65"/>
       <c r="D23" s="61" t="str">
@@ -14233,7 +14263,7 @@
       <c r="I23" s="50"/>
     </row>
     <row r="24" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
+      <c r="A24" s="112"/>
       <c r="B24" s="64" t="s">
         <v>62</v>
       </c>
@@ -14249,7 +14279,7 @@
       <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="64" t="s">
         <v>57</v>
       </c>
@@ -14265,7 +14295,7 @@
       <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="66" t="s">
         <v>64</v>
       </c>
@@ -14287,20 +14317,20 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
-      <c r="B27" s="107" t="str">
+      <c r="B27" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
       <c r="M27" s="44"/>
       <c r="N27" s="44"/>
       <c r="O27" s="44"/>
@@ -14311,17 +14341,17 @@
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="117"/>
       <c r="M28" s="44"/>
       <c r="N28" s="44"/>
       <c r="O28" s="44"/>
@@ -14337,10 +14367,10 @@
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
-      <c r="G29" s="108" t="s">
+      <c r="G29" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="109"/>
+      <c r="H29" s="108"/>
       <c r="I29" s="45"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
@@ -14410,11 +14440,15 @@
       <c r="S31" s="44"/>
     </row>
     <row r="32" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="110" t="s">
+      <c r="A32" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="63"/>
+      <c r="B32" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="63">
+        <v>20</v>
+      </c>
       <c r="D32" s="60" t="str">
         <f>IF(C32&lt;&gt;"",IF(AND(C32&lt;&gt;1,C32&lt;&gt;2,C32&lt;&gt;3,C32&lt;&gt;5,C32&lt;&gt;8,C32&lt;&gt;13,C32&lt;&gt;20,C32&lt;&gt;40,C32&lt;&gt;100),"Fout",""),"")</f>
         <v/>
@@ -14427,11 +14461,11 @@
       </c>
       <c r="G32" s="17">
         <f>AB34</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H32" s="20">
         <f>AB34-F32</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I32" s="21">
         <f>G32-H32</f>
@@ -14439,29 +14473,31 @@
       </c>
     </row>
     <row r="33" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="34"/>
       <c r="C33" s="104"/>
       <c r="D33" s="98"/>
       <c r="E33" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="100"/>
+      <c r="F33" s="100">
+        <v>0</v>
+      </c>
       <c r="G33" s="101">
         <f t="shared" ref="G33:G42" si="6">(G32-(AB$34/10))</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="96" t="e">
+        <v>18</v>
+      </c>
+      <c r="H33" s="96">
         <f>IF(F33="",NA(),H32-F33)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I33" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I33" s="22">
         <f t="shared" ref="I33:I36" si="7">IF(F33="","",G33-H33)</f>
-        <v/>
+        <v>-2</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="111"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="64"/>
       <c r="C34" s="68"/>
       <c r="D34" s="61" t="str">
@@ -14471,29 +14507,31 @@
       <c r="E34" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="75"/>
+      <c r="F34" s="75">
+        <v>0</v>
+      </c>
       <c r="G34" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="96" t="e">
+        <v>16</v>
+      </c>
+      <c r="H34" s="96">
         <f>IF(F34="",NA(),H33-F34)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I34" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I34" s="22">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-4</v>
       </c>
       <c r="AA34" t="s">
         <v>3</v>
       </c>
       <c r="AB34">
         <f>SUM(C32:C52)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
+      <c r="A35" s="112"/>
       <c r="B35" s="64"/>
       <c r="C35" s="65"/>
       <c r="D35" s="61" t="str">
@@ -14503,22 +14541,24 @@
       <c r="E35" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="75"/>
+      <c r="F35" s="75">
+        <v>0</v>
+      </c>
       <c r="G35" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="96" t="e">
+        <v>14</v>
+      </c>
+      <c r="H35" s="96">
         <f t="shared" ref="H35:H42" si="9">IF(F35="",NA(),H34-F35)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I35" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I35" s="22">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-6</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="111"/>
+      <c r="A36" s="112"/>
       <c r="B36" s="64"/>
       <c r="C36" s="65"/>
       <c r="D36" s="61" t="str">
@@ -14528,22 +14568,24 @@
       <c r="E36" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="75"/>
+      <c r="F36" s="75">
+        <v>0</v>
+      </c>
       <c r="G36" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="96" t="e">
+        <v>12</v>
+      </c>
+      <c r="H36" s="96">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I36" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I36" s="22">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-8</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
+      <c r="A37" s="112"/>
       <c r="B37" s="64"/>
       <c r="C37" s="65"/>
       <c r="D37" s="61" t="str">
@@ -14553,22 +14595,24 @@
       <c r="E37" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="75"/>
+      <c r="F37" s="75">
+        <v>0</v>
+      </c>
       <c r="G37" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="96" t="e">
+        <v>10</v>
+      </c>
+      <c r="H37" s="96">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I37" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I37" s="22">
         <f>IF(F37="","",G37-H37)</f>
-        <v/>
+        <v>-10</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="111"/>
+      <c r="A38" s="112"/>
       <c r="B38" s="64"/>
       <c r="C38" s="65"/>
       <c r="D38" s="61" t="str">
@@ -14578,22 +14622,24 @@
       <c r="E38" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="75"/>
+      <c r="F38" s="75">
+        <v>0</v>
+      </c>
       <c r="G38" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="96" t="e">
+        <v>8</v>
+      </c>
+      <c r="H38" s="96">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I38" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I38" s="22">
         <f t="shared" ref="I38:I42" si="10">IF(F38="","",G38-H38)</f>
-        <v/>
+        <v>-12</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
+      <c r="A39" s="112"/>
       <c r="B39" s="64"/>
       <c r="C39" s="65"/>
       <c r="D39" s="61" t="str">
@@ -14603,22 +14649,24 @@
       <c r="E39" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="75"/>
+      <c r="F39" s="75">
+        <v>0</v>
+      </c>
       <c r="G39" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H39" s="96" t="e">
+        <v>6</v>
+      </c>
+      <c r="H39" s="96">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I39" s="22" t="str">
+        <v>20</v>
+      </c>
+      <c r="I39" s="22">
         <f t="shared" si="10"/>
-        <v/>
+        <v>-14</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="111"/>
+      <c r="A40" s="112"/>
       <c r="B40" s="64"/>
       <c r="C40" s="65"/>
       <c r="D40" s="61" t="str">
@@ -14628,22 +14676,24 @@
       <c r="E40" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="75"/>
+      <c r="F40" s="75">
+        <v>20</v>
+      </c>
       <c r="G40" s="18">
         <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H40" s="96">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H40" s="96" t="e">
-        <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I40" s="22" t="str">
+      <c r="I40" s="22">
         <f t="shared" si="10"/>
-        <v/>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="64"/>
       <c r="C41" s="65"/>
       <c r="D41" s="61" t="str">
@@ -14653,22 +14703,24 @@
       <c r="E41" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="75"/>
+      <c r="F41" s="75">
+        <v>0</v>
+      </c>
       <c r="G41" s="18">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H41" s="96">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H41" s="96" t="e">
-        <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I41" s="22" t="str">
+      <c r="I41" s="22">
         <f t="shared" si="10"/>
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="111"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="64"/>
       <c r="C42" s="65"/>
       <c r="D42" s="61" t="str">
@@ -14678,22 +14730,24 @@
       <c r="E42" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="76"/>
+      <c r="F42" s="76">
+        <v>0</v>
+      </c>
       <c r="G42" s="19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H42" s="97" t="e">
+      <c r="H42" s="97">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I42" s="77" t="str">
+        <v>0</v>
+      </c>
+      <c r="I42" s="77">
         <f t="shared" si="10"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
+      <c r="A43" s="112"/>
       <c r="B43" s="64"/>
       <c r="C43" s="65"/>
       <c r="D43" s="61" t="str">
@@ -14707,7 +14761,7 @@
       <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="111"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="64"/>
       <c r="C44" s="65"/>
       <c r="D44" s="61" t="str">
@@ -14721,7 +14775,7 @@
       <c r="I44" s="50"/>
     </row>
     <row r="45" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
+      <c r="A45" s="112"/>
       <c r="B45" s="64"/>
       <c r="C45" s="65"/>
       <c r="D45" s="61" t="str">
@@ -14736,51 +14790,51 @@
       </c>
       <c r="I45" s="28">
         <f>AB34/10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="64"/>
       <c r="C46" s="65"/>
       <c r="D46" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E46" s="113" t="str">
+      <c r="E46" s="109" t="str">
         <f>IF(F42&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
-        <v/>
-      </c>
-      <c r="F46" s="114"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="114"/>
-      <c r="I46" s="12" t="str">
+        <v># Uren afgetikt aan het eind van de sprint:</v>
+      </c>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
+      <c r="I46" s="12">
         <f>IF(F42&lt;&gt;"",SUM(F32:F42),"")</f>
-        <v/>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="111"/>
+      <c r="A47" s="112"/>
       <c r="B47" s="64"/>
       <c r="C47" s="65"/>
       <c r="D47" s="61" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E47" s="115" t="str">
+      <c r="E47" s="114" t="str">
         <f>IF(F42&lt;&gt;"","Dit moesten er zijn:","")</f>
-        <v/>
-      </c>
-      <c r="F47" s="116"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="116"/>
-      <c r="I47" s="16" t="str">
+        <v>Dit moesten er zijn:</v>
+      </c>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="16">
         <f>IF(F42&lt;&gt;"",AB34,"")</f>
-        <v/>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="112"/>
       <c r="B48" s="34"/>
       <c r="C48" s="69"/>
       <c r="D48" s="61" t="str">
@@ -14793,11 +14847,11 @@
       <c r="H48" s="47"/>
       <c r="I48" s="51" t="str">
         <f>IF(F42="","",IF(I46&lt;I47,"Dus te weinig.","Keurig"))</f>
-        <v/>
+        <v>Keurig</v>
       </c>
     </row>
     <row r="49" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="112"/>
       <c r="B49" s="34"/>
       <c r="C49" s="65"/>
       <c r="D49" s="61" t="str">
@@ -14811,8 +14865,10 @@
       <c r="I49" s="50"/>
     </row>
     <row r="50" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
-      <c r="B50" s="34"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="C50" s="65"/>
       <c r="D50" s="61" t="str">
         <f t="shared" si="8"/>
@@ -14825,8 +14881,10 @@
       <c r="I50" s="50"/>
     </row>
     <row r="51" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="111"/>
-      <c r="B51" s="34"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="34" t="s">
+        <v>79</v>
+      </c>
       <c r="C51" s="65"/>
       <c r="D51" s="61" t="str">
         <f t="shared" si="8"/>
@@ -14839,8 +14897,10 @@
       <c r="I51" s="50"/>
     </row>
     <row r="52" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="112"/>
-      <c r="B52" s="70"/>
+      <c r="A52" s="113"/>
+      <c r="B52" s="70" t="s">
+        <v>78</v>
+      </c>
       <c r="C52" s="67"/>
       <c r="D52" s="62" t="str">
         <f t="shared" si="8"/>
@@ -14851,28 +14911,28 @@
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
-      <c r="H52" s="26" t="str">
+      <c r="H52" s="26">
         <f>I46</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
-      <c r="B53" s="107" t="str">
+      <c r="B53" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C53" s="107"/>
-      <c r="D53" s="107"/>
-      <c r="E53" s="107"/>
-      <c r="F53" s="107"/>
-      <c r="G53" s="107"/>
-      <c r="H53" s="107"/>
-      <c r="I53" s="107"/>
-      <c r="J53" s="107"/>
-      <c r="K53" s="107"/>
-      <c r="L53" s="107"/>
+      <c r="C53" s="117"/>
+      <c r="D53" s="117"/>
+      <c r="E53" s="117"/>
+      <c r="F53" s="117"/>
+      <c r="G53" s="117"/>
+      <c r="H53" s="117"/>
+      <c r="I53" s="117"/>
+      <c r="J53" s="117"/>
+      <c r="K53" s="117"/>
+      <c r="L53" s="117"/>
       <c r="M53" s="44"/>
       <c r="N53" s="44"/>
       <c r="O53" s="44"/>
@@ -14883,17 +14943,17 @@
     </row>
     <row r="54" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="107"/>
-      <c r="F54" s="107"/>
-      <c r="G54" s="107"/>
-      <c r="H54" s="107"/>
-      <c r="I54" s="107"/>
-      <c r="J54" s="107"/>
-      <c r="K54" s="107"/>
-      <c r="L54" s="107"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="117"/>
+      <c r="D54" s="117"/>
+      <c r="E54" s="117"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="117"/>
+      <c r="H54" s="117"/>
+      <c r="I54" s="117"/>
+      <c r="J54" s="117"/>
+      <c r="K54" s="117"/>
+      <c r="L54" s="117"/>
       <c r="M54" s="44"/>
       <c r="N54" s="44"/>
       <c r="O54" s="44"/>
@@ -14909,10 +14969,10 @@
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
       <c r="F55" s="44"/>
-      <c r="G55" s="108" t="s">
+      <c r="G55" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H55" s="109"/>
+      <c r="H55" s="108"/>
       <c r="I55" s="45"/>
       <c r="J55" s="44"/>
       <c r="K55" s="44"/>
@@ -14982,11 +15042,11 @@
       <c r="S57" s="44"/>
     </row>
     <row r="58" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="110" t="s">
+      <c r="A58" s="111" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="63">
         <v>5</v>
@@ -15016,9 +15076,9 @@
       <c r="J58" s="106"/>
     </row>
     <row r="59" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="111"/>
+      <c r="A59" s="112"/>
       <c r="B59" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="104">
         <v>10</v>
@@ -15045,9 +15105,9 @@
       <c r="J59" s="106"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A60" s="111"/>
+      <c r="A60" s="112"/>
       <c r="B60" s="64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="68">
         <v>3</v>
@@ -15084,7 +15144,7 @@
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A61" s="111"/>
+      <c r="A61" s="112"/>
       <c r="B61" s="64"/>
       <c r="C61" s="65"/>
       <c r="D61" s="61" t="str">
@@ -15112,7 +15172,7 @@
       <c r="J61" s="106"/>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A62" s="111"/>
+      <c r="A62" s="112"/>
       <c r="B62" s="64"/>
       <c r="C62" s="65"/>
       <c r="D62" s="61" t="str">
@@ -15140,7 +15200,7 @@
       <c r="J62" s="106"/>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A63" s="111"/>
+      <c r="A63" s="112"/>
       <c r="B63" s="64"/>
       <c r="C63" s="65"/>
       <c r="D63" s="61" t="str">
@@ -15168,7 +15228,7 @@
       <c r="J63" s="106"/>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A64" s="111"/>
+      <c r="A64" s="112"/>
       <c r="B64" s="64"/>
       <c r="C64" s="65"/>
       <c r="D64" s="61" t="str">
@@ -15196,7 +15256,7 @@
       <c r="J64" s="106"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="111"/>
+      <c r="A65" s="112"/>
       <c r="B65" s="64"/>
       <c r="C65" s="65"/>
       <c r="D65" s="61" t="str">
@@ -15224,7 +15284,7 @@
       <c r="J65" s="106"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="111"/>
+      <c r="A66" s="112"/>
       <c r="B66" s="64"/>
       <c r="C66" s="65"/>
       <c r="D66" s="61" t="str">
@@ -15252,7 +15312,7 @@
       <c r="J66" s="106"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="111"/>
+      <c r="A67" s="112"/>
       <c r="B67" s="64"/>
       <c r="C67" s="65"/>
       <c r="D67" s="61" t="str">
@@ -15280,7 +15340,7 @@
       <c r="J67" s="106"/>
     </row>
     <row r="68" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="111"/>
+      <c r="A68" s="112"/>
       <c r="B68" s="64"/>
       <c r="C68" s="65"/>
       <c r="D68" s="61" t="str">
@@ -15308,7 +15368,7 @@
       <c r="J68" s="106"/>
     </row>
     <row r="69" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="111"/>
+      <c r="A69" s="112"/>
       <c r="B69" s="64"/>
       <c r="C69" s="65"/>
       <c r="D69" s="61" t="str">
@@ -15322,7 +15382,7 @@
       <c r="I69" s="50"/>
     </row>
     <row r="70" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="111"/>
+      <c r="A70" s="112"/>
       <c r="B70" s="64"/>
       <c r="C70" s="65"/>
       <c r="D70" s="61" t="str">
@@ -15336,7 +15396,7 @@
       <c r="I70" s="50"/>
     </row>
     <row r="71" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="111"/>
+      <c r="A71" s="112"/>
       <c r="B71" s="64"/>
       <c r="C71" s="65"/>
       <c r="D71" s="61" t="str">
@@ -15355,47 +15415,47 @@
       </c>
     </row>
     <row r="72" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="111"/>
+      <c r="A72" s="112"/>
       <c r="B72" s="64"/>
       <c r="C72" s="65"/>
       <c r="D72" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E72" s="113" t="str">
+      <c r="E72" s="109" t="str">
         <f>IF(F68&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
         <v># Uren afgetikt aan het eind van de sprint:</v>
       </c>
-      <c r="F72" s="114"/>
-      <c r="G72" s="114"/>
-      <c r="H72" s="114"/>
+      <c r="F72" s="110"/>
+      <c r="G72" s="110"/>
+      <c r="H72" s="110"/>
       <c r="I72" s="12">
         <f>IF(F68&lt;&gt;"",SUM(F58:F68),"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:19" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="111"/>
+      <c r="A73" s="112"/>
       <c r="B73" s="64"/>
       <c r="C73" s="65"/>
       <c r="D73" s="61" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="E73" s="115" t="str">
+      <c r="E73" s="114" t="str">
         <f>IF(F68&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v>Dit moesten er zijn:</v>
       </c>
-      <c r="F73" s="116"/>
-      <c r="G73" s="116"/>
-      <c r="H73" s="116"/>
+      <c r="F73" s="115"/>
+      <c r="G73" s="115"/>
+      <c r="H73" s="115"/>
       <c r="I73" s="16">
         <f>IF(F68&lt;&gt;"",AB60,"")</f>
         <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
+      <c r="A74" s="112"/>
       <c r="B74" s="64"/>
       <c r="C74" s="65"/>
       <c r="D74" s="61" t="str">
@@ -15412,9 +15472,9 @@
       </c>
     </row>
     <row r="75" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
+      <c r="A75" s="112"/>
       <c r="B75" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="65"/>
       <c r="D75" s="61" t="str">
@@ -15428,7 +15488,7 @@
       <c r="I75" s="50"/>
     </row>
     <row r="76" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="111"/>
+      <c r="A76" s="112"/>
       <c r="B76" s="64" t="s">
         <v>57</v>
       </c>
@@ -15444,9 +15504,9 @@
       <c r="I76" s="50"/>
     </row>
     <row r="77" spans="1:19" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="111"/>
+      <c r="A77" s="112"/>
       <c r="B77" s="64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C77" s="65"/>
       <c r="D77" s="61" t="str">
@@ -15460,9 +15520,9 @@
       <c r="I77" s="50"/>
     </row>
     <row r="78" spans="1:19" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="112"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="66" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C78" s="67"/>
       <c r="D78" s="62" t="str">
@@ -15482,20 +15542,20 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
-      <c r="B79" s="107" t="str">
+      <c r="B79" s="117" t="str">
         <f>B1</f>
         <v>Iwan</v>
       </c>
-      <c r="C79" s="107"/>
-      <c r="D79" s="107"/>
-      <c r="E79" s="107"/>
-      <c r="F79" s="107"/>
-      <c r="G79" s="107"/>
-      <c r="H79" s="107"/>
-      <c r="I79" s="107"/>
-      <c r="J79" s="107"/>
-      <c r="K79" s="107"/>
-      <c r="L79" s="107"/>
+      <c r="C79" s="117"/>
+      <c r="D79" s="117"/>
+      <c r="E79" s="117"/>
+      <c r="F79" s="117"/>
+      <c r="G79" s="117"/>
+      <c r="H79" s="117"/>
+      <c r="I79" s="117"/>
+      <c r="J79" s="117"/>
+      <c r="K79" s="117"/>
+      <c r="L79" s="117"/>
       <c r="M79" s="44"/>
       <c r="N79" s="44"/>
       <c r="O79" s="44"/>
@@ -15506,17 +15566,17 @@
     </row>
     <row r="80" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="43"/>
-      <c r="B80" s="107"/>
-      <c r="C80" s="107"/>
-      <c r="D80" s="107"/>
-      <c r="E80" s="107"/>
-      <c r="F80" s="107"/>
-      <c r="G80" s="107"/>
-      <c r="H80" s="107"/>
-      <c r="I80" s="107"/>
-      <c r="J80" s="107"/>
-      <c r="K80" s="107"/>
-      <c r="L80" s="107"/>
+      <c r="B80" s="117"/>
+      <c r="C80" s="117"/>
+      <c r="D80" s="117"/>
+      <c r="E80" s="117"/>
+      <c r="F80" s="117"/>
+      <c r="G80" s="117"/>
+      <c r="H80" s="117"/>
+      <c r="I80" s="117"/>
+      <c r="J80" s="117"/>
+      <c r="K80" s="117"/>
+      <c r="L80" s="117"/>
       <c r="M80" s="44"/>
       <c r="N80" s="44"/>
       <c r="O80" s="44"/>
@@ -15532,10 +15592,10 @@
       <c r="D81" s="44"/>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
-      <c r="G81" s="108" t="s">
+      <c r="G81" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H81" s="109"/>
+      <c r="H81" s="108"/>
       <c r="I81" s="45"/>
       <c r="J81" s="44"/>
       <c r="K81" s="44"/>
@@ -15605,11 +15665,15 @@
       <c r="S83" s="44"/>
     </row>
     <row r="84" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="110" t="s">
+      <c r="A84" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="B84" s="33"/>
-      <c r="C84" s="63"/>
+      <c r="B84" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" s="63">
+        <v>5</v>
+      </c>
       <c r="D84" s="60" t="str">
         <f>IF(C84&lt;&gt;"",IF(AND(C84&lt;&gt;1,C84&lt;&gt;2,C84&lt;&gt;3,C84&lt;&gt;5,C84&lt;&gt;8,C84&lt;&gt;13,C84&lt;&gt;20,C84&lt;&gt;40,C84&lt;&gt;100),"Fout",""),"")</f>
         <v/>
@@ -15622,11 +15686,11 @@
       </c>
       <c r="G84" s="17">
         <f>AB86</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H84" s="20">
         <f>AB86-F84</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I84" s="21">
         <f>G84-H84</f>
@@ -15634,31 +15698,41 @@
       </c>
     </row>
     <row r="85" spans="1:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="69"/>
+      <c r="A85" s="112"/>
+      <c r="B85" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C85" s="69">
+        <v>8</v>
+      </c>
       <c r="D85" s="98"/>
       <c r="E85" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="F85" s="100"/>
+      <c r="F85" s="100">
+        <v>0</v>
+      </c>
       <c r="G85" s="101">
         <f t="shared" ref="G85:G94" si="16">(G84-(AB$86/10))</f>
-        <v>0</v>
-      </c>
-      <c r="H85" s="96" t="e">
+        <v>19.8</v>
+      </c>
+      <c r="H85" s="96">
         <f>IF(F85="",NA(),H84-F85)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I85" s="22" t="str">
+        <v>22</v>
+      </c>
+      <c r="I85" s="22">
         <f t="shared" ref="I85:I88" si="17">IF(F85="","",G85-H85)</f>
-        <v/>
+        <v>-2.1999999999999993</v>
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A86" s="111"/>
-      <c r="B86" s="64"/>
-      <c r="C86" s="65"/>
+      <c r="A86" s="112"/>
+      <c r="B86" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="65">
+        <v>1</v>
+      </c>
       <c r="D86" s="61" t="str">
         <f t="shared" ref="D86:D104" si="18">IF(C86&lt;&gt;"",IF(AND(C86&lt;&gt;1,C86&lt;&gt;2,C86&lt;&gt;3,C86&lt;&gt;5,C86&lt;&gt;8,C86&lt;&gt;13,C86&lt;&gt;20,C86&lt;&gt;40,C86&lt;&gt;100),"Fout",""),"")</f>
         <v/>
@@ -15666,31 +15740,37 @@
       <c r="E86" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="F86" s="75"/>
+      <c r="F86" s="75">
+        <v>0</v>
+      </c>
       <c r="G86" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H86" s="96" t="e">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H86" s="96">
         <f>IF(F86="",NA(),H85-F86)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I86" s="22" t="str">
+        <v>22</v>
+      </c>
+      <c r="I86" s="22">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-4.3999999999999986</v>
       </c>
       <c r="AA86" t="s">
         <v>3</v>
       </c>
       <c r="AB86">
         <f>SUM(C84:C104)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A87" s="111"/>
-      <c r="B87" s="64"/>
-      <c r="C87" s="65"/>
+      <c r="A87" s="112"/>
+      <c r="B87" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="65">
+        <v>8</v>
+      </c>
       <c r="D87" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -15698,22 +15778,24 @@
       <c r="E87" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="F87" s="75"/>
+      <c r="F87" s="75">
+        <v>0</v>
+      </c>
       <c r="G87" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H87" s="96" t="e">
+        <v>15.400000000000002</v>
+      </c>
+      <c r="H87" s="96">
         <f t="shared" ref="H87:H94" si="19">IF(F87="",NA(),H86-F87)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I87" s="22" t="str">
+        <v>22</v>
+      </c>
+      <c r="I87" s="22">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-6.5999999999999979</v>
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A88" s="111"/>
+      <c r="A88" s="112"/>
       <c r="B88" s="64"/>
       <c r="C88" s="65"/>
       <c r="D88" s="61" t="str">
@@ -15723,22 +15805,24 @@
       <c r="E88" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="F88" s="75"/>
+      <c r="F88" s="75">
+        <v>5</v>
+      </c>
       <c r="G88" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H88" s="96" t="e">
+        <v>13.200000000000003</v>
+      </c>
+      <c r="H88" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I88" s="22" t="str">
+        <v>17</v>
+      </c>
+      <c r="I88" s="22">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-3.7999999999999972</v>
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A89" s="111"/>
+      <c r="A89" s="112"/>
       <c r="B89" s="64"/>
       <c r="C89" s="65"/>
       <c r="D89" s="61" t="str">
@@ -15748,22 +15832,24 @@
       <c r="E89" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F89" s="75"/>
+      <c r="F89" s="75">
+        <v>0</v>
+      </c>
       <c r="G89" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H89" s="96" t="e">
+        <v>11.000000000000004</v>
+      </c>
+      <c r="H89" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I89" s="22" t="str">
+        <v>17</v>
+      </c>
+      <c r="I89" s="22">
         <f>IF(F89="","",G89-H89)</f>
-        <v/>
+        <v>-5.9999999999999964</v>
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A90" s="111"/>
+      <c r="A90" s="112"/>
       <c r="B90" s="64"/>
       <c r="C90" s="65"/>
       <c r="D90" s="61" t="str">
@@ -15773,22 +15859,24 @@
       <c r="E90" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="F90" s="75"/>
+      <c r="F90" s="75">
+        <v>0</v>
+      </c>
       <c r="G90" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H90" s="96" t="e">
+        <v>8.8000000000000043</v>
+      </c>
+      <c r="H90" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I90" s="22" t="str">
+        <v>17</v>
+      </c>
+      <c r="I90" s="22">
         <f t="shared" ref="I90:I94" si="20">IF(F90="","",G90-H90)</f>
-        <v/>
+        <v>-8.1999999999999957</v>
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="111"/>
+      <c r="A91" s="112"/>
       <c r="B91" s="64"/>
       <c r="C91" s="65"/>
       <c r="D91" s="61" t="str">
@@ -15798,22 +15886,24 @@
       <c r="E91" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="F91" s="75"/>
+      <c r="F91" s="75">
+        <v>0</v>
+      </c>
       <c r="G91" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H91" s="96" t="e">
+        <v>6.6000000000000041</v>
+      </c>
+      <c r="H91" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I91" s="22" t="str">
+        <v>17</v>
+      </c>
+      <c r="I91" s="22">
         <f t="shared" si="20"/>
-        <v/>
+        <v>-10.399999999999995</v>
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A92" s="111"/>
+      <c r="A92" s="112"/>
       <c r="B92" s="64"/>
       <c r="C92" s="65"/>
       <c r="D92" s="61" t="str">
@@ -15823,22 +15913,24 @@
       <c r="E92" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="F92" s="75"/>
+      <c r="F92" s="75">
+        <v>8</v>
+      </c>
       <c r="G92" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H92" s="96" t="e">
+        <v>4.4000000000000039</v>
+      </c>
+      <c r="H92" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I92" s="22" t="str">
+        <v>9</v>
+      </c>
+      <c r="I92" s="22">
         <f t="shared" si="20"/>
-        <v/>
+        <v>-4.5999999999999961</v>
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A93" s="111"/>
+      <c r="A93" s="112"/>
       <c r="B93" s="64"/>
       <c r="C93" s="65"/>
       <c r="D93" s="61" t="str">
@@ -15848,22 +15940,24 @@
       <c r="E93" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F93" s="75"/>
+      <c r="F93" s="75">
+        <v>1</v>
+      </c>
       <c r="G93" s="18">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H93" s="96" t="e">
+        <v>2.2000000000000037</v>
+      </c>
+      <c r="H93" s="96">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I93" s="22" t="str">
+        <v>8</v>
+      </c>
+      <c r="I93" s="22">
         <f t="shared" si="20"/>
-        <v/>
+        <v>-5.7999999999999963</v>
       </c>
     </row>
     <row r="94" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="111"/>
+      <c r="A94" s="112"/>
       <c r="B94" s="64"/>
       <c r="C94" s="65"/>
       <c r="D94" s="61" t="str">
@@ -15873,22 +15967,24 @@
       <c r="E94" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="F94" s="76"/>
+      <c r="F94" s="76">
+        <v>8</v>
+      </c>
       <c r="G94" s="19">
         <f t="shared" si="16"/>
+        <v>3.5527136788005009E-15</v>
+      </c>
+      <c r="H94" s="97">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H94" s="97" t="e">
-        <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I94" s="77" t="str">
+      <c r="I94" s="77">
         <f t="shared" si="20"/>
-        <v/>
+        <v>3.5527136788005009E-15</v>
       </c>
     </row>
     <row r="95" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="111"/>
+      <c r="A95" s="112"/>
       <c r="B95" s="64"/>
       <c r="C95" s="65"/>
       <c r="D95" s="61" t="str">
@@ -15902,7 +15998,7 @@
       <c r="I95" s="50"/>
     </row>
     <row r="96" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="111"/>
+      <c r="A96" s="112"/>
       <c r="B96" s="64"/>
       <c r="C96" s="65"/>
       <c r="D96" s="61" t="str">
@@ -15916,7 +16012,7 @@
       <c r="I96" s="50"/>
     </row>
     <row r="97" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="111"/>
+      <c r="A97" s="112"/>
       <c r="B97" s="64"/>
       <c r="C97" s="65"/>
       <c r="D97" s="61" t="str">
@@ -15931,51 +16027,51 @@
       </c>
       <c r="I97" s="28">
         <f>AB86/10</f>
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:28" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="111"/>
+      <c r="A98" s="112"/>
       <c r="B98" s="64"/>
       <c r="C98" s="65"/>
       <c r="D98" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E98" s="113" t="str">
+      <c r="E98" s="109" t="str">
         <f>IF(F94&lt;&gt;"","# Uren afgetikt aan het eind van de sprint:","")</f>
-        <v/>
-      </c>
-      <c r="F98" s="114"/>
-      <c r="G98" s="114"/>
-      <c r="H98" s="114"/>
-      <c r="I98" s="12" t="str">
+        <v># Uren afgetikt aan het eind van de sprint:</v>
+      </c>
+      <c r="F98" s="110"/>
+      <c r="G98" s="110"/>
+      <c r="H98" s="110"/>
+      <c r="I98" s="12">
         <f>IF(F94&lt;&gt;"",SUM(F84:F94),"")</f>
-        <v/>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:28" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="111"/>
+      <c r="A99" s="112"/>
       <c r="B99" s="64"/>
       <c r="C99" s="65"/>
       <c r="D99" s="61" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="E99" s="115" t="str">
+      <c r="E99" s="114" t="str">
         <f>IF(F94&lt;&gt;"","Dit moesten er zijn:","")</f>
-        <v/>
-      </c>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116"/>
-      <c r="I99" s="16" t="str">
+        <v>Dit moesten er zijn:</v>
+      </c>
+      <c r="F99" s="115"/>
+      <c r="G99" s="115"/>
+      <c r="H99" s="115"/>
+      <c r="I99" s="16">
         <f>IF(F94&lt;&gt;"",AB86,"")</f>
-        <v/>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="111"/>
+      <c r="A100" s="112"/>
       <c r="B100" s="64"/>
       <c r="C100" s="65"/>
       <c r="D100" s="61" t="str">
@@ -15988,12 +16084,14 @@
       <c r="H100" s="47"/>
       <c r="I100" s="51" t="str">
         <f>IF(F94="","",IF(I98&lt;I99,"Dus te weinig.","Keurig"))</f>
-        <v/>
+        <v>Keurig</v>
       </c>
     </row>
     <row r="101" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="111"/>
-      <c r="B101" s="64"/>
+      <c r="A101" s="112"/>
+      <c r="B101" s="64" t="s">
+        <v>76</v>
+      </c>
       <c r="C101" s="65"/>
       <c r="D101" s="61" t="str">
         <f t="shared" si="18"/>
@@ -16006,8 +16104,10 @@
       <c r="I101" s="50"/>
     </row>
     <row r="102" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="111"/>
-      <c r="B102" s="64"/>
+      <c r="A102" s="112"/>
+      <c r="B102" s="64" t="s">
+        <v>75</v>
+      </c>
       <c r="C102" s="65"/>
       <c r="D102" s="61" t="str">
         <f t="shared" si="18"/>
@@ -16020,8 +16120,10 @@
       <c r="I102" s="50"/>
     </row>
     <row r="103" spans="1:28" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="111"/>
-      <c r="B103" s="64"/>
+      <c r="A103" s="112"/>
+      <c r="B103" s="64" t="s">
+        <v>74</v>
+      </c>
       <c r="C103" s="65"/>
       <c r="D103" s="61" t="str">
         <f t="shared" si="18"/>
@@ -16034,8 +16136,10 @@
       <c r="I103" s="50"/>
     </row>
     <row r="104" spans="1:28" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="112"/>
-      <c r="B104" s="66"/>
+      <c r="A104" s="113"/>
+      <c r="B104" s="66" t="s">
+        <v>73</v>
+      </c>
       <c r="C104" s="67"/>
       <c r="D104" s="62" t="str">
         <f t="shared" si="18"/>
@@ -16046,27 +16150,27 @@
       </c>
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
-      <c r="H104" s="26" t="str">
+      <c r="H104" s="26">
         <f>I98</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="I104" s="27"/>
     </row>
     <row r="105" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="43"/>
-      <c r="B105" s="107" t="s">
+      <c r="B105" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C105" s="107"/>
-      <c r="D105" s="107"/>
-      <c r="E105" s="107"/>
-      <c r="F105" s="107"/>
-      <c r="G105" s="107"/>
-      <c r="H105" s="107"/>
-      <c r="I105" s="107"/>
-      <c r="J105" s="107"/>
-      <c r="K105" s="107"/>
-      <c r="L105" s="107"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
       <c r="M105" s="44"/>
       <c r="N105" s="44"/>
       <c r="O105" s="44"/>
@@ -16077,17 +16181,17 @@
     </row>
     <row r="106" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="43"/>
-      <c r="B106" s="107"/>
-      <c r="C106" s="107"/>
-      <c r="D106" s="107"/>
-      <c r="E106" s="107"/>
-      <c r="F106" s="107"/>
-      <c r="G106" s="107"/>
-      <c r="H106" s="107"/>
-      <c r="I106" s="107"/>
-      <c r="J106" s="107"/>
-      <c r="K106" s="107"/>
-      <c r="L106" s="107"/>
+      <c r="B106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
       <c r="M106" s="44"/>
       <c r="N106" s="44"/>
       <c r="O106" s="44"/>
@@ -16103,10 +16207,10 @@
       <c r="D107" s="44"/>
       <c r="E107" s="44"/>
       <c r="F107" s="44"/>
-      <c r="G107" s="108" t="s">
+      <c r="G107" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H107" s="109"/>
+      <c r="H107" s="108"/>
       <c r="I107" s="45"/>
       <c r="J107" s="44"/>
       <c r="K107" s="44"/>
@@ -16176,7 +16280,7 @@
       <c r="S109" s="44"/>
     </row>
     <row r="110" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="110" t="s">
+      <c r="A110" s="111" t="s">
         <v>26</v>
       </c>
       <c r="B110" s="56"/>
@@ -16206,7 +16310,7 @@
       </c>
     </row>
     <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="111"/>
+      <c r="A111" s="112"/>
       <c r="B111" s="56"/>
       <c r="C111" s="32"/>
       <c r="D111" s="10" t="str">
@@ -16238,7 +16342,7 @@
       </c>
     </row>
     <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="111"/>
+      <c r="A112" s="112"/>
       <c r="B112" s="56"/>
       <c r="C112" s="32"/>
       <c r="D112" s="10" t="str">
@@ -16260,7 +16364,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="111"/>
+      <c r="A113" s="112"/>
       <c r="B113" s="56"/>
       <c r="C113" s="32"/>
       <c r="D113" s="10" t="str">
@@ -16282,7 +16386,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="111"/>
+      <c r="A114" s="112"/>
       <c r="B114" s="56"/>
       <c r="C114" s="32"/>
       <c r="D114" s="10" t="str">
@@ -16304,7 +16408,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="111"/>
+      <c r="A115" s="112"/>
       <c r="B115" s="56"/>
       <c r="C115" s="32"/>
       <c r="D115" s="10" t="str">
@@ -16326,7 +16430,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="111"/>
+      <c r="A116" s="112"/>
       <c r="B116" s="56"/>
       <c r="C116" s="32"/>
       <c r="D116" s="10" t="str">
@@ -16348,7 +16452,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="111"/>
+      <c r="A117" s="112"/>
       <c r="B117" s="56"/>
       <c r="C117" s="32"/>
       <c r="D117" s="10" t="str">
@@ -16370,7 +16474,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="111"/>
+      <c r="A118" s="112"/>
       <c r="B118" s="56"/>
       <c r="C118" s="32"/>
       <c r="D118" s="10" t="str">
@@ -16392,7 +16496,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="111"/>
+      <c r="A119" s="112"/>
       <c r="B119" s="56"/>
       <c r="C119" s="32"/>
       <c r="D119" s="10" t="str">
@@ -16412,7 +16516,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="111"/>
+      <c r="A120" s="112"/>
       <c r="B120" s="56"/>
       <c r="C120" s="32"/>
       <c r="D120" s="10" t="str">
@@ -16426,7 +16530,7 @@
       <c r="I120" s="49"/>
     </row>
     <row r="121" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="111"/>
+      <c r="A121" s="112"/>
       <c r="B121" s="56"/>
       <c r="C121" s="32"/>
       <c r="D121" s="10" t="str">
@@ -16440,7 +16544,7 @@
       <c r="I121" s="50"/>
     </row>
     <row r="122" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="111"/>
+      <c r="A122" s="112"/>
       <c r="B122" s="56"/>
       <c r="C122" s="32"/>
       <c r="D122" s="10" t="str">
@@ -16459,47 +16563,47 @@
       </c>
     </row>
     <row r="123" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="111"/>
+      <c r="A123" s="112"/>
       <c r="B123" s="56"/>
       <c r="C123" s="32"/>
       <c r="D123" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E123" s="113" t="str">
+      <c r="E123" s="109" t="str">
         <f>IF(F119&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F123" s="114"/>
-      <c r="G123" s="114"/>
-      <c r="H123" s="114"/>
+      <c r="F123" s="110"/>
+      <c r="G123" s="110"/>
+      <c r="H123" s="110"/>
       <c r="I123" s="12" t="str">
         <f>IF(F119&lt;&gt;"",SUM(F110:F119),"")</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="111"/>
+      <c r="A124" s="112"/>
       <c r="B124" s="56"/>
       <c r="C124" s="32"/>
       <c r="D124" s="10" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="E124" s="115" t="str">
+      <c r="E124" s="114" t="str">
         <f>IF(F119&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F124" s="116"/>
-      <c r="G124" s="116"/>
-      <c r="H124" s="116"/>
+      <c r="F124" s="115"/>
+      <c r="G124" s="115"/>
+      <c r="H124" s="115"/>
       <c r="I124" s="16" t="str">
         <f>IF(F119&lt;&gt;"",AB111,"")</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="111"/>
+      <c r="A125" s="112"/>
       <c r="B125" s="34"/>
       <c r="C125" s="58"/>
       <c r="D125" s="10" t="str">
@@ -16516,7 +16620,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="111"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="34"/>
       <c r="C126" s="32"/>
       <c r="D126" s="10" t="str">
@@ -16530,7 +16634,7 @@
       <c r="I126" s="50"/>
     </row>
     <row r="127" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="111"/>
+      <c r="A127" s="112"/>
       <c r="B127" s="34"/>
       <c r="C127" s="32"/>
       <c r="D127" s="10" t="str">
@@ -16544,7 +16648,7 @@
       <c r="I127" s="50"/>
     </row>
     <row r="128" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="111"/>
+      <c r="A128" s="112"/>
       <c r="B128" s="34"/>
       <c r="C128" s="32"/>
       <c r="D128" s="10" t="str">
@@ -16558,7 +16662,7 @@
       <c r="I128" s="50"/>
     </row>
     <row r="129" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="112"/>
+      <c r="A129" s="113"/>
       <c r="B129" s="34"/>
       <c r="C129" s="32"/>
       <c r="D129" s="11" t="str">
@@ -16578,19 +16682,19 @@
     </row>
     <row r="130" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="43"/>
-      <c r="B130" s="107" t="s">
+      <c r="B130" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C130" s="107"/>
-      <c r="D130" s="107"/>
-      <c r="E130" s="107"/>
-      <c r="F130" s="107"/>
-      <c r="G130" s="107"/>
-      <c r="H130" s="107"/>
-      <c r="I130" s="107"/>
-      <c r="J130" s="107"/>
-      <c r="K130" s="107"/>
-      <c r="L130" s="107"/>
+      <c r="C130" s="117"/>
+      <c r="D130" s="117"/>
+      <c r="E130" s="117"/>
+      <c r="F130" s="117"/>
+      <c r="G130" s="117"/>
+      <c r="H130" s="117"/>
+      <c r="I130" s="117"/>
+      <c r="J130" s="117"/>
+      <c r="K130" s="117"/>
+      <c r="L130" s="117"/>
       <c r="M130" s="44"/>
       <c r="N130" s="44"/>
       <c r="O130" s="44"/>
@@ -16601,17 +16705,17 @@
     </row>
     <row r="131" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="43"/>
-      <c r="B131" s="107"/>
-      <c r="C131" s="107"/>
-      <c r="D131" s="107"/>
-      <c r="E131" s="107"/>
-      <c r="F131" s="107"/>
-      <c r="G131" s="107"/>
-      <c r="H131" s="107"/>
-      <c r="I131" s="107"/>
-      <c r="J131" s="107"/>
-      <c r="K131" s="107"/>
-      <c r="L131" s="107"/>
+      <c r="B131" s="117"/>
+      <c r="C131" s="117"/>
+      <c r="D131" s="117"/>
+      <c r="E131" s="117"/>
+      <c r="F131" s="117"/>
+      <c r="G131" s="117"/>
+      <c r="H131" s="117"/>
+      <c r="I131" s="117"/>
+      <c r="J131" s="117"/>
+      <c r="K131" s="117"/>
+      <c r="L131" s="117"/>
       <c r="M131" s="44"/>
       <c r="N131" s="44"/>
       <c r="O131" s="44"/>
@@ -16627,10 +16731,10 @@
       <c r="D132" s="44"/>
       <c r="E132" s="44"/>
       <c r="F132" s="44"/>
-      <c r="G132" s="108" t="s">
+      <c r="G132" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H132" s="109"/>
+      <c r="H132" s="108"/>
       <c r="I132" s="45"/>
       <c r="J132" s="44"/>
       <c r="K132" s="44"/>
@@ -16700,7 +16804,7 @@
       <c r="S134" s="44"/>
     </row>
     <row r="135" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="110" t="s">
+      <c r="A135" s="111" t="s">
         <v>27</v>
       </c>
       <c r="B135" s="57"/>
@@ -16730,7 +16834,7 @@
       </c>
     </row>
     <row r="136" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="111"/>
+      <c r="A136" s="112"/>
       <c r="B136" s="56"/>
       <c r="C136" s="32"/>
       <c r="D136" s="10" t="str">
@@ -16762,7 +16866,7 @@
       </c>
     </row>
     <row r="137" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="111"/>
+      <c r="A137" s="112"/>
       <c r="B137" s="56"/>
       <c r="C137" s="32"/>
       <c r="D137" s="10" t="str">
@@ -16784,7 +16888,7 @@
       </c>
     </row>
     <row r="138" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="111"/>
+      <c r="A138" s="112"/>
       <c r="B138" s="56"/>
       <c r="C138" s="32"/>
       <c r="D138" s="10" t="str">
@@ -16806,7 +16910,7 @@
       </c>
     </row>
     <row r="139" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="111"/>
+      <c r="A139" s="112"/>
       <c r="B139" s="56"/>
       <c r="C139" s="32"/>
       <c r="D139" s="10" t="str">
@@ -16828,7 +16932,7 @@
       </c>
     </row>
     <row r="140" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="111"/>
+      <c r="A140" s="112"/>
       <c r="B140" s="56"/>
       <c r="C140" s="32"/>
       <c r="D140" s="10" t="str">
@@ -16850,7 +16954,7 @@
       </c>
     </row>
     <row r="141" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="111"/>
+      <c r="A141" s="112"/>
       <c r="B141" s="56"/>
       <c r="C141" s="32"/>
       <c r="D141" s="10" t="str">
@@ -16872,7 +16976,7 @@
       </c>
     </row>
     <row r="142" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="111"/>
+      <c r="A142" s="112"/>
       <c r="B142" s="56"/>
       <c r="C142" s="32"/>
       <c r="D142" s="10" t="str">
@@ -16894,7 +16998,7 @@
       </c>
     </row>
     <row r="143" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="111"/>
+      <c r="A143" s="112"/>
       <c r="B143" s="56"/>
       <c r="C143" s="32"/>
       <c r="D143" s="10" t="str">
@@ -16916,7 +17020,7 @@
       </c>
     </row>
     <row r="144" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="111"/>
+      <c r="A144" s="112"/>
       <c r="B144" s="56"/>
       <c r="C144" s="32"/>
       <c r="D144" s="10" t="str">
@@ -16936,7 +17040,7 @@
       </c>
     </row>
     <row r="145" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="111"/>
+      <c r="A145" s="112"/>
       <c r="B145" s="56"/>
       <c r="C145" s="32"/>
       <c r="D145" s="10" t="str">
@@ -16950,7 +17054,7 @@
       <c r="I145" s="49"/>
     </row>
     <row r="146" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="111"/>
+      <c r="A146" s="112"/>
       <c r="B146" s="56"/>
       <c r="C146" s="32"/>
       <c r="D146" s="10" t="str">
@@ -16964,7 +17068,7 @@
       <c r="I146" s="50"/>
     </row>
     <row r="147" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="111"/>
+      <c r="A147" s="112"/>
       <c r="B147" s="56"/>
       <c r="C147" s="32"/>
       <c r="D147" s="10" t="str">
@@ -16983,47 +17087,47 @@
       </c>
     </row>
     <row r="148" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="111"/>
+      <c r="A148" s="112"/>
       <c r="B148" s="56"/>
       <c r="C148" s="32"/>
       <c r="D148" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E148" s="113" t="str">
+      <c r="E148" s="109" t="str">
         <f>IF(F144&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F148" s="114"/>
-      <c r="G148" s="114"/>
-      <c r="H148" s="114"/>
+      <c r="F148" s="110"/>
+      <c r="G148" s="110"/>
+      <c r="H148" s="110"/>
       <c r="I148" s="12" t="str">
         <f>IF(F144&lt;&gt;"",SUM(F135:F144),"")</f>
         <v/>
       </c>
     </row>
     <row r="149" spans="1:27" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="111"/>
+      <c r="A149" s="112"/>
       <c r="B149" s="56"/>
       <c r="C149" s="32"/>
       <c r="D149" s="10" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="E149" s="115" t="str">
+      <c r="E149" s="114" t="str">
         <f>IF(F144&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F149" s="116"/>
-      <c r="G149" s="116"/>
-      <c r="H149" s="116"/>
+      <c r="F149" s="115"/>
+      <c r="G149" s="115"/>
+      <c r="H149" s="115"/>
       <c r="I149" s="16" t="str">
         <f>IF(F144&lt;&gt;"",AB136,"")</f>
         <v/>
       </c>
     </row>
     <row r="150" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="111"/>
+      <c r="A150" s="112"/>
       <c r="B150" s="56"/>
       <c r="C150" s="32"/>
       <c r="D150" s="10" t="str">
@@ -17040,7 +17144,7 @@
       </c>
     </row>
     <row r="151" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="111"/>
+      <c r="A151" s="112"/>
       <c r="B151" s="34"/>
       <c r="C151" s="32"/>
       <c r="D151" s="10" t="str">
@@ -17054,7 +17158,7 @@
       <c r="I151" s="50"/>
     </row>
     <row r="152" spans="1:27" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="111"/>
+      <c r="A152" s="112"/>
       <c r="B152" s="34"/>
       <c r="C152" s="32"/>
       <c r="D152" s="10" t="str">
@@ -17068,7 +17172,7 @@
       <c r="I152" s="50"/>
     </row>
     <row r="153" spans="1:27" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="111"/>
+      <c r="A153" s="112"/>
       <c r="B153" s="34"/>
       <c r="C153" s="32"/>
       <c r="D153" s="10" t="str">
@@ -17082,7 +17186,7 @@
       <c r="I153" s="50"/>
     </row>
     <row r="154" spans="1:27" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="112"/>
+      <c r="A154" s="113"/>
       <c r="B154" s="34"/>
       <c r="C154" s="32"/>
       <c r="D154" s="11" t="str">
@@ -17102,19 +17206,19 @@
     </row>
     <row r="155" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="43"/>
-      <c r="B155" s="107" t="s">
+      <c r="B155" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C155" s="107"/>
-      <c r="D155" s="107"/>
-      <c r="E155" s="107"/>
-      <c r="F155" s="107"/>
-      <c r="G155" s="107"/>
-      <c r="H155" s="107"/>
-      <c r="I155" s="107"/>
-      <c r="J155" s="107"/>
-      <c r="K155" s="107"/>
-      <c r="L155" s="107"/>
+      <c r="C155" s="117"/>
+      <c r="D155" s="117"/>
+      <c r="E155" s="117"/>
+      <c r="F155" s="117"/>
+      <c r="G155" s="117"/>
+      <c r="H155" s="117"/>
+      <c r="I155" s="117"/>
+      <c r="J155" s="117"/>
+      <c r="K155" s="117"/>
+      <c r="L155" s="117"/>
       <c r="M155" s="44"/>
       <c r="N155" s="44"/>
       <c r="O155" s="44"/>
@@ -17125,17 +17229,17 @@
     </row>
     <row r="156" spans="1:27" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="43"/>
-      <c r="B156" s="107"/>
-      <c r="C156" s="107"/>
-      <c r="D156" s="107"/>
-      <c r="E156" s="107"/>
-      <c r="F156" s="107"/>
-      <c r="G156" s="107"/>
-      <c r="H156" s="107"/>
-      <c r="I156" s="107"/>
-      <c r="J156" s="107"/>
-      <c r="K156" s="107"/>
-      <c r="L156" s="107"/>
+      <c r="B156" s="117"/>
+      <c r="C156" s="117"/>
+      <c r="D156" s="117"/>
+      <c r="E156" s="117"/>
+      <c r="F156" s="117"/>
+      <c r="G156" s="117"/>
+      <c r="H156" s="117"/>
+      <c r="I156" s="117"/>
+      <c r="J156" s="117"/>
+      <c r="K156" s="117"/>
+      <c r="L156" s="117"/>
       <c r="M156" s="44"/>
       <c r="N156" s="44"/>
       <c r="O156" s="44"/>
@@ -17151,10 +17255,10 @@
       <c r="D157" s="44"/>
       <c r="E157" s="44"/>
       <c r="F157" s="44"/>
-      <c r="G157" s="108" t="s">
+      <c r="G157" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H157" s="109"/>
+      <c r="H157" s="108"/>
       <c r="I157" s="45"/>
       <c r="J157" s="44"/>
       <c r="K157" s="44"/>
@@ -17224,7 +17328,7 @@
       <c r="S159" s="44"/>
     </row>
     <row r="160" spans="1:27" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="110" t="s">
+      <c r="A160" s="111" t="s">
         <v>28</v>
       </c>
       <c r="B160" s="56"/>
@@ -17254,7 +17358,7 @@
       </c>
     </row>
     <row r="161" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="111"/>
+      <c r="A161" s="112"/>
       <c r="B161" s="56"/>
       <c r="C161" s="32"/>
       <c r="D161" s="10" t="str">
@@ -17286,7 +17390,7 @@
       </c>
     </row>
     <row r="162" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="111"/>
+      <c r="A162" s="112"/>
       <c r="B162" s="56"/>
       <c r="C162" s="32"/>
       <c r="D162" s="10" t="str">
@@ -17308,7 +17412,7 @@
       </c>
     </row>
     <row r="163" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="111"/>
+      <c r="A163" s="112"/>
       <c r="B163" s="56"/>
       <c r="C163" s="32"/>
       <c r="D163" s="10" t="str">
@@ -17330,7 +17434,7 @@
       </c>
     </row>
     <row r="164" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="111"/>
+      <c r="A164" s="112"/>
       <c r="B164" s="56"/>
       <c r="C164" s="32"/>
       <c r="D164" s="10" t="str">
@@ -17352,7 +17456,7 @@
       </c>
     </row>
     <row r="165" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="111"/>
+      <c r="A165" s="112"/>
       <c r="B165" s="56"/>
       <c r="C165" s="32"/>
       <c r="D165" s="10" t="str">
@@ -17374,7 +17478,7 @@
       </c>
     </row>
     <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="111"/>
+      <c r="A166" s="112"/>
       <c r="B166" s="56"/>
       <c r="C166" s="32"/>
       <c r="D166" s="10" t="str">
@@ -17396,7 +17500,7 @@
       </c>
     </row>
     <row r="167" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="111"/>
+      <c r="A167" s="112"/>
       <c r="B167" s="56"/>
       <c r="C167" s="32"/>
       <c r="D167" s="10" t="str">
@@ -17418,7 +17522,7 @@
       </c>
     </row>
     <row r="168" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="111"/>
+      <c r="A168" s="112"/>
       <c r="B168" s="56"/>
       <c r="C168" s="32"/>
       <c r="D168" s="10" t="str">
@@ -17440,7 +17544,7 @@
       </c>
     </row>
     <row r="169" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="111"/>
+      <c r="A169" s="112"/>
       <c r="B169" s="56"/>
       <c r="C169" s="32"/>
       <c r="D169" s="10" t="str">
@@ -17460,7 +17564,7 @@
       </c>
     </row>
     <row r="170" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="111"/>
+      <c r="A170" s="112"/>
       <c r="B170" s="56"/>
       <c r="C170" s="32"/>
       <c r="D170" s="10" t="str">
@@ -17474,7 +17578,7 @@
       <c r="I170" s="49"/>
     </row>
     <row r="171" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="111"/>
+      <c r="A171" s="112"/>
       <c r="B171" s="56"/>
       <c r="C171" s="32"/>
       <c r="D171" s="10" t="str">
@@ -17488,7 +17592,7 @@
       <c r="I171" s="50"/>
     </row>
     <row r="172" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="111"/>
+      <c r="A172" s="112"/>
       <c r="B172" s="56"/>
       <c r="C172" s="32"/>
       <c r="D172" s="10" t="str">
@@ -17507,47 +17611,47 @@
       </c>
     </row>
     <row r="173" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="111"/>
+      <c r="A173" s="112"/>
       <c r="B173" s="56"/>
       <c r="C173" s="32"/>
       <c r="D173" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E173" s="113" t="str">
+      <c r="E173" s="109" t="str">
         <f>IF(F169&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F173" s="114"/>
-      <c r="G173" s="114"/>
-      <c r="H173" s="114"/>
+      <c r="F173" s="110"/>
+      <c r="G173" s="110"/>
+      <c r="H173" s="110"/>
       <c r="I173" s="12" t="str">
         <f>IF(F169&lt;&gt;"",SUM(F160:F169),"")</f>
         <v/>
       </c>
     </row>
     <row r="174" spans="1:28" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="111"/>
+      <c r="A174" s="112"/>
       <c r="B174" s="56"/>
       <c r="C174" s="32"/>
       <c r="D174" s="10" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="E174" s="115" t="str">
+      <c r="E174" s="114" t="str">
         <f>IF(F169&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F174" s="116"/>
-      <c r="G174" s="116"/>
-      <c r="H174" s="116"/>
+      <c r="F174" s="115"/>
+      <c r="G174" s="115"/>
+      <c r="H174" s="115"/>
       <c r="I174" s="16" t="str">
         <f>IF(F169&lt;&gt;"",AB161,"")</f>
         <v/>
       </c>
     </row>
     <row r="175" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="111"/>
+      <c r="A175" s="112"/>
       <c r="B175" s="34"/>
       <c r="C175" s="58"/>
       <c r="D175" s="10" t="str">
@@ -17564,7 +17668,7 @@
       </c>
     </row>
     <row r="176" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="111"/>
+      <c r="A176" s="112"/>
       <c r="B176" s="34"/>
       <c r="C176" s="32"/>
       <c r="D176" s="10" t="str">
@@ -17578,7 +17682,7 @@
       <c r="I176" s="50"/>
     </row>
     <row r="177" spans="1:28" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="111"/>
+      <c r="A177" s="112"/>
       <c r="B177" s="34"/>
       <c r="C177" s="32"/>
       <c r="D177" s="10" t="str">
@@ -17592,7 +17696,7 @@
       <c r="I177" s="50"/>
     </row>
     <row r="178" spans="1:28" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="111"/>
+      <c r="A178" s="112"/>
       <c r="B178" s="34"/>
       <c r="C178" s="32"/>
       <c r="D178" s="10" t="str">
@@ -17606,7 +17710,7 @@
       <c r="I178" s="50"/>
     </row>
     <row r="179" spans="1:28" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="112"/>
+      <c r="A179" s="113"/>
       <c r="B179" s="34"/>
       <c r="C179" s="32"/>
       <c r="D179" s="11" t="str">
@@ -17626,19 +17730,19 @@
     </row>
     <row r="180" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="43"/>
-      <c r="B180" s="107" t="s">
+      <c r="B180" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C180" s="107"/>
-      <c r="D180" s="107"/>
-      <c r="E180" s="107"/>
-      <c r="F180" s="107"/>
-      <c r="G180" s="107"/>
-      <c r="H180" s="107"/>
-      <c r="I180" s="107"/>
-      <c r="J180" s="107"/>
-      <c r="K180" s="107"/>
-      <c r="L180" s="107"/>
+      <c r="C180" s="117"/>
+      <c r="D180" s="117"/>
+      <c r="E180" s="117"/>
+      <c r="F180" s="117"/>
+      <c r="G180" s="117"/>
+      <c r="H180" s="117"/>
+      <c r="I180" s="117"/>
+      <c r="J180" s="117"/>
+      <c r="K180" s="117"/>
+      <c r="L180" s="117"/>
       <c r="M180" s="44"/>
       <c r="N180" s="44"/>
       <c r="O180" s="44"/>
@@ -17649,17 +17753,17 @@
     </row>
     <row r="181" spans="1:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="43"/>
-      <c r="B181" s="107"/>
-      <c r="C181" s="107"/>
-      <c r="D181" s="107"/>
-      <c r="E181" s="107"/>
-      <c r="F181" s="107"/>
-      <c r="G181" s="107"/>
-      <c r="H181" s="107"/>
-      <c r="I181" s="107"/>
-      <c r="J181" s="107"/>
-      <c r="K181" s="107"/>
-      <c r="L181" s="107"/>
+      <c r="B181" s="117"/>
+      <c r="C181" s="117"/>
+      <c r="D181" s="117"/>
+      <c r="E181" s="117"/>
+      <c r="F181" s="117"/>
+      <c r="G181" s="117"/>
+      <c r="H181" s="117"/>
+      <c r="I181" s="117"/>
+      <c r="J181" s="117"/>
+      <c r="K181" s="117"/>
+      <c r="L181" s="117"/>
       <c r="M181" s="44"/>
       <c r="N181" s="44"/>
       <c r="O181" s="44"/>
@@ -17675,10 +17779,10 @@
       <c r="D182" s="44"/>
       <c r="E182" s="44"/>
       <c r="F182" s="44"/>
-      <c r="G182" s="108" t="s">
+      <c r="G182" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H182" s="109"/>
+      <c r="H182" s="108"/>
       <c r="I182" s="45"/>
       <c r="J182" s="44"/>
       <c r="K182" s="44"/>
@@ -17748,7 +17852,7 @@
       <c r="S184" s="44"/>
     </row>
     <row r="185" spans="1:28" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="110" t="s">
+      <c r="A185" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B185" s="56"/>
@@ -17778,7 +17882,7 @@
       </c>
     </row>
     <row r="186" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="111"/>
+      <c r="A186" s="112"/>
       <c r="B186" s="56"/>
       <c r="C186" s="32"/>
       <c r="D186" s="10" t="str">
@@ -17810,7 +17914,7 @@
       </c>
     </row>
     <row r="187" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="111"/>
+      <c r="A187" s="112"/>
       <c r="B187" s="56"/>
       <c r="C187" s="32"/>
       <c r="D187" s="10" t="str">
@@ -17832,7 +17936,7 @@
       </c>
     </row>
     <row r="188" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="111"/>
+      <c r="A188" s="112"/>
       <c r="B188" s="56"/>
       <c r="C188" s="32"/>
       <c r="D188" s="10" t="str">
@@ -17854,7 +17958,7 @@
       </c>
     </row>
     <row r="189" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="111"/>
+      <c r="A189" s="112"/>
       <c r="B189" s="56"/>
       <c r="C189" s="32"/>
       <c r="D189" s="10" t="str">
@@ -17876,7 +17980,7 @@
       </c>
     </row>
     <row r="190" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="111"/>
+      <c r="A190" s="112"/>
       <c r="B190" s="56"/>
       <c r="C190" s="32"/>
       <c r="D190" s="10" t="str">
@@ -17898,7 +18002,7 @@
       </c>
     </row>
     <row r="191" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="111"/>
+      <c r="A191" s="112"/>
       <c r="B191" s="56"/>
       <c r="C191" s="32"/>
       <c r="D191" s="10" t="str">
@@ -17920,7 +18024,7 @@
       </c>
     </row>
     <row r="192" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="111"/>
+      <c r="A192" s="112"/>
       <c r="B192" s="56"/>
       <c r="C192" s="32"/>
       <c r="D192" s="10" t="str">
@@ -17942,7 +18046,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="111"/>
+      <c r="A193" s="112"/>
       <c r="B193" s="56"/>
       <c r="C193" s="32"/>
       <c r="D193" s="10" t="str">
@@ -17964,7 +18068,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="111"/>
+      <c r="A194" s="112"/>
       <c r="B194" s="56"/>
       <c r="C194" s="32"/>
       <c r="D194" s="10" t="str">
@@ -17984,7 +18088,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="111"/>
+      <c r="A195" s="112"/>
       <c r="B195" s="56"/>
       <c r="C195" s="32"/>
       <c r="D195" s="10" t="str">
@@ -17998,7 +18102,7 @@
       <c r="I195" s="49"/>
     </row>
     <row r="196" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="111"/>
+      <c r="A196" s="112"/>
       <c r="B196" s="56"/>
       <c r="C196" s="32"/>
       <c r="D196" s="10" t="str">
@@ -18012,7 +18116,7 @@
       <c r="I196" s="50"/>
     </row>
     <row r="197" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="111"/>
+      <c r="A197" s="112"/>
       <c r="B197" s="56"/>
       <c r="C197" s="32"/>
       <c r="D197" s="10" t="str">
@@ -18031,47 +18135,47 @@
       </c>
     </row>
     <row r="198" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="111"/>
+      <c r="A198" s="112"/>
       <c r="B198" s="56"/>
       <c r="C198" s="32"/>
       <c r="D198" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E198" s="113" t="str">
+      <c r="E198" s="109" t="str">
         <f>IF(F194&lt;&gt;"","# Points afgetikt aan het eind van de sprint:","")</f>
         <v/>
       </c>
-      <c r="F198" s="114"/>
-      <c r="G198" s="114"/>
-      <c r="H198" s="114"/>
+      <c r="F198" s="110"/>
+      <c r="G198" s="110"/>
+      <c r="H198" s="110"/>
       <c r="I198" s="12" t="str">
         <f>IF(F194&lt;&gt;"",SUM(F185:F194),"")</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="1:9" s="6" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="111"/>
+      <c r="A199" s="112"/>
       <c r="B199" s="56"/>
       <c r="C199" s="32"/>
       <c r="D199" s="10" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="E199" s="115" t="str">
+      <c r="E199" s="114" t="str">
         <f>IF(F194&lt;&gt;"","Dit moesten er zijn:","")</f>
         <v/>
       </c>
-      <c r="F199" s="116"/>
-      <c r="G199" s="116"/>
-      <c r="H199" s="116"/>
+      <c r="F199" s="115"/>
+      <c r="G199" s="115"/>
+      <c r="H199" s="115"/>
       <c r="I199" s="16" t="str">
         <f>IF(F194&lt;&gt;"",AB186,"")</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="111"/>
+      <c r="A200" s="112"/>
       <c r="B200" s="56"/>
       <c r="C200" s="32"/>
       <c r="D200" s="10" t="str">
@@ -18088,7 +18192,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="111"/>
+      <c r="A201" s="112"/>
       <c r="B201" s="34"/>
       <c r="C201" s="32"/>
       <c r="D201" s="10" t="str">
@@ -18102,7 +18206,7 @@
       <c r="I201" s="50"/>
     </row>
     <row r="202" spans="1:9" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="111"/>
+      <c r="A202" s="112"/>
       <c r="B202" s="34"/>
       <c r="C202" s="32"/>
       <c r="D202" s="10" t="str">
@@ -18116,7 +18220,7 @@
       <c r="I202" s="50"/>
     </row>
     <row r="203" spans="1:9" s="6" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="111"/>
+      <c r="A203" s="112"/>
       <c r="B203" s="34"/>
       <c r="C203" s="32"/>
       <c r="D203" s="10" t="str">
@@ -18130,7 +18234,7 @@
       <c r="I203" s="50"/>
     </row>
     <row r="204" spans="1:9" s="2" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="112"/>
+      <c r="A204" s="113"/>
       <c r="B204" s="34"/>
       <c r="C204" s="32"/>
       <c r="D204" s="11" t="str">
@@ -18151,46 +18255,46 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xvw55rBl+8QauwDbqXfPTEJvlFDUCVQW9eBF4D1fCPDMzZnBE0eg23U/adjRGpGtDkno/gEp3o8WBaDX9CrDpg==" saltValue="kVJ3wM2y/GPu2SWvmMPnkg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="40">
+    <mergeCell ref="B180:L181"/>
+    <mergeCell ref="G182:H182"/>
+    <mergeCell ref="A185:A204"/>
+    <mergeCell ref="E198:H198"/>
+    <mergeCell ref="E199:H199"/>
+    <mergeCell ref="B155:L156"/>
+    <mergeCell ref="G157:H157"/>
+    <mergeCell ref="A160:A179"/>
+    <mergeCell ref="E173:H173"/>
+    <mergeCell ref="E174:H174"/>
+    <mergeCell ref="B130:L131"/>
+    <mergeCell ref="G132:H132"/>
+    <mergeCell ref="A135:A154"/>
+    <mergeCell ref="E148:H148"/>
+    <mergeCell ref="E149:H149"/>
+    <mergeCell ref="B105:L106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="A110:A129"/>
+    <mergeCell ref="E123:H123"/>
+    <mergeCell ref="E124:H124"/>
+    <mergeCell ref="B79:L80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="A84:A104"/>
+    <mergeCell ref="E98:H98"/>
+    <mergeCell ref="E99:H99"/>
+    <mergeCell ref="B53:L54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A58:A78"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="B27:L28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A32:A52"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="A6:A26"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="B1:L2"/>
-    <mergeCell ref="B27:L28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A32:A52"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="B53:L54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A58:A78"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="B79:L80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="A84:A104"/>
-    <mergeCell ref="E98:H98"/>
-    <mergeCell ref="E99:H99"/>
-    <mergeCell ref="B105:L106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="A110:A129"/>
-    <mergeCell ref="E123:H123"/>
-    <mergeCell ref="E124:H124"/>
-    <mergeCell ref="B130:L131"/>
-    <mergeCell ref="G132:H132"/>
-    <mergeCell ref="A135:A154"/>
-    <mergeCell ref="E148:H148"/>
-    <mergeCell ref="E149:H149"/>
-    <mergeCell ref="B155:L156"/>
-    <mergeCell ref="G157:H157"/>
-    <mergeCell ref="A160:A179"/>
-    <mergeCell ref="E173:H173"/>
-    <mergeCell ref="E174:H174"/>
-    <mergeCell ref="B180:L181"/>
-    <mergeCell ref="G182:H182"/>
-    <mergeCell ref="A185:A204"/>
-    <mergeCell ref="E198:H198"/>
-    <mergeCell ref="E199:H199"/>
   </mergeCells>
   <conditionalFormatting sqref="I205:I1048576 I3:I6 I8:I16">
     <cfRule type="cellIs" dxfId="35" priority="57" operator="lessThan">
@@ -18380,21 +18484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -18443,16 +18532,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18466,16 +18571,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69266CD-281A-4B62-8FE6-339EF1280C12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCA063-1453-446E-9A57-D30E1A450384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>